<commit_message>
🔄 Sync automático del tracker - 2025-08-16 02:21:37 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -513,10 +513,8 @@
           <t>86.29%</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1.5</t>
-        </is>
+      <c r="G2" t="n">
+        <v>1.5</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -560,10 +558,8 @@
           <t>93.73%</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1.42</t>
-        </is>
+      <c r="G3" t="n">
+        <v>1.42</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -607,10 +603,8 @@
           <t>52.11%</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2.2</t>
-        </is>
+      <c r="G4" t="n">
+        <v>2.2</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -654,10 +648,8 @@
           <t>92.79%</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1.44</t>
-        </is>
+      <c r="G5" t="n">
+        <v>1.44</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -701,10 +693,8 @@
           <t>90.90%</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1.45</t>
-        </is>
+      <c r="G6" t="n">
+        <v>1.45</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -748,10 +738,8 @@
           <t>44.59%</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2.4</t>
-        </is>
+      <c r="G7" t="n">
+        <v>2.4</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -795,10 +783,8 @@
           <t>98.28%</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>1.2</t>
-        </is>
+      <c r="G8" t="n">
+        <v>1.2</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -842,10 +828,8 @@
           <t>91.78%</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>1.45</t>
-        </is>
+      <c r="G9" t="n">
+        <v>1.45</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -889,10 +873,8 @@
           <t>56.92%</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
+      <c r="G10" t="n">
+        <v>2</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -936,10 +918,8 @@
           <t>91.56%</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>1.45</t>
-        </is>
+      <c r="G11" t="n">
+        <v>1.45</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -983,10 +963,8 @@
           <t>65.11%</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>1.9</t>
-        </is>
+      <c r="G12" t="n">
+        <v>1.9</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1030,10 +1008,8 @@
           <t>46.66%</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2.38</t>
-        </is>
+      <c r="G13" t="n">
+        <v>2.38</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1077,10 +1053,8 @@
           <t>63.43%</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
+      <c r="G14" t="n">
+        <v>2</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1124,10 +1098,8 @@
           <t>55.51%</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2.2</t>
-        </is>
+      <c r="G15" t="n">
+        <v>2.2</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1171,10 +1143,8 @@
           <t>67.35%</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>1.95</t>
-        </is>
+      <c r="G16" t="n">
+        <v>1.95</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1218,10 +1188,8 @@
           <t>74.17%</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>1.75</t>
-        </is>
+      <c r="G17" t="n">
+        <v>1.75</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1265,10 +1233,8 @@
           <t>43.29%</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>2.6</t>
-        </is>
+      <c r="G18" t="n">
+        <v>2.6</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1312,10 +1278,8 @@
           <t>54.85%</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2.38</t>
-        </is>
+      <c r="G19" t="n">
+        <v>2.38</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1359,10 +1323,8 @@
           <t>56.92%</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>1.9</t>
-        </is>
+      <c r="G20" t="n">
+        <v>1.9</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1406,10 +1368,8 @@
           <t>89.33%</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>1.4</t>
-        </is>
+      <c r="G21" t="n">
+        <v>1.4</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1453,10 +1413,8 @@
           <t>68.28%</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>1.9</t>
-        </is>
+      <c r="G22" t="n">
+        <v>1.9</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1500,10 +1458,8 @@
           <t>60.49%</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>1.95</t>
-        </is>
+      <c r="G23" t="n">
+        <v>1.95</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-17 10:59:23 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,30 +12,19 @@
     <sheet name="Summary" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -49,27 +39,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -82,17 +57,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -455,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,47 +436,47 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Liga</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Local</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Visitante</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Predicción</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Probabilidad</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Cuota_Bet365</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>EV</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -551,7 +523,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -596,7 +568,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -641,7 +613,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -686,7 +658,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -731,7 +703,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -776,7 +748,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -821,7 +793,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -866,7 +838,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -911,7 +883,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -956,7 +928,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1001,7 +973,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1018,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1063,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1108,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1153,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1198,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1243,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1316,7 +1288,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1361,7 +1333,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1406,7 +1378,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1423,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1496,7 +1468,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1720,6 +1692,141 @@
         </is>
       </c>
       <c r="I28" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>nantes</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>paris saint germain</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>42.83%</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>178.39%</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Segunda División</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>real sociedad ii</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>zaragoza</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>42.07%</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>3</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>26.21%</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>fc volendam</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>az alkmaar</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>36.29%</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>5</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>81.45%</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>Completed</t>
         </is>
@@ -1736,7 +1843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1745,49 +1852,54 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Liga</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Local</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Visitante</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Resultado_Real</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Predicción</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Acierto</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Profit</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ROI</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha_Partido</t>
         </is>
       </c>
     </row>
@@ -1831,6 +1943,7 @@
       <c r="I2" t="n">
         <v>75</v>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1872,6 +1985,7 @@
       <c r="I3" t="n">
         <v>-100</v>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1913,6 +2027,7 @@
       <c r="I4" t="n">
         <v>105</v>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1954,6 +2069,7 @@
       <c r="I5" t="n">
         <v>-100</v>
       </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1994,6 +2110,1065 @@
       </c>
       <c r="I6" t="n">
         <v>-100</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>zulte waregem</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>club brugge kv</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I7" t="n">
+        <v>50</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>mallorca</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>barcelona</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="I8" t="n">
+        <v>42</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>sunderland</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>west ham</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>wolves</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>manchester city</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="I10" t="n">
+        <v>44</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>excelsior</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>feyenoord</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I11" t="n">
+        <v>45</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>tondela</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>famalicao</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="I12" t="n">
+        <v>140</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>estrela</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>benfica</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I13" t="n">
+        <v>20</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Allsvenskan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>halmstad</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>malmo ff</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I14" t="n">
+        <v>45</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Allsvenskan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ifk norrkoping</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>if elfsborg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>tsv hartberg</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>red bull salzburg</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I16" t="n">
+        <v>45</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ried</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>sturm graz</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I17" t="n">
+        <v>90</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>derby</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>coventry</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="I18" t="n">
+        <v>138</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>preston</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>leicester</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>blackburn</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>birmingham</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="I20" t="n">
+        <v>120</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sheffield wednesday</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>stoke city</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I21" t="n">
+        <v>95</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>goztepe</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>fenerbahce</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Liga Profesional Argentina</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>huracan</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>argentinos jrs</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Primera B</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>tigres fc</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>jaguares</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="I24" t="n">
+        <v>138</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2. Division</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ishøj</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>roskilde</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I25" t="n">
+        <v>90</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2. Division</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>brabrand</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>ab copenhagen</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I26" t="n">
+        <v>40</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>alebrijes de oaxaca</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>cancún</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I27" t="n">
+        <v>90</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-08-15</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ca la paz</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>mineros de zacatecas</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="I28" t="n">
+        <v>95</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>fc volendam</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>az alkmaar</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>2025-08-14</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -2016,17 +3191,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Metric</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Last_Updated</t>
         </is>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-17 21:40:10 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -1783,7 +1783,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1843,7 +1843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3168,6 +3168,52 @@
       <c r="J29" t="inlineStr">
         <is>
           <t>2025-08-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Segunda División</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>real sociedad ii</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>zaragoza</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-18 02:34:50 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -1738,7 +1738,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1843,7 +1843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3212,6 +3212,52 @@
         <v>-100</v>
       </c>
       <c r="J30" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-17</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>nantes</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>paris saint germain</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J31" t="inlineStr">
         <is>
           <t>2025-08-17</t>
         </is>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-20 02:17:15 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -750,4 +751,75 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Liga</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Resultado_Real</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Predicción</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Profit</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ROI</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha_Partido</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-20 21:39:57 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Results" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,76 +747,1397 @@
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Liga</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Local</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Visitante</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Resultado_Real</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Predicción</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Acierto</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Profit</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>ROI</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha_Partido</t>
-        </is>
-      </c>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Primera A</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>millonarios</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>union magdalena</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>76.01%</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>614.91%</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.731919789518835</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fc midtjylland</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>kups</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>83.10%</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>11</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>804.97%</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.8141149399466718</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>brann</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>aek larnaca</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>51.55%</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>114.35%</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.03640992038768812</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.3640992038768812</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>malmo ff</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>sigma olomouc</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>60.62%</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>245.09%</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.5233108791362672</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>zrinjski</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>utrecht</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>53.95%</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>118.97%</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.03909149222452285</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.3909149222452285</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>panathinaikos</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>samsunspor</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>57.67%</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>199.72%</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.04770498260447133</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.4770498260447133</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>lincoln red imps fc</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>sc braga</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>92.57%</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>15</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1274.61%</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.9203501868068823</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>bk hacken</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>cfr 1907 cluj</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>43.50%</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>42.10%</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.01893008614938482</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.1893008614938481</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>wolfsberger ac</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>omonia nicosia</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>46.15%</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>73.62%</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.02692024367845594</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.2692024367845594</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>istanbul basaksehir</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>universitatea craiova</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>55.23%</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>159.72%</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.04329059734770679</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.4329059734770678</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>polessya</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>fiorentina</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>71.18%</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>7</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>393.27%</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>5</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.6637498722062879</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>anderlecht</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>aek athens fc</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>43.29%</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>39.28%</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.01808190495725335</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.1808190495725334</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>levski sofia</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>az alkmaar</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>55.58%</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>138.25%</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0422388529008511</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.4223885290085109</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>shakhtar donetsk</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>servette fc</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>68.67%</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>341.88%</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>5</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.6297121761790173</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>neman</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>rayo vallecano</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>85.80%</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>11</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>834.31%</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>5</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.8437493790044812</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sparta praha</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>riga</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>74.58%</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>527.61%</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>5</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.7119282007099271</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>strasbourg</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>brondby</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>56.65%</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>166.38%</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.04508675507864759</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.4508675507864759</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>celje</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>baník ostrava</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>42.95%</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>3</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>27.55%</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.01442114394489741</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.1442114394489741</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>breidablik</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>virtus</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>98.40%</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>26</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2432.92%</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>5</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.9834005308532693</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>jagiellonia</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>dinamo tirana</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>77.31%</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>550.57%</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>5</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.7428594933713921</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>shelbourne</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>linfield</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>49.27%</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>111.22%</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.03404144430250197</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.3404144430250196</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>crystal palace</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>fredrikstad</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>97.70%</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>26</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2414.81%</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>5</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.9760845451803558</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>santa clara</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>shamrock rovers</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>72.29%</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>508.35%</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>5</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.6859918340748814</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>UEFA Europa Conference League</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>raków częstochowa</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>arda kardzhali</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>85.68%</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>13</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>1002.69%</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>5</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.8448562169463129</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-21 09:23:08 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,11 @@
           <t>ROI</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -565,13 +570,30 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>2025-08-21 09:11:33</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -623,13 +645,30 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>-4.3</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2025-08-21 09:11:33</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -681,13 +720,30 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>2025-08-21 09:11:33</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -739,13 +795,30 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>-4.3</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>2025-08-21 09:11:33</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -797,13 +870,30 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>850</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2025-08-21 09:11:33</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -862,6 +952,7 @@
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -920,6 +1011,7 @@
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -978,6 +1070,7 @@
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1036,6 +1129,7 @@
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1094,6 +1188,7 @@
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1152,6 +1247,7 @@
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1210,6 +1306,7 @@
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1268,6 +1365,7 @@
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1326,6 +1424,7 @@
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1384,6 +1483,7 @@
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1442,6 +1542,7 @@
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1500,6 +1601,7 @@
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1558,6 +1660,7 @@
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1616,6 +1719,7 @@
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1674,6 +1778,7 @@
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1732,6 +1837,7 @@
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1790,6 +1896,7 @@
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1848,6 +1955,7 @@
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1906,6 +2014,7 @@
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1964,6 +2073,7 @@
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2022,6 +2132,7 @@
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2080,6 +2191,7 @@
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2138,6 +2250,7 @@
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-21 18:47:23 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2252,6 +2252,773 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>paris saint germain</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>angers</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>98.41%</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>21</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>1945.95%</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.9833078686563578</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>real betis</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>alaves</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>48.73%</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>121.91%</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.03448745631990931</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.344874563199093</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Segunda División</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>eibar</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>granada cf</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>44.20%</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>57.52%</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.02273606502137256</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.2273606502137256</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Segunda División</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>leganes</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>cadiz</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>47.78%</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>112.85%</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.03285799271357884</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.3285799271357884</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>west ham</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>chelsea</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>59.34%</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>179.07%</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>6</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.04850299398501735</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.4850299398501735</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Eliteserien</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>kfum oslo</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>ham-kam</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>53.43%</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>177.69%</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.04247001729525227</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.4247001729525227</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Ekstraklasa</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>radomiak radom</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>nieciecza</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>43.47%</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>54.94%</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.02173134634323324</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.2173134634323323</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Superliga</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>vllaznia shkodër</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>egnatia rrogozhinë</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>40.15%</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>29.19%</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.01355307647359828</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.1355307647359828</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2. Bundesliga</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>sv elversberg</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>1. fc kaiserslautern</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>40.93%</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>31.70%</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.01467980316853604</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.1467980316853604</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>League</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>sama al sarhan</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>al salt</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>53.30%</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>121.61%</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.03870251266414631</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.387025126641463</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Liga Profesional Argentina</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>tigre</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>independ. rivadavia</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>42.39%</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>59.45%</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.02180870899900153</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.2180870899900152</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Primera B</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>real cartagena</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>tigres fc</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>69.06%</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>8</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>446.92%</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.6463526766868029</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1. Division</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>aalborg</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>hvidovre</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>42.99%</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>44.69%</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.01922983319639007</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.1922983319639007</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-21 22:40:32 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -945,14 +945,30 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1004,14 +1020,30 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>-3.6</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1063,14 +1095,30 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1122,14 +1170,30 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>-3.9</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1181,14 +1245,30 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>-4.8</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1240,14 +1320,30 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1299,14 +1395,30 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="P13" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1358,14 +1470,30 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="P14" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1417,14 +1545,30 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>16.12</v>
+      </c>
+      <c r="P15" t="n">
+        <v>375</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1476,14 +1620,30 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P16" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1535,14 +1695,30 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="P17" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1594,14 +1770,30 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>-4.2</v>
+      </c>
+      <c r="P18" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1653,14 +1845,30 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P19" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1712,14 +1920,30 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P20" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1771,14 +1995,30 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P21" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1830,14 +2070,30 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="P22" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1889,14 +2145,30 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="P23" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1948,14 +2220,30 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P24" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2007,14 +2295,30 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O25" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2066,14 +2370,30 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O26" t="n">
+        <v>-3.4</v>
+      </c>
+      <c r="P26" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>2025-08-21 21:17:49</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2125,13 +2445,25 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O27" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P27" t="n">
+        <v>-100</v>
+      </c>
       <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
@@ -2184,13 +2516,25 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="P28" t="n">
+        <v>750</v>
+      </c>
       <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
@@ -2243,13 +2587,25 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O29" t="n">
+        <v>-5</v>
+      </c>
+      <c r="P29" t="n">
+        <v>-100</v>
+      </c>
       <c r="Q29" t="inlineStr"/>
     </row>
     <row r="30">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-22 03:27:46 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -2464,7 +2464,11 @@
       <c r="P27" t="n">
         <v>-100</v>
       </c>
-      <c r="Q27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>2025-08-22 02:39:08</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2535,7 +2539,11 @@
       <c r="P28" t="n">
         <v>750</v>
       </c>
-      <c r="Q28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>2025-08-22 02:39:08</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2606,7 +2614,11 @@
       <c r="P29" t="n">
         <v>-100</v>
       </c>
-      <c r="Q29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>2025-08-22 02:39:08</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-22 18:47:41 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3387,6 +3387,4077 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>sc freiburg</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>fc augsburg</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>48.27%</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>100.71%</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.03210580164783154</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.3210580164783154</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>bayer leverkusen</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>1899 hoffenheim</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>58.70%</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>205.11%</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.04898573470099921</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.489857347009992</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>eintracht frankfurt</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>werder bremen</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>52.34%</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>146.13%</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.03963185294962115</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.3963185294962115</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>fc st. pauli</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>borussia dortmund</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>59.60%</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>165.50%</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.04805241413326483</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.4805241413326483</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>marseille</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>paris fc</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>70.80%</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>425.71%</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.6631051595202225</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>nice</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>auxerre</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>52.33%</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>146.09%</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.0396214688122223</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.3962146881222229</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>lyon</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>metz</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>70.57%</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>7</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>389.05%</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.6566485912115758</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Premiership</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>celtic</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>livingston</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>93.12%</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>17</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>1467.21%</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.9268993022669484</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Premiership</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>kilmarnock</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>dundee</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>45.87%</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>96.63%</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.02961363197022342</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.2961363197022342</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Premiership</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>heart of midlothian</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>motherwell</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>58.59%</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>204.50%</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.04884177806207579</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.4884177806207579</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>atletico madrid</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>elche</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>88.80%</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>15</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>1218.74%</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.8800446778715231</v>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>levante</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>barcelona</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>87.96%</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>11</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>857.92%</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.8676002771579947</v>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Segunda División</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>zaragoza</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>fc andorra</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>49.38%</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>111.67%</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.0341764649366852</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.341764649366852</v>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>manchester city</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>tottenham</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>63.28%</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>260.19%</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.5554358465001181</v>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>bournemouth</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>wolves</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>49.10%</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>104.17%</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>3</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.03319633700111928</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.3319633700111927</v>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>arsenal</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>leeds</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>81.06%</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>662.34%</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.7882887588355706</v>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>sassuolo</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>napoli</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>65.31%</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>271.79%</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.580097790992555</v>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>genoa</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>lecce</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>48.79%</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>117.36%</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.03415755124929473</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.3415755124929472</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ac milan</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>cremonese</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>74.97%</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>9</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>567.97%</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.7183979179435752</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>as roma</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>bologna</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>41.59%</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>44.12%</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.01822865913324155</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.1822865913324155</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Serie B</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>empoli</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>padova</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>46.29%</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>74.14%</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.02710831080246111</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.2710831080246111</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Serie B</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>palermo</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>reggiana</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>52.55%</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>147.10%</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.03989174251503966</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.3989174251503966</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Serie B</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>monza</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>mantova</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>49.14%</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>99.45%</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>3</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.03273050610739808</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.3273050610739808</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>go ahead eagles</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>sparta rotterdam</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>41.46%</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>35.47%</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.01601489383978273</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.1601489383978273</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>psv eindhoven</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>groningen</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>89.70%</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>12</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>965.59%</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.8875966184105462</v>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>nacional</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>sporting cp</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>83.92%</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>9</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>647.70%</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.8190650142720641</v>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>benfica</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>tondela</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>93.27%</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>17</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>1469.71%</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.9284794690032385</v>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>arouca</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>rio ave</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>43.60%</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>68.32%</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.02414645113995433</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.2414645113995432</v>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Superliga</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>fc copenhagen</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>odense</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>72.66%</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>7</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>403.55%</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.6810554055158541</v>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Super League</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>fc zurich</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>fc thun</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>41.08%</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>30.15%</t>
+        </is>
+      </c>
+      <c r="I72" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.01430176719825711</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.1430176719825711</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>red bull salzburg</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>lask linz</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>61.96%</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>237.40%</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.5351260205787802</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>fc bw linz</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>ried</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>41.04%</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>38.13%</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.01646812632775779</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.1646812632775778</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Ekstraklasa</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>korona kielce</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>motor lublin</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>43.05%</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>53.43%</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.02114600566324421</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.2114600566324421</v>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Ekstraklasa</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>gornik zabrze</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>gks katowice</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>50.47%</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>109.85%</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.03498907715798458</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.3498907715798458</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Superliga</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>af elbasani</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>flamurtari</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>49.86%</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>107.30%</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.03418490043117883</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.3418490043117882</v>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>hull city</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>blackburn</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>40.21%</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>27.39%</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.01303438321185186</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.1303438321185186</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>swansea</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>watford</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>46.11%</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>78.02%</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.02752370961224401</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.2752370961224401</v>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>southampton</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>stoke city</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>49.16%</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>119.01%</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.0346354821789761</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.346354821789761</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>birmingham</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>oxford united</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>60.83%</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>246.29%</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.5258788482999873</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr"/>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>west brom</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>portsmouth</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>50.29%</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>124.06%</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.03609105136561119</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.3609105136561119</v>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>sheffield utd</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>millwall</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>44.50%</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>63.02%</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.02395063453848542</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.2395063453848542</v>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr"/>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>coventry</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>qpr</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>59.78%</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>225.50%</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0.508426269822349</v>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>wrexham</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>sheffield wednesday</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>60.23%</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>242.86%</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.5185771711769417</v>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>fenerbahce</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>kocaelispor</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>71.13%</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>7</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>392.93%</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0.6631824736233448</v>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>gazişehir gaziantep</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>genclerbirligi</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>54.34%</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>155.54%</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0.04216696153962424</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.4216696153962424</v>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2. Bundesliga</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>hannover 96</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>1. fc magdeburg</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>45.14%</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>67.60%</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0.02519646327644949</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0.2519646327644949</v>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2. Bundesliga</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>sc paderborn 07</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>fortuna düsseldorf</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>48.93%</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>98.60%</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0.03245377564570808</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0.3245377564570808</v>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2. Bundesliga</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>karlsruher sc</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>eintracht braunschweig</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>44.13%</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>70.40%</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0.02486931760915075</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0.2486931760915075</v>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>League</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>al ramtha</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>al buqa'a</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>58.73%</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>176.17%</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.04772199016436784</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0.4772199016436783</v>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>League</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>shabab al ordon</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>al hussein</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>85.27%</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>10</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>744.12%</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0.8362794051006492</v>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>cruzeiro</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>internacional</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>48.26%</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>5</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>138.89%</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.03532674756390638</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0.3532674756390637</v>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Liga Profesional Argentina</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>san lorenzo</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>instituto cordoba</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>45.75%</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>96.11%</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0.02945665150533124</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0.2945665150533123</v>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Liga Profesional Argentina</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>rosario central</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>newells old boys</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>54.90%</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>198.96%</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.04488342110185454</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0.4488342110185454</v>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Liga Profesional Argentina</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>san martin s.j.</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>gimnasia l.p.</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>41.45%</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>55.95%</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.02054434039899138</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0.2054434039899138</v>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Torneo Federal A</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>guillermo brown</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>santamarina</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>46.35%</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>4</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>83.55%</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0.02846969491678806</v>
+      </c>
+      <c r="K97" t="n">
+        <v>0.2846969491678806</v>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Torneo Federal A</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>crucero del norte</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>boca unidos</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>37.47%</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>3</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>11.28%</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0.006202140707103194</v>
+      </c>
+      <c r="K98" t="n">
+        <v>0.06202140707103193</v>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+      <c r="Q98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Primera A</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>llaneros</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>deportivo pasto</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>50.27%</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>123.95%</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0.03606047063981269</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0.3606047063981269</v>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Primera A</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>independiente medellin</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>la equidad</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>57.63%</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>256.61%</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0.04956434625870758</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0.4956434625870758</v>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Primera B</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>quindio</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>depor fc</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>56.57%</t>
+        </is>
+      </c>
+      <c r="G101" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>194.01%</t>
+        </is>
+      </c>
+      <c r="I101" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0.04634852228013139</v>
+      </c>
+      <c r="K101" t="n">
+        <v>0.4634852228013139</v>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
+      <c r="Q101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>1. Division</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>b 93</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>kolding if</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>50.10%</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>83.50%</t>
+        </is>
+      </c>
+      <c r="I102" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0.03161266235016244</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0.3161266235016244</v>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
+      <c r="Q102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>1. Division</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>hillerød</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>hb koge</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>64.07%</t>
+        </is>
+      </c>
+      <c r="G103" t="n">
+        <v>6</v>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>280.57%</t>
+        </is>
+      </c>
+      <c r="I103" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J103" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K103" t="n">
+        <v>0.5688349482695851</v>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+      <c r="Q103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2. Division</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>ab copenhagen</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>thisted fc</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>54.61%</t>
+        </is>
+      </c>
+      <c r="G104" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>121.66%</t>
+        </is>
+      </c>
+      <c r="I104" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0.03996772740473215</v>
+      </c>
+      <c r="K104" t="n">
+        <v>0.3996772740473215</v>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+      <c r="Q104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>venados fc</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>ca la paz</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>50.72%</t>
+        </is>
+      </c>
+      <c r="G105" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>110.88%</t>
+        </is>
+      </c>
+      <c r="I105" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J105" t="n">
+        <v>0.03531459716995338</v>
+      </c>
+      <c r="K105" t="n">
+        <v>0.3531459716995338</v>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+      <c r="Q105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>tepatitlán</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>dorados</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>61.02%</t>
+        </is>
+      </c>
+      <c r="G106" t="n">
+        <v>6</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>262.43%</t>
+        </is>
+      </c>
+      <c r="I106" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K106" t="n">
+        <v>0.5321848281952739</v>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>leones negros udg</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>tapatío</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>47.72%</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>93.69%</t>
+        </is>
+      </c>
+      <c r="I107" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J107" t="n">
+        <v>0.03085280643169922</v>
+      </c>
+      <c r="K107" t="n">
+        <v>0.3085280643169922</v>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Liga MX</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>fc juarez</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>santos laguna</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>56.87%</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>209.67%</t>
+        </is>
+      </c>
+      <c r="I108" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J108" t="n">
+        <v>0.04728881955146522</v>
+      </c>
+      <c r="K108" t="n">
+        <v>0.4728881955146522</v>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+      <c r="Q108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>philadelphia union</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>chicago fire</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>49.48%</t>
+        </is>
+      </c>
+      <c r="G109" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>91.06%</t>
+        </is>
+      </c>
+      <c r="I109" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J109" t="n">
+        <v>0.0320638285294936</v>
+      </c>
+      <c r="K109" t="n">
+        <v>0.3206382852949359</v>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>columbus crew</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>new england revolution</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>60.97%</t>
+        </is>
+      </c>
+      <c r="G110" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>247.10%</t>
+        </is>
+      </c>
+      <c r="I110" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J110" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K110" t="n">
+        <v>0.5275823014510532</v>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+      <c r="Q110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>fc cincinnati</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>new york city fc</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>44.38%</t>
+        </is>
+      </c>
+      <c r="G111" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>53.79%</t>
+        </is>
+      </c>
+      <c r="I111" t="n">
+        <v>2</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0.02213609713993531</v>
+      </c>
+      <c r="K111" t="n">
+        <v>0.2213609713993531</v>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-22 22:39:48 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -2670,14 +2670,30 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="P30" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2788,14 +2804,30 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O32" t="n">
+        <v>-2.8</v>
+      </c>
+      <c r="P32" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2906,14 +2938,30 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O34" t="n">
+        <v>-6</v>
+      </c>
+      <c r="P34" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2965,14 +3013,30 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O35" t="n">
+        <v>-5.3</v>
+      </c>
+      <c r="P35" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3024,14 +3088,30 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O36" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="P36" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3083,14 +3163,30 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O37" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P37" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3142,14 +3238,30 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O38" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="P38" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3201,14 +3313,30 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O39" t="n">
+        <v>-4.8</v>
+      </c>
+      <c r="P39" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3378,14 +3506,30 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O42" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="P42" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3850,14 +3994,30 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
-      <c r="Q50" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O50" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="P50" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5974,14 +6134,30 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr"/>
-      <c r="N86" t="inlineStr"/>
-      <c r="O86" t="inlineStr"/>
-      <c r="P86" t="inlineStr"/>
-      <c r="Q86" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O86" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="P86" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -6446,14 +6622,30 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr"/>
-      <c r="N94" t="inlineStr"/>
-      <c r="O94" t="inlineStr"/>
-      <c r="P94" t="inlineStr"/>
-      <c r="Q94" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O94" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="P94" t="n">
+        <v>333</v>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>2025-08-22 21:17:28</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-23 03:22:47 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -2745,14 +2745,30 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>-4.3</v>
+      </c>
+      <c r="P31" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>2025-08-23 02:25:43</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2879,14 +2895,30 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O33" t="n">
+        <v>-4.1</v>
+      </c>
+      <c r="P33" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>2025-08-23 02:25:43</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3388,14 +3420,30 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O40" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="P40" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>2025-08-23 02:25:43</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3447,14 +3495,30 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O41" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="P41" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>2025-08-23 02:25:43</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-29 18:44:51 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -1,29 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-25905" yWindow="-3570" windowWidth="26010" windowHeight="20985" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -37,12 +41,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,14 +74,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,87 +456,87 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Liga</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Local</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Visitante</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Prediccion</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Probabilidad</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Cuota_Bet365</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>EV</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Stake</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>StakePct</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>KellyFrac</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>Resultado_Real</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="2" t="inlineStr">
         <is>
           <t>Profit</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="2" t="inlineStr">
         <is>
           <t>ROI</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="2" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
@@ -570,14 +592,30 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="P2" t="n">
+        <v>130</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>2025-08-29 18:26:03</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1051,537 +1089,6 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Serie A</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Cremonese</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Sassuolo</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Home Win</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>50.10%</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>14.09%</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.01172288410770104</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.1172288410770104</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>La Liga</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Elche</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Levante</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Home Win</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>55.16%</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>2.15</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>17.40%</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.01616060688585717</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.1616060688585717</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Eredivisie</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Groningen</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Heracles</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Home Win</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>66.80%</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>1.85</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>22.34%</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.02773509445282878</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.2773509445282877</v>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Süper Lig</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Goztepe</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Konyaspor</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Home Win</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>62.62%</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>1.95</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>20.89%</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.02327370309292166</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.2327370309292165</v>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Serie A</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Lecce</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>AC Milan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Away Win</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>79.46%</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>31.37%</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.04880205707307923</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.4880205707307923</v>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Jupiler Pro League</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Cercle Brugge</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>St. Truiden</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Home Win</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>50.74%</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>10.51%</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.009689707931872626</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.09689707931872625</v>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Ligue 1</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Lens</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Stade Brestois 29</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Home Win</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>65.75%</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
-        <v>1.91</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>24.33%</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.02811728286770778</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.2811728286770778</v>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>La Liga</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Valencia</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Getafe</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Home Win</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>52.89%</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>15.19%</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.01362814432924039</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.1362814432924039</v>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Liga de Expansión MX</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Tapatío</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Atlante FC</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Away Win</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>47.36%</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>7.85%</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.006875409234375524</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0.06875409234375524</v>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-29 21:38:20 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -1,33 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-25905" yWindow="-3570" windowWidth="26010" windowHeight="20985" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -41,27 +37,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -74,17 +55,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -447,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,87 +434,87 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Liga</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Local</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Visitante</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Prediccion</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Probabilidad</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Cuota_Bet365</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>EV</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Stake</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>StakePct</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>KellyFrac</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Resultado_Real</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Profit</t>
         </is>
       </c>
-      <c r="P1" s="2" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>ROI</t>
         </is>
       </c>
-      <c r="Q1" s="2" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
@@ -667,14 +645,30 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="P3" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2025-08-29 21:36:35</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -726,14 +720,30 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="P4" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>2025-08-29 21:36:35</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -785,14 +795,30 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>-2.3</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>2025-08-29 21:36:35</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -844,14 +870,30 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="P6" t="n">
+        <v>67</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2025-08-29 21:36:35</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -903,14 +945,30 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>2025-08-29 21:36:35</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -962,14 +1020,30 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="P8" t="n">
+        <v>91</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>2025-08-29 21:36:35</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1021,14 +1095,30 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="P9" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2025-08-29 21:36:35</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1089,6 +1179,1599 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Correcaminos Uat</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Tepatitlán</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>55.90%</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>16.22%</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.01580964466711851</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.1580964466711851</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CA La Paz</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Dorados</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>71.96%</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>24.67%</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.03457280562635075</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.3457280562635074</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>81.52%</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>26.70%</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>5</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.04909559739067899</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.4909559739067899</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1899 Hoffenheim</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Eintracht Frankfurt</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>46.79%</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>4.23%</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.004228089782112123</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.04228089782112123</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1. FC Heidenheim</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>88.28%</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>25.85%</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.6163852598885579</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>VfB Stuttgart</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Borussia Mönchengladbach</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>81.02%</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>28.33%</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>5</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.04937507587864312</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.4937507587864312</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Werder Bremen</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Bayer Leverkusen</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>64.55%</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>22.06%</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.02559346436817269</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.2559346436817269</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Sunderland</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>45.68%</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>7.63%</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.006313855677549</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.06313855677548999</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>73.87%</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>27.98%</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>4</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.03902794791662595</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.3902794791662594</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>KV Mechelen</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>RAAL La Louvière</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>77.82%</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>24.80%</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.04203355619475313</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.4203355619475312</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Lorient</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Lille</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>56.67%</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>17.82%</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.01727837088123952</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.1727837088123952</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Alaves</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>74.65%</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>33.03%</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.04297256930010711</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.4297256930010711</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Kasimpasa</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Gazişehir Gaziantep</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>64.95%</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>18.96%</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.02372280190707685</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.2372280190707685</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Kocaelispor</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Kayserispor</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>55.20%</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>17.49%</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.01624370685655212</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.1624370685655212</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>67.82%</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>27.58%</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.03207125218708107</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.3207125218708107</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>57.55%</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>19.64%</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.01895520766078265</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.1895520766078264</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Heerenveen</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>GO Ahead Eagles</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>50.21%</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>9.36%</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.00872368454743617</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.0872368454743617</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Oviedo</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>53.29%</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>18.71%</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.01592451459956846</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.1592451459956846</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>AVS</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Famalicao</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>66.23%</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>25.23%</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>3</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.02911229353745573</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.2911229353745572</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Guimaraes</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Arouca</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>69.18%</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>23.28%</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.03065030762556403</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.3065030762556403</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Antalyaspor</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Fatih Karagümrük</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>62.62%</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>20.89%</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.02327370309292166</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.2327370309292165</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Pisa</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>AS Roma</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>76.65%</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>31.27%</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.04465783127262833</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.4465783127262833</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Charleroi</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Dender</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>72.49%</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>22.01%</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.03320038537987239</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.3320038537987239</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Excelsior</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Twente</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>67.61%</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>22.49%</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.02858543913583976</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.2858543913583976</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Sporting CP</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>FC Porto</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>61.32%</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>2</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>21.42%</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.02264637133937901</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.2264637133937901</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>New York City FC</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>DC United</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>83.87%</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>28.69%</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.5452866410665622</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Toronto FC</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>CF Montreal</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>63.53%</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>22.65%</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.02515057719935727</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.2515057719935727</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-30 18:43:35 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -1170,14 +1170,30 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1229,14 +1245,30 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="P11" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1288,14 +1320,30 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="P12" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1347,14 +1395,30 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="P13" t="n">
+        <v>57</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1406,14 +1470,30 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P14" t="n">
+        <v>125</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1465,14 +1545,30 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="P15" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1524,14 +1620,30 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>3</v>
+      </c>
+      <c r="P16" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1583,14 +1695,30 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>-2.6</v>
+      </c>
+      <c r="P17" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1642,14 +1770,30 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="P18" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1701,14 +1845,30 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>-4</v>
+      </c>
+      <c r="P19" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1760,14 +1920,30 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="P20" t="n">
+        <v>62</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1819,14 +1995,30 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="P21" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1878,14 +2070,30 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>-4.4</v>
+      </c>
+      <c r="P22" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1937,14 +2145,30 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O23" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="P23" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1996,14 +2220,30 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O24" t="n">
+        <v>-1.6</v>
+      </c>
+      <c r="P24" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2055,14 +2295,30 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O25" t="n">
+        <v>-3.3</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2114,14 +2370,30 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O26" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="P26" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>2025-08-30 18:23:58</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-30 22:38:05 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3044,6 +3044,1894 @@
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Austin</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>San Jose Earthquakes</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>53.83%</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>11.91%</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.01185935992232205</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.1185935992232205</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Sporting Kansas City</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Colorado Rapids</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>58.15%</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>2</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>15.14%</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.01629821757331635</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.1629821757331635</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Minnesota United FC</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Portland Timbers</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>73.61%</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>27.53%</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.03843006390250685</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.3843006390250685</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Nashville SC</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Atlanta United FC</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>87.87%</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>25.27%</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.6030328745841734</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Fortuna Sittard</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>NEC Nijmegen</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>49.38%</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>7.54%</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.007187961864934366</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.07187961864934365</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Gent</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Club Brugge KV</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>80.89%</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>29.74%</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.500760157021969</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Sparta Rotterdam</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Feyenoord</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>67.61%</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>22.49%</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>3</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.02858543913583976</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.2858543913583976</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>PEC Zwolle</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>50.65%</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>10.31%</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.009524246937548303</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.09524246937548302</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Brighton</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>67.98%</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>24.51%</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.03031818664193643</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.3031818664193643</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Nottingham Forest</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>West Ham</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>75.77%</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>25.27%</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.03959937087708185</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.3959937087708185</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Angers</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Rennes</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>61.15%</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>2</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>21.08%</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.02230459415956969</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.2230459415956969</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>VfL Wolfsburg</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>FSV Mainz 05</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>61.05%</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>2</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>20.89%</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.0221066358449753</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.221066358449753</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>OH Leuven</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Standard Liege</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>54.09%</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>15.14%</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.0141775166322042</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.141775166322042</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>NAC Breda</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>AZ Alkmaar</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>82.19%</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>27.74%</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.5093392164581518</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Le Havre</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>59.07%</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>19.89%</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.02009732743400738</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.2009732743400738</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Strasbourg</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>82.37%</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>26.40%</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.5031254641766906</v>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Paris FC</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Metz</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>72.47%</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>25.55%</t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.03575920729919848</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.3575920729919848</v>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Borussia Dortmund</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Union Berlin</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>90.40%</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>25.29%</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.6639485662539361</v>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Istanbul Basaksehir</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Eyüpspor</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>63.78%</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>23.14%</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.02566256111386165</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.2566256111386165</v>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>71.25%</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>29.09%</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.0366167279866688</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.366167279866688</v>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>47.32%</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>12.43%</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.00969258356476905</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.0969258356476905</v>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Union St. Gilloise</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Anderlecht</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>80.89%</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>24.13%</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.04615507774293427</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.4615507774293426</v>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Real Betis</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Athletic Club</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>45.39%</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>10.08%</t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.007721574202561839</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.07721574202561839</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Aston Villa</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>69.61%</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>26.11%</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.03299757013756545</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.3299757013756545</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Leones Negros UDG</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Tlaxcala</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>84.10%</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>24.89%</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.5230112549280651</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Alanyaspor</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Besiktas</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>54.30%</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>12.90%</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.01276081193961335</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.1276081193961335</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Trabzonspor</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Samsunspor</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>73.63%</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>26.11%</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>4</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.0375062794028851</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.375062794028851</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Verona</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>84.63%</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>25.67%</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.5387770815986485</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Lyon</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Marseille</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>45.72%</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>4.10%</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.003965179902846045</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.03965179902846044</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Rayo Vallecano</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>91.11%</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>26.29%</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.6890210134428515</v>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Rio Ave</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>SC Braga</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>78.19%</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>29.28%</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.04564856690064723</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.4564856690064723</v>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Santa Clara</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Estrela</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>66.74%</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>20.91%</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.02666366764812174</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.2666366764812174</v>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-08-31 20:21:00 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -4095,14 +4095,30 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
-      <c r="Q49" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O49" t="n">
+        <v>-2.3</v>
+      </c>
+      <c r="P49" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4154,14 +4170,30 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
-      <c r="Q50" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O50" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="P50" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4213,14 +4245,30 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
-      <c r="Q51" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O51" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="P51" t="n">
+        <v>57</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4272,14 +4320,30 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O52" t="n">
+        <v>-2.1</v>
+      </c>
+      <c r="P52" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4331,14 +4395,30 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O53" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="P53" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4390,14 +4470,30 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr"/>
-      <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O54" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="P54" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4449,14 +4545,30 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
-      <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O55" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="P55" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4508,14 +4620,30 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="inlineStr"/>
-      <c r="O56" t="inlineStr"/>
-      <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O56" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="P56" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4567,14 +4695,30 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O57" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="P57" t="n">
+        <v>83</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4626,14 +4770,30 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
-      <c r="O58" t="inlineStr"/>
-      <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O58" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P58" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4685,14 +4845,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr"/>
-      <c r="O59" t="inlineStr"/>
-      <c r="P59" t="inlineStr"/>
-      <c r="Q59" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O59" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="P59" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4744,14 +4920,30 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr"/>
-      <c r="O60" t="inlineStr"/>
-      <c r="P60" t="inlineStr"/>
-      <c r="Q60" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O60" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="P60" t="n">
+        <v>145</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>2025-08-31 19:17:12</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-01 18:45:42 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -4995,14 +4995,30 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr"/>
-      <c r="N61" t="inlineStr"/>
-      <c r="O61" t="inlineStr"/>
-      <c r="P61" t="inlineStr"/>
-      <c r="Q61" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O61" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="P61" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5054,14 +5070,30 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr"/>
-      <c r="N62" t="inlineStr"/>
-      <c r="O62" t="inlineStr"/>
-      <c r="P62" t="inlineStr"/>
-      <c r="Q62" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O62" t="n">
+        <v>-5.3</v>
+      </c>
+      <c r="P62" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -5113,14 +5145,30 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr"/>
-      <c r="N63" t="inlineStr"/>
-      <c r="O63" t="inlineStr"/>
-      <c r="P63" t="inlineStr"/>
-      <c r="Q63" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O63" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="P63" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -5172,14 +5220,30 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr"/>
-      <c r="N64" t="inlineStr"/>
-      <c r="O64" t="inlineStr"/>
-      <c r="P64" t="inlineStr"/>
-      <c r="Q64" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O64" t="n">
+        <v>-4</v>
+      </c>
+      <c r="P64" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5231,14 +5295,30 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr"/>
-      <c r="N65" t="inlineStr"/>
-      <c r="O65" t="inlineStr"/>
-      <c r="P65" t="inlineStr"/>
-      <c r="Q65" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O65" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="P65" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -5290,14 +5370,30 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M66" t="inlineStr"/>
-      <c r="N66" t="inlineStr"/>
-      <c r="O66" t="inlineStr"/>
-      <c r="P66" t="inlineStr"/>
-      <c r="Q66" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O66" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="P66" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5349,14 +5445,30 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr"/>
-      <c r="N67" t="inlineStr"/>
-      <c r="O67" t="inlineStr"/>
-      <c r="P67" t="inlineStr"/>
-      <c r="Q67" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O67" t="n">
+        <v>-5.3</v>
+      </c>
+      <c r="P67" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5408,14 +5520,30 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="inlineStr"/>
-      <c r="O68" t="inlineStr"/>
-      <c r="P68" t="inlineStr"/>
-      <c r="Q68" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O68" t="n">
+        <v>-4.8</v>
+      </c>
+      <c r="P68" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5467,14 +5595,30 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M69" t="inlineStr"/>
-      <c r="N69" t="inlineStr"/>
-      <c r="O69" t="inlineStr"/>
-      <c r="P69" t="inlineStr"/>
-      <c r="Q69" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O69" t="n">
+        <v>-2.8</v>
+      </c>
+      <c r="P69" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>2025-09-01 04:32:43</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-02 18:45:13 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -5670,14 +5670,30 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M70" t="inlineStr"/>
-      <c r="N70" t="inlineStr"/>
-      <c r="O70" t="inlineStr"/>
-      <c r="P70" t="inlineStr"/>
-      <c r="Q70" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O70" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P70" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>2025-09-02 04:28:07</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-05 18:44:30 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q70"/>
+  <dimension ref="A1:Q73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5695,6 +5695,183 @@
         </is>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Mineros de Zacatecas</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Cancún</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>62.18%</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>20.04%</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.02236911800293895</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.2236911800293895</v>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Dorados</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Irapuato</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>49.64%</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>8.12%</t>
+        </is>
+      </c>
+      <c r="I72" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.007673772179820727</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.07673772179820727</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Tlaxcala</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Alebrijes de Oaxaca</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>72.66%</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>25.88%</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.03620043620502014</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.3620043620502013</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-06 18:42:01 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5872,6 +5872,301 @@
       <c r="P73" t="inlineStr"/>
       <c r="Q73" t="inlineStr"/>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Houston Dynamo</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Los Angeles Galaxy</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>69.42%</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>27.14%</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>2</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.033443613920573</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.33443613920573</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Chicago Fire</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>New England Revolution</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>72.83%</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>26.19%</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.03661302357767575</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.3661302357767575</v>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>St. Louis City</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>FC Dallas</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>57.45%</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>16.60%</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.01692920300529338</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.1692920300529338</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>CDS Tampico Madero</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Tapatío</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>77.01%</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>23.51%</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.03993199911892363</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.3993199911892363</v>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Tepatitlán</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Leones Negros UDG</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>57.80%</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>20.16%</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.01942729720001626</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.1942729720001626</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-07 18:41:50 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -5745,14 +5745,30 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr"/>
-      <c r="N71" t="inlineStr"/>
-      <c r="O71" t="inlineStr"/>
-      <c r="P71" t="inlineStr"/>
-      <c r="Q71" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O71" t="n">
+        <v>-1.3</v>
+      </c>
+      <c r="P71" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>2025-09-07 04:25:41</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -5804,14 +5820,30 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
-      <c r="O72" t="inlineStr"/>
-      <c r="P72" t="inlineStr"/>
-      <c r="Q72" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O72" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="P72" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>2025-09-07 04:25:41</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5863,14 +5895,30 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M73" t="inlineStr"/>
-      <c r="N73" t="inlineStr"/>
-      <c r="O73" t="inlineStr"/>
-      <c r="P73" t="inlineStr"/>
-      <c r="Q73" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O73" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="P73" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>2025-09-07 04:25:41</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-08 18:46:42 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -5970,14 +5970,30 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M74" t="inlineStr"/>
-      <c r="N74" t="inlineStr"/>
-      <c r="O74" t="inlineStr"/>
-      <c r="P74" t="inlineStr"/>
-      <c r="Q74" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O74" t="n">
+        <v>-2</v>
+      </c>
+      <c r="P74" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>2025-09-08 04:28:17</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -6029,14 +6045,30 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M75" t="inlineStr"/>
-      <c r="N75" t="inlineStr"/>
-      <c r="O75" t="inlineStr"/>
-      <c r="P75" t="inlineStr"/>
-      <c r="Q75" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O75" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="P75" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>2025-09-08 04:28:17</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -6088,14 +6120,30 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M76" t="inlineStr"/>
-      <c r="N76" t="inlineStr"/>
-      <c r="O76" t="inlineStr"/>
-      <c r="P76" t="inlineStr"/>
-      <c r="Q76" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O76" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P76" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>2025-09-08 04:28:17</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -6147,14 +6195,30 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr"/>
-      <c r="N77" t="inlineStr"/>
-      <c r="O77" t="inlineStr"/>
-      <c r="P77" t="inlineStr"/>
-      <c r="Q77" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O77" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="P77" t="n">
+        <v>62</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>2025-09-08 04:28:17</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -6206,14 +6270,30 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M78" t="inlineStr"/>
-      <c r="N78" t="inlineStr"/>
-      <c r="O78" t="inlineStr"/>
-      <c r="P78" t="inlineStr"/>
-      <c r="Q78" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O78" t="n">
+        <v>-1.1</v>
+      </c>
+      <c r="P78" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>2025-09-08 04:28:17</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-11 18:43:58 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6295,6 +6295,65 @@
         </is>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Elche</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>62.06%</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>22.87%</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.02411183574615652</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.2411183574615652</v>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-12 18:43:07 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6354,6 +6354,1658 @@
       <c r="P79" t="inlineStr"/>
       <c r="Q79" t="inlineStr"/>
     </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Correcaminos Uat</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>CDS Tampico Madero</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>58.97%</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>19.67%</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.01988624114580646</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.1988624114580645</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Getafe</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Oviedo</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>62.15%</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>19.98%</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.02230649609137533</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.2230649609137533</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr"/>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>55.10%</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>17.29%</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J82" t="n">
+        <v>0.01606474219962978</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.1606474219962978</v>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>1. FC Heidenheim</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Borussia Dortmund</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>84.47%</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>29.62%</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0.5623251953879485</v>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr"/>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>VfL Wolfsburg</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>1.FC Köln</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>64.00%</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>23.56%</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J84" t="n">
+        <v>0.02610924401215796</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0.2610924401215796</v>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Sunderland</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>76.42%</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>24.84%</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J85" t="n">
+        <v>0.04015353241636593</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.4015353241636593</v>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>64.83%</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>22.59%</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J86" t="n">
+        <v>0.02618707513496685</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0.2618707513496685</v>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>88.79%</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>24.82%</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0.6210598392500283</v>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Samsunspor</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Antalyaspor</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>69.76%</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>24.32%</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J88" t="n">
+        <v>0.03196629946353581</v>
+      </c>
+      <c r="K88" t="n">
+        <v>0.3196629946353581</v>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>81.86%</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>29.67%</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K89" t="n">
+        <v>0.5163749543988497</v>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Estoril</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>AVS</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>67.92%</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>24.40%</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0.03018285873126307</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0.3018285873126307</v>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Nantes</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>74.11%</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>24.73%</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.0371311239114537</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0.371311239114537</v>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Dender</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Union St. Gilloise</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>88.16%</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>29.18%</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0.6350262346143163</v>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>West Ham</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>56.48%</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>17.42%</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>1</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.01691036133749682</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0.1691036133749682</v>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Athletic Club</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Alaves</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>79.34%</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>25.68%</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0.04490876163234837</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0.4490876163234837</v>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>GO Ahead Eagles</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>FC Volendam</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>83.69%</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>26.76%</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0.5290389848704895</v>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>NEC Nijmegen</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>PSV Eindhoven</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>80.63%</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>29.31%</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.04937842097351816</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0.4937842097351816</v>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Besiktas</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Istanbul Basaksehir</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>74.97%</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>26.18%</t>
+        </is>
+      </c>
+      <c r="I97" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0.03922194584395017</v>
+      </c>
+      <c r="K97" t="n">
+        <v>0.3922194584395016</v>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Konyaspor</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Alanyaspor</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>57.80%</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>20.16%</t>
+        </is>
+      </c>
+      <c r="I98" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0.01942729720001626</v>
+      </c>
+      <c r="K98" t="n">
+        <v>0.1942729720001626</v>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+      <c r="Q98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>55.32%</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>20.49%</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0.01808582341703811</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0.180858234170381</v>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>RAAL La Louvière</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Club Brugge KV</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>86.76%</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>27.12%</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0.5918001672972516</v>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>74.10%</t>
+        </is>
+      </c>
+      <c r="G101" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>28.38%</t>
+        </is>
+      </c>
+      <c r="I101" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0.03957039603630205</v>
+      </c>
+      <c r="K101" t="n">
+        <v>0.3957039603630205</v>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
+      <c r="Q101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Twente</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>NAC Breda</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>87.44%</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>24.65%</t>
+        </is>
+      </c>
+      <c r="I102" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0.588892452875154</v>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
+      <c r="Q102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>70.09%</t>
+        </is>
+      </c>
+      <c r="G103" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>24.90%</t>
+        </is>
+      </c>
+      <c r="I103" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J103" t="n">
+        <v>0.03269932008483693</v>
+      </c>
+      <c r="K103" t="n">
+        <v>0.3269932008483693</v>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+      <c r="Q103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Auxerre</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>81.12%</t>
+        </is>
+      </c>
+      <c r="G104" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>28.49%</t>
+        </is>
+      </c>
+      <c r="I104" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0.04964487277068237</v>
+      </c>
+      <c r="K104" t="n">
+        <v>0.4964487277068237</v>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+      <c r="Q104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Alebrijes de Oaxaca</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Atlante FC</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>75.64%</t>
+        </is>
+      </c>
+      <c r="G105" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>27.30%</t>
+        </is>
+      </c>
+      <c r="I105" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J105" t="n">
+        <v>0.040843449230829</v>
+      </c>
+      <c r="K105" t="n">
+        <v>0.4084344923082899</v>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+      <c r="Q105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>DC United</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Orlando City SC</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>54.26%</t>
+        </is>
+      </c>
+      <c r="G106" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>15.50%</t>
+        </is>
+      </c>
+      <c r="I106" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0.01449162217910136</v>
+      </c>
+      <c r="K106" t="n">
+        <v>0.1449162217910136</v>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>New England Revolution</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Toronto FC</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>73.87%</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>27.98%</t>
+        </is>
+      </c>
+      <c r="I107" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J107" t="n">
+        <v>0.03902794791662595</v>
+      </c>
+      <c r="K107" t="n">
+        <v>0.3902794791662594</v>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-13 18:40:54 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q107"/>
+  <dimension ref="A1:Q140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6345,14 +6345,30 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr"/>
-      <c r="N79" t="inlineStr"/>
-      <c r="O79" t="inlineStr"/>
-      <c r="P79" t="inlineStr"/>
-      <c r="Q79" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O79" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="P79" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>2025-09-13 04:25:19</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -8006,6 +8022,1953 @@
       <c r="P107" t="inlineStr"/>
       <c r="Q107" t="inlineStr"/>
     </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>San Jose Earthquakes</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Los Angeles FC</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>49.30%</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>7.37%</t>
+        </is>
+      </c>
+      <c r="I108" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J108" t="n">
+        <v>0.007047009386941619</v>
+      </c>
+      <c r="K108" t="n">
+        <v>0.07047009386941619</v>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+      <c r="Q108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Chicago Fire</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>New York City FC</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>55.81%</t>
+        </is>
+      </c>
+      <c r="G109" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>16.03%</t>
+        </is>
+      </c>
+      <c r="I109" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J109" t="n">
+        <v>0.01564250164831843</v>
+      </c>
+      <c r="K109" t="n">
+        <v>0.1564250164831842</v>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Cancún</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Venados FC</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>71.94%</t>
+        </is>
+      </c>
+      <c r="G110" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>23.22%</t>
+        </is>
+      </c>
+      <c r="I110" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J110" t="n">
+        <v>0.03351227333764964</v>
+      </c>
+      <c r="K110" t="n">
+        <v>0.3351227333764964</v>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+      <c r="Q110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Monarcas</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Dorados</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>87.90%</t>
+        </is>
+      </c>
+      <c r="G111" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>25.31%</t>
+        </is>
+      </c>
+      <c r="I111" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K111" t="n">
+        <v>0.603991928740388</v>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Colorado Rapids</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Houston Dynamo</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>60.01%</t>
+        </is>
+      </c>
+      <c r="G112" t="n">
+        <v>2</v>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>18.82%</t>
+        </is>
+      </c>
+      <c r="I112" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J112" t="n">
+        <v>0.02001793549425894</v>
+      </c>
+      <c r="K112" t="n">
+        <v>0.2001793549425894</v>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
+      <c r="Q112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Real Salt Lake</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Sporting Kansas City</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>85.50%</t>
+        </is>
+      </c>
+      <c r="G113" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>26.96%</t>
+        </is>
+      </c>
+      <c r="I113" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J113" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K113" t="n">
+        <v>0.5649301371622064</v>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+      <c r="Q113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Vancouver Whitecaps</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Philadelphia Union</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>52.61%</t>
+        </is>
+      </c>
+      <c r="G114" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>11.99%</t>
+        </is>
+      </c>
+      <c r="I114" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J114" t="n">
+        <v>0.01140859740333694</v>
+      </c>
+      <c r="K114" t="n">
+        <v>0.1140859740333694</v>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
+      <c r="Q114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Portland Timbers</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>New York Red Bulls</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>59.02%</t>
+        </is>
+      </c>
+      <c r="G115" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>19.78%</t>
+        </is>
+      </c>
+      <c r="I115" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J115" t="n">
+        <v>0.01999374803077246</v>
+      </c>
+      <c r="K115" t="n">
+        <v>0.1999374803077246</v>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
+      <c r="Q115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Minnesota United FC</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>71.78%</t>
+        </is>
+      </c>
+      <c r="G116" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>27.92%</t>
+        </is>
+      </c>
+      <c r="I116" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J116" t="n">
+        <v>0.03651087443621034</v>
+      </c>
+      <c r="K116" t="n">
+        <v>0.3651087443621034</v>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr"/>
+      <c r="O116" t="inlineStr"/>
+      <c r="P116" t="inlineStr"/>
+      <c r="Q116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Excelsior</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Sparta Rotterdam</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>53.06%</t>
+        </is>
+      </c>
+      <c r="G117" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>12.93%</t>
+        </is>
+      </c>
+      <c r="I117" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J117" t="n">
+        <v>0.01223737297702819</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0.1223737297702819</v>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
+      <c r="P117" t="inlineStr"/>
+      <c r="Q117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>AS Roma</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>84.63%</t>
+        </is>
+      </c>
+      <c r="G118" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>25.67%</t>
+        </is>
+      </c>
+      <c r="I118" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J118" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0.5387770815986485</v>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" t="inlineStr"/>
+      <c r="O118" t="inlineStr"/>
+      <c r="P118" t="inlineStr"/>
+      <c r="Q118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Celta Vigo</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Girona</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>78.06%</t>
+        </is>
+      </c>
+      <c r="G119" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>27.52%</t>
+        </is>
+      </c>
+      <c r="I119" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J119" t="n">
+        <v>0.04431251547776804</v>
+      </c>
+      <c r="K119" t="n">
+        <v>0.4431251547776804</v>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" t="inlineStr"/>
+      <c r="O119" t="inlineStr"/>
+      <c r="P119" t="inlineStr"/>
+      <c r="Q119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Heracles</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>AZ Alkmaar</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>87.09%</t>
+        </is>
+      </c>
+      <c r="G120" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>29.32%</t>
+        </is>
+      </c>
+      <c r="I120" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J120" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0.6125719010818987</v>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" t="inlineStr"/>
+      <c r="O120" t="inlineStr"/>
+      <c r="P120" t="inlineStr"/>
+      <c r="Q120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Groningen</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>73.61%</t>
+        </is>
+      </c>
+      <c r="G121" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>27.53%</t>
+        </is>
+      </c>
+      <c r="I121" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J121" t="n">
+        <v>0.03843006390250685</v>
+      </c>
+      <c r="K121" t="n">
+        <v>0.3843006390250685</v>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" t="inlineStr"/>
+      <c r="O121" t="inlineStr"/>
+      <c r="P121" t="inlineStr"/>
+      <c r="Q121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Lille</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Toulouse</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>72.47%</t>
+        </is>
+      </c>
+      <c r="G122" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>25.55%</t>
+        </is>
+      </c>
+      <c r="I122" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J122" t="n">
+        <v>0.03575920729919848</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0.3575920729919848</v>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" t="inlineStr"/>
+      <c r="Q122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>FC St. Pauli</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>FC Augsburg</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>56.30%</t>
+        </is>
+      </c>
+      <c r="G123" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>19.83%</t>
+        </is>
+      </c>
+      <c r="I123" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J123" t="n">
+        <v>0.01829776601395399</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0.1829776601395399</v>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Cercle Brugge</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Charleroi</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>57.30%</t>
+        </is>
+      </c>
+      <c r="G124" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>19.13%</t>
+        </is>
+      </c>
+      <c r="I124" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J124" t="n">
+        <v>0.01848467630931988</v>
+      </c>
+      <c r="K124" t="n">
+        <v>0.1848467630931988</v>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" t="inlineStr"/>
+      <c r="Q124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Kayserispor</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Goztepe</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>53.98%</t>
+        </is>
+      </c>
+      <c r="G125" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>17.57%</t>
+        </is>
+      </c>
+      <c r="I125" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J125" t="n">
+        <v>0.01563153151189391</v>
+      </c>
+      <c r="K125" t="n">
+        <v>0.1563153151189391</v>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M125" t="inlineStr"/>
+      <c r="N125" t="inlineStr"/>
+      <c r="O125" t="inlineStr"/>
+      <c r="P125" t="inlineStr"/>
+      <c r="Q125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Levante</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Real Betis</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>51.97%</t>
+        </is>
+      </c>
+      <c r="G126" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>15.76%</t>
+        </is>
+      </c>
+      <c r="I126" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J126" t="n">
+        <v>0.01354333851322352</v>
+      </c>
+      <c r="K126" t="n">
+        <v>0.1354333851322352</v>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" t="inlineStr"/>
+      <c r="O126" t="inlineStr"/>
+      <c r="P126" t="inlineStr"/>
+      <c r="Q126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Estrela</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Guimaraes</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>50.15%</t>
+        </is>
+      </c>
+      <c r="G127" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>14.19%</t>
+        </is>
+      </c>
+      <c r="I127" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J127" t="n">
+        <v>0.01180596490493394</v>
+      </c>
+      <c r="K127" t="n">
+        <v>0.1180596490493394</v>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" t="inlineStr"/>
+      <c r="O127" t="inlineStr"/>
+      <c r="P127" t="inlineStr"/>
+      <c r="Q127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Stade Brestois 29</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Paris FC</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>50.17%</t>
+        </is>
+      </c>
+      <c r="G128" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>11.76%</t>
+        </is>
+      </c>
+      <c r="I128" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J128" t="n">
+        <v>0.01030979901131838</v>
+      </c>
+      <c r="K128" t="n">
+        <v>0.1030979901131838</v>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" t="inlineStr"/>
+      <c r="O128" t="inlineStr"/>
+      <c r="P128" t="inlineStr"/>
+      <c r="Q128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Metz</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Angers</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>51.43%</t>
+        </is>
+      </c>
+      <c r="G129" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>14.56%</t>
+        </is>
+      </c>
+      <c r="I129" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J129" t="n">
+        <v>0.01257633158278628</v>
+      </c>
+      <c r="K129" t="n">
+        <v>0.1257633158278628</v>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr"/>
+      <c r="O129" t="inlineStr"/>
+      <c r="P129" t="inlineStr"/>
+      <c r="Q129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Strasbourg</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Le Havre</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>79.10%</t>
+        </is>
+      </c>
+      <c r="G130" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>26.87%</t>
+        </is>
+      </c>
+      <c r="I130" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0.04540276999099699</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0.4540276999099699</v>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr"/>
+      <c r="O130" t="inlineStr"/>
+      <c r="P130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Manchester United</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>72.76%</t>
+        </is>
+      </c>
+      <c r="G131" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>26.06%</t>
+        </is>
+      </c>
+      <c r="I131" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J131" t="n">
+        <v>0.03643947667392133</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0.3643947667392133</v>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr"/>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" t="inlineStr"/>
+      <c r="Q131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Borussia Mönchengladbach</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Werder Bremen</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>61.51%</t>
+        </is>
+      </c>
+      <c r="G132" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>18.74%</t>
+        </is>
+      </c>
+      <c r="I132" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J132" t="n">
+        <v>0.02098618985030318</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0.2098618985030318</v>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" t="inlineStr"/>
+      <c r="O132" t="inlineStr"/>
+      <c r="P132" t="inlineStr"/>
+      <c r="Q132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Sassuolo</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>61.29%</t>
+        </is>
+      </c>
+      <c r="G133" t="n">
+        <v>2</v>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>21.35%</t>
+        </is>
+      </c>
+      <c r="I133" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0.02257258681026608</v>
+      </c>
+      <c r="K133" t="n">
+        <v>0.2257258681026608</v>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M133" t="inlineStr"/>
+      <c r="N133" t="inlineStr"/>
+      <c r="O133" t="inlineStr"/>
+      <c r="P133" t="inlineStr"/>
+      <c r="Q133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Fenerbahce</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Trabzonspor</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>87.87%</t>
+        </is>
+      </c>
+      <c r="G134" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>25.27%</t>
+        </is>
+      </c>
+      <c r="I134" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J134" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K134" t="n">
+        <v>0.6030328745841734</v>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M134" t="inlineStr"/>
+      <c r="N134" t="inlineStr"/>
+      <c r="O134" t="inlineStr"/>
+      <c r="P134" t="inlineStr"/>
+      <c r="Q134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Gazişehir Gaziantep</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Kocaelispor</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>59.59%</t>
+        </is>
+      </c>
+      <c r="G135" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>20.94%</t>
+        </is>
+      </c>
+      <c r="I135" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J135" t="n">
+        <v>0.02110836872212143</v>
+      </c>
+      <c r="K135" t="n">
+        <v>0.2110836872212143</v>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M135" t="inlineStr"/>
+      <c r="N135" t="inlineStr"/>
+      <c r="O135" t="inlineStr"/>
+      <c r="P135" t="inlineStr"/>
+      <c r="Q135" t="inlineStr"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Arouca</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Casa Pia</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>61.04%</t>
+        </is>
+      </c>
+      <c r="G136" t="n">
+        <v>2</v>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>20.85%</t>
+        </is>
+      </c>
+      <c r="I136" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0.02207190588922747</v>
+      </c>
+      <c r="K136" t="n">
+        <v>0.2207190588922747</v>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr"/>
+      <c r="N136" t="inlineStr"/>
+      <c r="O136" t="inlineStr"/>
+      <c r="P136" t="inlineStr"/>
+      <c r="Q136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>St. Truiden</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>KVC Westerlo</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>61.30%</t>
+        </is>
+      </c>
+      <c r="G137" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>18.34%</t>
+        </is>
+      </c>
+      <c r="I137" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J137" t="n">
+        <v>0.02056033433299227</v>
+      </c>
+      <c r="K137" t="n">
+        <v>0.2056033433299227</v>
+      </c>
+      <c r="L137" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" t="inlineStr"/>
+      <c r="O137" t="inlineStr"/>
+      <c r="P137" t="inlineStr"/>
+      <c r="Q137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Leones Negros UDG</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>CA La Paz</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>79.85%</t>
+        </is>
+      </c>
+      <c r="G138" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>26.48%</t>
+        </is>
+      </c>
+      <c r="I138" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J138" t="n">
+        <v>0.04625747396032839</v>
+      </c>
+      <c r="K138" t="n">
+        <v>0.4625747396032839</v>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" t="inlineStr"/>
+      <c r="O138" t="inlineStr"/>
+      <c r="P138" t="inlineStr"/>
+      <c r="Q138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>AC Milan</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>64.66%</t>
+        </is>
+      </c>
+      <c r="G139" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>22.27%</t>
+        </is>
+      </c>
+      <c r="I139" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0.02582843735030266</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0.2582843735030266</v>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M139" t="inlineStr"/>
+      <c r="N139" t="inlineStr"/>
+      <c r="O139" t="inlineStr"/>
+      <c r="P139" t="inlineStr"/>
+      <c r="Q139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>SC Braga</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>GIL Vicente</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>84.10%</t>
+        </is>
+      </c>
+      <c r="G140" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>24.89%</t>
+        </is>
+      </c>
+      <c r="I140" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J140" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K140" t="n">
+        <v>0.5230112549280651</v>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M140" t="inlineStr"/>
+      <c r="N140" t="inlineStr"/>
+      <c r="O140" t="inlineStr"/>
+      <c r="P140" t="inlineStr"/>
+      <c r="Q140" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-14 18:25:27 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q140"/>
+  <dimension ref="A1:Q144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6420,14 +6420,30 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr"/>
-      <c r="N80" t="inlineStr"/>
-      <c r="O80" t="inlineStr"/>
-      <c r="P80" t="inlineStr"/>
-      <c r="Q80" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O80" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="P80" t="n">
+        <v>105</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -6479,14 +6495,30 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr"/>
-      <c r="N81" t="inlineStr"/>
-      <c r="O81" t="inlineStr"/>
-      <c r="P81" t="inlineStr"/>
-      <c r="Q81" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O81" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="P81" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -6538,14 +6570,30 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr"/>
-      <c r="N82" t="inlineStr"/>
-      <c r="O82" t="inlineStr"/>
-      <c r="P82" t="inlineStr"/>
-      <c r="Q82" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O82" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="P82" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -6597,14 +6645,30 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr"/>
-      <c r="N83" t="inlineStr"/>
-      <c r="O83" t="inlineStr"/>
-      <c r="P83" t="inlineStr"/>
-      <c r="Q83" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O83" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="P83" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -6656,14 +6720,30 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
-      <c r="O84" t="inlineStr"/>
-      <c r="P84" t="inlineStr"/>
-      <c r="Q84" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O84" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="P84" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -6715,14 +6795,30 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M85" t="inlineStr"/>
-      <c r="N85" t="inlineStr"/>
-      <c r="O85" t="inlineStr"/>
-      <c r="P85" t="inlineStr"/>
-      <c r="Q85" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O85" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="P85" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -6774,14 +6870,30 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr"/>
-      <c r="N86" t="inlineStr"/>
-      <c r="O86" t="inlineStr"/>
-      <c r="P86" t="inlineStr"/>
-      <c r="Q86" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O86" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="P86" t="n">
+        <v>91</v>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -6833,14 +6945,30 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr"/>
-      <c r="N87" t="inlineStr"/>
-      <c r="O87" t="inlineStr"/>
-      <c r="P87" t="inlineStr"/>
-      <c r="Q87" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O87" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="P87" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -6892,14 +7020,30 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
-      <c r="O88" t="inlineStr"/>
-      <c r="P88" t="inlineStr"/>
-      <c r="Q88" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O88" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="P88" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6951,14 +7095,30 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
-      <c r="O89" t="inlineStr"/>
-      <c r="P89" t="inlineStr"/>
-      <c r="Q89" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O89" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="P89" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -7010,14 +7170,30 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr"/>
-      <c r="P90" t="inlineStr"/>
-      <c r="Q90" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O90" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="P90" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -7069,14 +7245,30 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr"/>
-      <c r="N91" t="inlineStr"/>
-      <c r="O91" t="inlineStr"/>
-      <c r="P91" t="inlineStr"/>
-      <c r="Q91" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O91" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="P91" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -7128,14 +7320,30 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
-      <c r="O92" t="inlineStr"/>
-      <c r="P92" t="inlineStr"/>
-      <c r="Q92" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O92" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="P92" t="n">
+        <v>48</v>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -7187,14 +7395,30 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr"/>
-      <c r="N93" t="inlineStr"/>
-      <c r="O93" t="inlineStr"/>
-      <c r="P93" t="inlineStr"/>
-      <c r="Q93" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O93" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="P93" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -7246,14 +7470,30 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr"/>
-      <c r="N94" t="inlineStr"/>
-      <c r="O94" t="inlineStr"/>
-      <c r="P94" t="inlineStr"/>
-      <c r="Q94" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O94" t="n">
+        <v>-2.6</v>
+      </c>
+      <c r="P94" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -7305,14 +7545,30 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr"/>
-      <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr"/>
-      <c r="P95" t="inlineStr"/>
-      <c r="Q95" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O95" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="P95" t="n">
+        <v>53</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -7364,14 +7620,30 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr"/>
-      <c r="N96" t="inlineStr"/>
-      <c r="O96" t="inlineStr"/>
-      <c r="P96" t="inlineStr"/>
-      <c r="Q96" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O96" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="P96" t="n">
+        <v>62</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -7423,14 +7695,30 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M97" t="inlineStr"/>
-      <c r="N97" t="inlineStr"/>
-      <c r="O97" t="inlineStr"/>
-      <c r="P97" t="inlineStr"/>
-      <c r="Q97" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O97" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="P97" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -7482,14 +7770,30 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr"/>
-      <c r="P98" t="inlineStr"/>
-      <c r="Q98" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O98" t="n">
+        <v>-1.1</v>
+      </c>
+      <c r="P98" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -7541,14 +7845,30 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr"/>
-      <c r="N99" t="inlineStr"/>
-      <c r="O99" t="inlineStr"/>
-      <c r="P99" t="inlineStr"/>
-      <c r="Q99" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O99" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="P99" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>2025-09-14 04:25:49</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -7600,14 +7920,30 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr"/>
-      <c r="N100" t="inlineStr"/>
-      <c r="O100" t="inlineStr"/>
-      <c r="P100" t="inlineStr"/>
-      <c r="Q100" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O100" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P100" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:33</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -7659,14 +7995,30 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr"/>
-      <c r="N101" t="inlineStr"/>
-      <c r="O101" t="inlineStr"/>
-      <c r="P101" t="inlineStr"/>
-      <c r="Q101" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O101" t="n">
+        <v>-2.3</v>
+      </c>
+      <c r="P101" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:33</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -7718,14 +8070,30 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M102" t="inlineStr"/>
-      <c r="N102" t="inlineStr"/>
-      <c r="O102" t="inlineStr"/>
-      <c r="P102" t="inlineStr"/>
-      <c r="Q102" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O102" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P102" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:33</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -7777,14 +8145,30 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M103" t="inlineStr"/>
-      <c r="N103" t="inlineStr"/>
-      <c r="O103" t="inlineStr"/>
-      <c r="P103" t="inlineStr"/>
-      <c r="Q103" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O103" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="P103" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:33</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -7836,14 +8220,30 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr"/>
-      <c r="N104" t="inlineStr"/>
-      <c r="O104" t="inlineStr"/>
-      <c r="P104" t="inlineStr"/>
-      <c r="Q104" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O104" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="P104" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:33</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -7895,14 +8295,30 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M105" t="inlineStr"/>
-      <c r="N105" t="inlineStr"/>
-      <c r="O105" t="inlineStr"/>
-      <c r="P105" t="inlineStr"/>
-      <c r="Q105" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O105" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="P105" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:33</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -7954,14 +8370,30 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M106" t="inlineStr"/>
-      <c r="N106" t="inlineStr"/>
-      <c r="O106" t="inlineStr"/>
-      <c r="P106" t="inlineStr"/>
-      <c r="Q106" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O106" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P106" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:33</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -8013,14 +8445,30 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M107" t="inlineStr"/>
-      <c r="N107" t="inlineStr"/>
-      <c r="O107" t="inlineStr"/>
-      <c r="P107" t="inlineStr"/>
-      <c r="Q107" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O107" t="n">
+        <v>-2.3</v>
+      </c>
+      <c r="P107" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:33</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -9969,6 +10417,242 @@
       <c r="P140" t="inlineStr"/>
       <c r="Q140" t="inlineStr"/>
     </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Irapuato</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Tepatitlán</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>54.89%</t>
+        </is>
+      </c>
+      <c r="G141" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>16.83%</t>
+        </is>
+      </c>
+      <c r="I141" t="n">
+        <v>1</v>
+      </c>
+      <c r="J141" t="n">
+        <v>0.01566385563149848</v>
+      </c>
+      <c r="K141" t="n">
+        <v>0.1566385563149848</v>
+      </c>
+      <c r="L141" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M141" t="inlineStr"/>
+      <c r="N141" t="inlineStr"/>
+      <c r="O141" t="inlineStr"/>
+      <c r="P141" t="inlineStr"/>
+      <c r="Q141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Rizespor</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Genclerbirligi</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>77.51%</t>
+        </is>
+      </c>
+      <c r="G142" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>24.32%</t>
+        </is>
+      </c>
+      <c r="I142" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J142" t="n">
+        <v>0.04124871888302439</v>
+      </c>
+      <c r="K142" t="n">
+        <v>0.4124871888302438</v>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M142" t="inlineStr"/>
+      <c r="N142" t="inlineStr"/>
+      <c r="O142" t="inlineStr"/>
+      <c r="P142" t="inlineStr"/>
+      <c r="Q142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>77.08%</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>25.91%</t>
+        </is>
+      </c>
+      <c r="I143" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J143" t="n">
+        <v>0.04182086198902012</v>
+      </c>
+      <c r="K143" t="n">
+        <v>0.4182086198902012</v>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M143" t="inlineStr"/>
+      <c r="N143" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
+      <c r="P143" t="inlineStr"/>
+      <c r="Q143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Espanyol</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>53.12%</t>
+        </is>
+      </c>
+      <c r="G144" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>15.69%</t>
+        </is>
+      </c>
+      <c r="I144" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J144" t="n">
+        <v>0.01404630659222537</v>
+      </c>
+      <c r="K144" t="n">
+        <v>0.1404630659222537</v>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr"/>
+      <c r="N144" t="inlineStr"/>
+      <c r="O144" t="inlineStr"/>
+      <c r="P144" t="inlineStr"/>
+      <c r="Q144" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-15 18:46:38 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q144"/>
+  <dimension ref="A1:Q149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8520,14 +8520,30 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M108" t="inlineStr"/>
-      <c r="N108" t="inlineStr"/>
-      <c r="O108" t="inlineStr"/>
-      <c r="P108" t="inlineStr"/>
-      <c r="Q108" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O108" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="P108" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -8579,14 +8595,30 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M109" t="inlineStr"/>
-      <c r="N109" t="inlineStr"/>
-      <c r="O109" t="inlineStr"/>
-      <c r="P109" t="inlineStr"/>
-      <c r="Q109" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O109" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P109" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -8638,14 +8670,30 @@
       </c>
       <c r="L110" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M110" t="inlineStr"/>
-      <c r="N110" t="inlineStr"/>
-      <c r="O110" t="inlineStr"/>
-      <c r="P110" t="inlineStr"/>
-      <c r="Q110" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O110" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="P110" t="n">
+        <v>73</v>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -8697,14 +8745,30 @@
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M111" t="inlineStr"/>
-      <c r="N111" t="inlineStr"/>
-      <c r="O111" t="inlineStr"/>
-      <c r="P111" t="inlineStr"/>
-      <c r="Q111" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O111" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="P111" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -8756,14 +8820,30 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M112" t="inlineStr"/>
-      <c r="N112" t="inlineStr"/>
-      <c r="O112" t="inlineStr"/>
-      <c r="P112" t="inlineStr"/>
-      <c r="Q112" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O112" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="P112" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -8815,14 +8895,30 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M113" t="inlineStr"/>
-      <c r="N113" t="inlineStr"/>
-      <c r="O113" t="inlineStr"/>
-      <c r="P113" t="inlineStr"/>
-      <c r="Q113" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O113" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="P113" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -8874,14 +8970,30 @@
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M114" t="inlineStr"/>
-      <c r="N114" t="inlineStr"/>
-      <c r="O114" t="inlineStr"/>
-      <c r="P114" t="inlineStr"/>
-      <c r="Q114" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O114" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P114" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -8933,14 +9045,30 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M115" t="inlineStr"/>
-      <c r="N115" t="inlineStr"/>
-      <c r="O115" t="inlineStr"/>
-      <c r="P115" t="inlineStr"/>
-      <c r="Q115" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O115" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="P115" t="n">
+        <v>105</v>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -8992,14 +9120,30 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M116" t="inlineStr"/>
-      <c r="N116" t="inlineStr"/>
-      <c r="O116" t="inlineStr"/>
-      <c r="P116" t="inlineStr"/>
-      <c r="Q116" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O116" t="n">
+        <v>-2.1</v>
+      </c>
+      <c r="P116" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -9051,14 +9195,30 @@
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M117" t="inlineStr"/>
-      <c r="N117" t="inlineStr"/>
-      <c r="O117" t="inlineStr"/>
-      <c r="P117" t="inlineStr"/>
-      <c r="Q117" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O117" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P117" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -9110,14 +9270,30 @@
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M118" t="inlineStr"/>
-      <c r="N118" t="inlineStr"/>
-      <c r="O118" t="inlineStr"/>
-      <c r="P118" t="inlineStr"/>
-      <c r="Q118" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O118" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P118" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -9169,14 +9345,30 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M119" t="inlineStr"/>
-      <c r="N119" t="inlineStr"/>
-      <c r="O119" t="inlineStr"/>
-      <c r="P119" t="inlineStr"/>
-      <c r="Q119" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O119" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="P119" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -9228,14 +9420,30 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M120" t="inlineStr"/>
-      <c r="N120" t="inlineStr"/>
-      <c r="O120" t="inlineStr"/>
-      <c r="P120" t="inlineStr"/>
-      <c r="Q120" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O120" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="P120" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -9287,14 +9495,30 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M121" t="inlineStr"/>
-      <c r="N121" t="inlineStr"/>
-      <c r="O121" t="inlineStr"/>
-      <c r="P121" t="inlineStr"/>
-      <c r="Q121" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O121" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="P121" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -9346,14 +9570,30 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M122" t="inlineStr"/>
-      <c r="N122" t="inlineStr"/>
-      <c r="O122" t="inlineStr"/>
-      <c r="P122" t="inlineStr"/>
-      <c r="Q122" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O122" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="P122" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -9405,14 +9645,30 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M123" t="inlineStr"/>
-      <c r="N123" t="inlineStr"/>
-      <c r="O123" t="inlineStr"/>
-      <c r="P123" t="inlineStr"/>
-      <c r="Q123" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O123" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="P123" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -9464,14 +9720,30 @@
       </c>
       <c r="L124" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M124" t="inlineStr"/>
-      <c r="N124" t="inlineStr"/>
-      <c r="O124" t="inlineStr"/>
-      <c r="P124" t="inlineStr"/>
-      <c r="Q124" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O124" t="n">
+        <v>-1.1</v>
+      </c>
+      <c r="P124" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -9523,14 +9795,30 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M125" t="inlineStr"/>
-      <c r="N125" t="inlineStr"/>
-      <c r="O125" t="inlineStr"/>
-      <c r="P125" t="inlineStr"/>
-      <c r="Q125" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O125" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P125" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -9582,14 +9870,30 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M126" t="inlineStr"/>
-      <c r="N126" t="inlineStr"/>
-      <c r="O126" t="inlineStr"/>
-      <c r="P126" t="inlineStr"/>
-      <c r="Q126" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N126" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O126" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="P126" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -9641,14 +9945,30 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M127" t="inlineStr"/>
-      <c r="N127" t="inlineStr"/>
-      <c r="O127" t="inlineStr"/>
-      <c r="P127" t="inlineStr"/>
-      <c r="Q127" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O127" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="P127" t="n">
+        <v>130</v>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>2025-09-15 04:27:55</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -9700,14 +10020,30 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M128" t="inlineStr"/>
-      <c r="N128" t="inlineStr"/>
-      <c r="O128" t="inlineStr"/>
-      <c r="P128" t="inlineStr"/>
-      <c r="Q128" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O128" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="P128" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -9759,14 +10095,30 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M129" t="inlineStr"/>
-      <c r="N129" t="inlineStr"/>
-      <c r="O129" t="inlineStr"/>
-      <c r="P129" t="inlineStr"/>
-      <c r="Q129" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O129" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="P129" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -9818,14 +10170,30 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M130" t="inlineStr"/>
-      <c r="N130" t="inlineStr"/>
-      <c r="O130" t="inlineStr"/>
-      <c r="P130" t="inlineStr"/>
-      <c r="Q130" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N130" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O130" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="P130" t="n">
+        <v>62</v>
+      </c>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -9877,14 +10245,30 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M131" t="inlineStr"/>
-      <c r="N131" t="inlineStr"/>
-      <c r="O131" t="inlineStr"/>
-      <c r="P131" t="inlineStr"/>
-      <c r="Q131" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N131" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O131" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="P131" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -9936,14 +10320,30 @@
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M132" t="inlineStr"/>
-      <c r="N132" t="inlineStr"/>
-      <c r="O132" t="inlineStr"/>
-      <c r="P132" t="inlineStr"/>
-      <c r="Q132" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N132" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O132" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="P132" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -9995,14 +10395,30 @@
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M133" t="inlineStr"/>
-      <c r="N133" t="inlineStr"/>
-      <c r="O133" t="inlineStr"/>
-      <c r="P133" t="inlineStr"/>
-      <c r="Q133" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N133" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O133" t="n">
+        <v>-1.3</v>
+      </c>
+      <c r="P133" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -10054,14 +10470,30 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M134" t="inlineStr"/>
-      <c r="N134" t="inlineStr"/>
-      <c r="O134" t="inlineStr"/>
-      <c r="P134" t="inlineStr"/>
-      <c r="Q134" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N134" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O134" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="P134" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -10113,14 +10545,30 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M135" t="inlineStr"/>
-      <c r="N135" t="inlineStr"/>
-      <c r="O135" t="inlineStr"/>
-      <c r="P135" t="inlineStr"/>
-      <c r="Q135" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N135" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O135" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="P135" t="n">
+        <v>105</v>
+      </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -10172,14 +10620,30 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M136" t="inlineStr"/>
-      <c r="N136" t="inlineStr"/>
-      <c r="O136" t="inlineStr"/>
-      <c r="P136" t="inlineStr"/>
-      <c r="Q136" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N136" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O136" t="n">
+        <v>-1.3</v>
+      </c>
+      <c r="P136" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -10231,14 +10695,30 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M137" t="inlineStr"/>
-      <c r="N137" t="inlineStr"/>
-      <c r="O137" t="inlineStr"/>
-      <c r="P137" t="inlineStr"/>
-      <c r="Q137" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N137" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O137" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="P137" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -10290,14 +10770,30 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M138" t="inlineStr"/>
-      <c r="N138" t="inlineStr"/>
-      <c r="O138" t="inlineStr"/>
-      <c r="P138" t="inlineStr"/>
-      <c r="Q138" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N138" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O138" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="P138" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -10349,14 +10845,30 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M139" t="inlineStr"/>
-      <c r="N139" t="inlineStr"/>
-      <c r="O139" t="inlineStr"/>
-      <c r="P139" t="inlineStr"/>
-      <c r="Q139" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N139" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O139" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="P139" t="n">
+        <v>91</v>
+      </c>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -10408,14 +10920,30 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M140" t="inlineStr"/>
-      <c r="N140" t="inlineStr"/>
-      <c r="O140" t="inlineStr"/>
-      <c r="P140" t="inlineStr"/>
-      <c r="Q140" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N140" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O140" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P140" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>2025-09-15 15:24:47</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -10653,6 +11181,301 @@
       <c r="P144" t="inlineStr"/>
       <c r="Q144" t="inlineStr"/>
     </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>PSV Eindhoven</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Union St. Gilloise</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>70.72%</t>
+        </is>
+      </c>
+      <c r="G145" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>22.53%</t>
+        </is>
+      </c>
+      <c r="I145" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J145" t="n">
+        <v>0.03168569966640591</v>
+      </c>
+      <c r="K145" t="n">
+        <v>0.316856996664059</v>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr"/>
+      <c r="N145" t="inlineStr"/>
+      <c r="O145" t="inlineStr"/>
+      <c r="P145" t="inlineStr"/>
+      <c r="Q145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Athletic Club</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>69.75%</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>27.75%</t>
+        </is>
+      </c>
+      <c r="I146" t="n">
+        <v>2</v>
+      </c>
+      <c r="J146" t="n">
+        <v>0.03417091746492983</v>
+      </c>
+      <c r="K146" t="n">
+        <v>0.3417091746492983</v>
+      </c>
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" t="inlineStr"/>
+      <c r="O146" t="inlineStr"/>
+      <c r="P146" t="inlineStr"/>
+      <c r="Q146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Borussia Dortmund</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>62.00%</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
+        <v>2</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>22.76%</t>
+        </is>
+      </c>
+      <c r="I147" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J147" t="n">
+        <v>0.02400252147796229</v>
+      </c>
+      <c r="K147" t="n">
+        <v>0.2400252147796229</v>
+      </c>
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr"/>
+      <c r="N147" t="inlineStr"/>
+      <c r="O147" t="inlineStr"/>
+      <c r="P147" t="inlineStr"/>
+      <c r="Q147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>68.40%</t>
+        </is>
+      </c>
+      <c r="G148" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>25.27%</t>
+        </is>
+      </c>
+      <c r="I148" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J148" t="n">
+        <v>0.0312141166391008</v>
+      </c>
+      <c r="K148" t="n">
+        <v>0.312141166391008</v>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr"/>
+      <c r="N148" t="inlineStr"/>
+      <c r="O148" t="inlineStr"/>
+      <c r="P148" t="inlineStr"/>
+      <c r="Q148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Inter Miami</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Seattle Sounders</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>61.05%</t>
+        </is>
+      </c>
+      <c r="G149" t="n">
+        <v>2</v>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>20.89%</t>
+        </is>
+      </c>
+      <c r="I149" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J149" t="n">
+        <v>0.0221066358449753</v>
+      </c>
+      <c r="K149" t="n">
+        <v>0.221066358449753</v>
+      </c>
+      <c r="L149" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr"/>
+      <c r="N149" t="inlineStr"/>
+      <c r="O149" t="inlineStr"/>
+      <c r="P149" t="inlineStr"/>
+      <c r="Q149" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-16 18:46:18 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q149"/>
+  <dimension ref="A1:Q159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10995,14 +10995,30 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M141" t="inlineStr"/>
-      <c r="N141" t="inlineStr"/>
-      <c r="O141" t="inlineStr"/>
-      <c r="P141" t="inlineStr"/>
-      <c r="Q141" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N141" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O141" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P141" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>2025-09-16 04:26:19</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -11054,14 +11070,30 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M142" t="inlineStr"/>
-      <c r="N142" t="inlineStr"/>
-      <c r="O142" t="inlineStr"/>
-      <c r="P142" t="inlineStr"/>
-      <c r="Q142" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N142" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O142" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="P142" t="n">
+        <v>62</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>2025-09-16 04:26:19</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -11113,14 +11145,30 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M143" t="inlineStr"/>
-      <c r="N143" t="inlineStr"/>
-      <c r="O143" t="inlineStr"/>
-      <c r="P143" t="inlineStr"/>
-      <c r="Q143" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N143" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O143" t="n">
+        <v>-2.6</v>
+      </c>
+      <c r="P143" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>2025-09-16 04:26:19</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -11172,14 +11220,30 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M144" t="inlineStr"/>
-      <c r="N144" t="inlineStr"/>
-      <c r="O144" t="inlineStr"/>
-      <c r="P144" t="inlineStr"/>
-      <c r="Q144" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N144" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O144" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="P144" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>2025-09-16 04:26:19</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -11476,6 +11540,596 @@
       <c r="P149" t="inlineStr"/>
       <c r="Q149" t="inlineStr"/>
     </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Olympiakos Piraeus</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Pafos</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>90.20%</t>
+        </is>
+      </c>
+      <c r="G150" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>25.02%</t>
+        </is>
+      </c>
+      <c r="I150" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J150" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K150" t="n">
+        <v>0.6570343192575333</v>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr"/>
+      <c r="N150" t="inlineStr"/>
+      <c r="O150" t="inlineStr"/>
+      <c r="P150" t="inlineStr"/>
+      <c r="Q150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Slavia Praha</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Bodo/Glimt</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>73.18%</t>
+        </is>
+      </c>
+      <c r="G151" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>26.78%</t>
+        </is>
+      </c>
+      <c r="I151" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J151" t="n">
+        <v>0.03742001338783531</v>
+      </c>
+      <c r="K151" t="n">
+        <v>0.3742001338783531</v>
+      </c>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr"/>
+      <c r="N151" t="inlineStr"/>
+      <c r="O151" t="inlineStr"/>
+      <c r="P151" t="inlineStr"/>
+      <c r="Q151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Fatih Karagümrük</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Istanbul Basaksehir</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>64.52%</t>
+        </is>
+      </c>
+      <c r="G152" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>22.00%</t>
+        </is>
+      </c>
+      <c r="I152" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J152" t="n">
+        <v>0.0255302801976002</v>
+      </c>
+      <c r="K152" t="n">
+        <v>0.255302801976002</v>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr"/>
+      <c r="N152" t="inlineStr"/>
+      <c r="O152" t="inlineStr"/>
+      <c r="P152" t="inlineStr"/>
+      <c r="Q152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Samsunspor</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Kasimpasa</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>70.54%</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>25.70%</t>
+        </is>
+      </c>
+      <c r="I153" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J153" t="n">
+        <v>0.03371245248403483</v>
+      </c>
+      <c r="K153" t="n">
+        <v>0.3371245248403483</v>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr"/>
+      <c r="N153" t="inlineStr"/>
+      <c r="O153" t="inlineStr"/>
+      <c r="P153" t="inlineStr"/>
+      <c r="Q153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Genk</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Charleroi</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>72.78%</t>
+        </is>
+      </c>
+      <c r="G154" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>22.50%</t>
+        </is>
+      </c>
+      <c r="I154" t="n">
+        <v>2</v>
+      </c>
+      <c r="J154" t="n">
+        <v>0.03390349092324032</v>
+      </c>
+      <c r="K154" t="n">
+        <v>0.3390349092324031</v>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr"/>
+      <c r="N154" t="inlineStr"/>
+      <c r="O154" t="inlineStr"/>
+      <c r="P154" t="inlineStr"/>
+      <c r="Q154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Ajax</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>71.12%</t>
+        </is>
+      </c>
+      <c r="G155" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>26.74%</t>
+        </is>
+      </c>
+      <c r="I155" t="n">
+        <v>2</v>
+      </c>
+      <c r="J155" t="n">
+        <v>0.03501982061867995</v>
+      </c>
+      <c r="K155" t="n">
+        <v>0.3501982061867995</v>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr"/>
+      <c r="N155" t="inlineStr"/>
+      <c r="O155" t="inlineStr"/>
+      <c r="P155" t="inlineStr"/>
+      <c r="Q155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Paris Saint Germain</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>87.75%</t>
+        </is>
+      </c>
+      <c r="G156" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>25.97%</t>
+        </is>
+      </c>
+      <c r="I156" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J156" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K156" t="n">
+        <v>0.6053342623591915</v>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M156" t="inlineStr"/>
+      <c r="N156" t="inlineStr"/>
+      <c r="O156" t="inlineStr"/>
+      <c r="P156" t="inlineStr"/>
+      <c r="Q156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>84.57%</t>
+        </is>
+      </c>
+      <c r="G157" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>25.58%</t>
+        </is>
+      </c>
+      <c r="I157" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J157" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K157" t="n">
+        <v>0.5369698608511987</v>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M157" t="inlineStr"/>
+      <c r="N157" t="inlineStr"/>
+      <c r="O157" t="inlineStr"/>
+      <c r="P157" t="inlineStr"/>
+      <c r="Q157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Bayern München</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>78.13%</t>
+        </is>
+      </c>
+      <c r="G158" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>27.62%</t>
+        </is>
+      </c>
+      <c r="I158" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J158" t="n">
+        <v>0.04447810602235108</v>
+      </c>
+      <c r="K158" t="n">
+        <v>0.4447810602235108</v>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M158" t="inlineStr"/>
+      <c r="N158" t="inlineStr"/>
+      <c r="O158" t="inlineStr"/>
+      <c r="P158" t="inlineStr"/>
+      <c r="Q158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>New York City FC</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Columbus Crew</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>55.20%</t>
+        </is>
+      </c>
+      <c r="G159" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>14.76%</t>
+        </is>
+      </c>
+      <c r="I159" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J159" t="n">
+        <v>0.01446775813821211</v>
+      </c>
+      <c r="K159" t="n">
+        <v>0.1446775813821211</v>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M159" t="inlineStr"/>
+      <c r="N159" t="inlineStr"/>
+      <c r="O159" t="inlineStr"/>
+      <c r="P159" t="inlineStr"/>
+      <c r="Q159" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-17 18:46:21 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q159"/>
+  <dimension ref="A1:Q163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11295,14 +11295,30 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M145" t="inlineStr"/>
-      <c r="N145" t="inlineStr"/>
-      <c r="O145" t="inlineStr"/>
-      <c r="P145" t="inlineStr"/>
-      <c r="Q145" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N145" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O145" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="P145" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>2025-09-17 04:26:45</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -11354,14 +11370,30 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M146" t="inlineStr"/>
-      <c r="N146" t="inlineStr"/>
-      <c r="O146" t="inlineStr"/>
-      <c r="P146" t="inlineStr"/>
-      <c r="Q146" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N146" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O146" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="P146" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>2025-09-17 04:26:45</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -11413,14 +11445,30 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M147" t="inlineStr"/>
-      <c r="N147" t="inlineStr"/>
-      <c r="O147" t="inlineStr"/>
-      <c r="P147" t="inlineStr"/>
-      <c r="Q147" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O147" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="P147" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>2025-09-17 04:26:45</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -11472,14 +11520,30 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M148" t="inlineStr"/>
-      <c r="N148" t="inlineStr"/>
-      <c r="O148" t="inlineStr"/>
-      <c r="P148" t="inlineStr"/>
-      <c r="Q148" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O148" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="P148" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>2025-09-17 04:26:45</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -11531,14 +11595,30 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M149" t="inlineStr"/>
-      <c r="N149" t="inlineStr"/>
-      <c r="O149" t="inlineStr"/>
-      <c r="P149" t="inlineStr"/>
-      <c r="Q149" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N149" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O149" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P149" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>2025-09-17 04:26:45</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -12130,6 +12210,242 @@
       <c r="P159" t="inlineStr"/>
       <c r="Q159" t="inlineStr"/>
     </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Real Salt Lake</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Los Angeles FC</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>48.27%</t>
+        </is>
+      </c>
+      <c r="G160" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>7.51%</t>
+        </is>
+      </c>
+      <c r="I160" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J160" t="n">
+        <v>0.006880097657915255</v>
+      </c>
+      <c r="K160" t="n">
+        <v>0.06880097657915255</v>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M160" t="inlineStr"/>
+      <c r="N160" t="inlineStr"/>
+      <c r="O160" t="inlineStr"/>
+      <c r="P160" t="inlineStr"/>
+      <c r="Q160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>FC Copenhagen</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Bayer Leverkusen</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>54.26%</t>
+        </is>
+      </c>
+      <c r="G161" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>15.50%</t>
+        </is>
+      </c>
+      <c r="I161" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J161" t="n">
+        <v>0.01449162217910136</v>
+      </c>
+      <c r="K161" t="n">
+        <v>0.1449162217910136</v>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M161" t="inlineStr"/>
+      <c r="N161" t="inlineStr"/>
+      <c r="O161" t="inlineStr"/>
+      <c r="P161" t="inlineStr"/>
+      <c r="Q161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Eintracht Frankfurt</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Galatasaray</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>54.05%</t>
+        </is>
+      </c>
+      <c r="G162" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>12.37%</t>
+        </is>
+      </c>
+      <c r="I162" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J162" t="n">
+        <v>0.0122756764106551</v>
+      </c>
+      <c r="K162" t="n">
+        <v>0.122756764106551</v>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M162" t="inlineStr"/>
+      <c r="N162" t="inlineStr"/>
+      <c r="O162" t="inlineStr"/>
+      <c r="P162" t="inlineStr"/>
+      <c r="Q162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>UEFA Champions League</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>77.32%</t>
+        </is>
+      </c>
+      <c r="G163" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>26.30%</t>
+        </is>
+      </c>
+      <c r="I163" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J163" t="n">
+        <v>0.04242606754060104</v>
+      </c>
+      <c r="K163" t="n">
+        <v>0.4242606754060104</v>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M163" t="inlineStr"/>
+      <c r="N163" t="inlineStr"/>
+      <c r="O163" t="inlineStr"/>
+      <c r="P163" t="inlineStr"/>
+      <c r="Q163" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-18 18:48:01 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q163"/>
+  <dimension ref="A1:Q169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11670,14 +11670,30 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M150" t="inlineStr"/>
-      <c r="N150" t="inlineStr"/>
-      <c r="O150" t="inlineStr"/>
-      <c r="P150" t="inlineStr"/>
-      <c r="Q150" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N150" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O150" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P150" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -11729,14 +11745,30 @@
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M151" t="inlineStr"/>
-      <c r="N151" t="inlineStr"/>
-      <c r="O151" t="inlineStr"/>
-      <c r="P151" t="inlineStr"/>
-      <c r="Q151" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N151" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O151" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="P151" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -11788,14 +11820,30 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M152" t="inlineStr"/>
-      <c r="N152" t="inlineStr"/>
-      <c r="O152" t="inlineStr"/>
-      <c r="P152" t="inlineStr"/>
-      <c r="Q152" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N152" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O152" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="P152" t="n">
+        <v>91</v>
+      </c>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -11847,14 +11895,30 @@
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M153" t="inlineStr"/>
-      <c r="N153" t="inlineStr"/>
-      <c r="O153" t="inlineStr"/>
-      <c r="P153" t="inlineStr"/>
-      <c r="Q153" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O153" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="P153" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -11906,14 +11970,30 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M154" t="inlineStr"/>
-      <c r="N154" t="inlineStr"/>
-      <c r="O154" t="inlineStr"/>
-      <c r="P154" t="inlineStr"/>
-      <c r="Q154" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N154" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O154" t="n">
+        <v>-2</v>
+      </c>
+      <c r="P154" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -11965,14 +12045,30 @@
       </c>
       <c r="L155" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M155" t="inlineStr"/>
-      <c r="N155" t="inlineStr"/>
-      <c r="O155" t="inlineStr"/>
-      <c r="P155" t="inlineStr"/>
-      <c r="Q155" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N155" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O155" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="P155" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -12024,14 +12120,30 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M156" t="inlineStr"/>
-      <c r="N156" t="inlineStr"/>
-      <c r="O156" t="inlineStr"/>
-      <c r="P156" t="inlineStr"/>
-      <c r="Q156" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N156" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O156" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P156" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q156" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -12083,14 +12195,30 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M157" t="inlineStr"/>
-      <c r="N157" t="inlineStr"/>
-      <c r="O157" t="inlineStr"/>
-      <c r="P157" t="inlineStr"/>
-      <c r="Q157" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N157" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O157" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="P157" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q157" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -12142,14 +12270,30 @@
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M158" t="inlineStr"/>
-      <c r="N158" t="inlineStr"/>
-      <c r="O158" t="inlineStr"/>
-      <c r="P158" t="inlineStr"/>
-      <c r="Q158" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N158" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O158" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="P158" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -12201,14 +12345,30 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M159" t="inlineStr"/>
-      <c r="N159" t="inlineStr"/>
-      <c r="O159" t="inlineStr"/>
-      <c r="P159" t="inlineStr"/>
-      <c r="Q159" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N159" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O159" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="P159" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:27:14</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -12446,6 +12606,360 @@
       <c r="P163" t="inlineStr"/>
       <c r="Q163" t="inlineStr"/>
     </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Sparta Rotterdam</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Twente</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>45.05%</t>
+        </is>
+      </c>
+      <c r="G164" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>4.81%</t>
+        </is>
+      </c>
+      <c r="I164" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J164" t="n">
+        <v>0.004344782829934631</v>
+      </c>
+      <c r="K164" t="n">
+        <v>0.04344782829934631</v>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M164" t="inlineStr"/>
+      <c r="N164" t="inlineStr"/>
+      <c r="O164" t="inlineStr"/>
+      <c r="P164" t="inlineStr"/>
+      <c r="Q164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>VfB Stuttgart</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>FC St. Pauli</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>75.61%</t>
+        </is>
+      </c>
+      <c r="G165" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>29.49%</t>
+        </is>
+      </c>
+      <c r="I165" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J165" t="n">
+        <v>0.04218802910321603</v>
+      </c>
+      <c r="K165" t="n">
+        <v>0.4218802910321602</v>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr"/>
+      <c r="N165" t="inlineStr"/>
+      <c r="O165" t="inlineStr"/>
+      <c r="P165" t="inlineStr"/>
+      <c r="Q165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Gent</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Dender</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>71.79%</t>
+        </is>
+      </c>
+      <c r="G166" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>22.96%</t>
+        </is>
+      </c>
+      <c r="I166" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J166" t="n">
+        <v>0.03314905704217487</v>
+      </c>
+      <c r="K166" t="n">
+        <v>0.3314905704217487</v>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M166" t="inlineStr"/>
+      <c r="N166" t="inlineStr"/>
+      <c r="O166" t="inlineStr"/>
+      <c r="P166" t="inlineStr"/>
+      <c r="Q166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Real Betis</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>62.37%</t>
+        </is>
+      </c>
+      <c r="G167" t="n">
+        <v>2</v>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>23.49%</t>
+        </is>
+      </c>
+      <c r="I167" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J167" t="n">
+        <v>0.02473234525645181</v>
+      </c>
+      <c r="K167" t="n">
+        <v>0.247323452564518</v>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" t="inlineStr"/>
+      <c r="O167" t="inlineStr"/>
+      <c r="P167" t="inlineStr"/>
+      <c r="Q167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Rio Ave</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>FC Porto</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>90.96%</t>
+        </is>
+      </c>
+      <c r="G168" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>27.87%</t>
+        </is>
+      </c>
+      <c r="I168" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J168" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K168" t="n">
+        <v>0.6943610353896599</v>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M168" t="inlineStr"/>
+      <c r="N168" t="inlineStr"/>
+      <c r="O168" t="inlineStr"/>
+      <c r="P168" t="inlineStr"/>
+      <c r="Q168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Tapatío</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Correcaminos Uat</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>71.94%</t>
+        </is>
+      </c>
+      <c r="G169" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>17.51%</t>
+        </is>
+      </c>
+      <c r="I169" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J169" t="n">
+        <v>0.02876458510447492</v>
+      </c>
+      <c r="K169" t="n">
+        <v>0.2876458510447492</v>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" t="inlineStr"/>
+      <c r="O169" t="inlineStr"/>
+      <c r="P169" t="inlineStr"/>
+      <c r="Q169" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-19 18:45:44 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q169"/>
+  <dimension ref="A1:Q196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12420,14 +12420,30 @@
       </c>
       <c r="L160" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M160" t="inlineStr"/>
-      <c r="N160" t="inlineStr"/>
-      <c r="O160" t="inlineStr"/>
-      <c r="P160" t="inlineStr"/>
-      <c r="Q160" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N160" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O160" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P160" t="n">
+        <v>125</v>
+      </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>2025-09-19 04:26:51</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -12479,14 +12495,30 @@
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M161" t="inlineStr"/>
-      <c r="N161" t="inlineStr"/>
-      <c r="O161" t="inlineStr"/>
-      <c r="P161" t="inlineStr"/>
-      <c r="Q161" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O161" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P161" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q161" t="inlineStr">
+        <is>
+          <t>2025-09-19 04:26:51</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -12538,14 +12570,30 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M162" t="inlineStr"/>
-      <c r="N162" t="inlineStr"/>
-      <c r="O162" t="inlineStr"/>
-      <c r="P162" t="inlineStr"/>
-      <c r="Q162" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N162" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O162" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="P162" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>2025-09-19 04:26:51</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -12597,14 +12645,30 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M163" t="inlineStr"/>
-      <c r="N163" t="inlineStr"/>
-      <c r="O163" t="inlineStr"/>
-      <c r="P163" t="inlineStr"/>
-      <c r="Q163" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N163" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O163" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="P163" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>2025-09-19 04:26:51</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -12960,6 +13024,1599 @@
       <c r="P169" t="inlineStr"/>
       <c r="Q169" t="inlineStr"/>
     </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Tepatitlán</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Tlaxcala</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>71.07%</t>
+        </is>
+      </c>
+      <c r="G170" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>19.61%</t>
+        </is>
+      </c>
+      <c r="I170" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J170" t="n">
+        <v>0.0297339720847923</v>
+      </c>
+      <c r="K170" t="n">
+        <v>0.297339720847923</v>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" t="inlineStr"/>
+      <c r="O170" t="inlineStr"/>
+      <c r="P170" t="inlineStr"/>
+      <c r="Q170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>87.75%</t>
+        </is>
+      </c>
+      <c r="G171" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>25.97%</t>
+        </is>
+      </c>
+      <c r="I171" t="n">
+        <v>3</v>
+      </c>
+      <c r="J171" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K171" t="n">
+        <v>0.6053342623591915</v>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr"/>
+      <c r="N171" t="inlineStr"/>
+      <c r="O171" t="inlineStr"/>
+      <c r="P171" t="inlineStr"/>
+      <c r="Q171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Girona</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Levante</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>65.82%</t>
+        </is>
+      </c>
+      <c r="G172" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>24.45%</t>
+        </is>
+      </c>
+      <c r="I172" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J172" t="n">
+        <v>0.02825134617093525</v>
+      </c>
+      <c r="K172" t="n">
+        <v>0.2825134617093524</v>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr"/>
+      <c r="N172" t="inlineStr"/>
+      <c r="O172" t="inlineStr"/>
+      <c r="P172" t="inlineStr"/>
+      <c r="Q172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>66.99%</t>
+        </is>
+      </c>
+      <c r="G173" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>22.69%</t>
+        </is>
+      </c>
+      <c r="I173" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J173" t="n">
+        <v>0.02814686866463166</v>
+      </c>
+      <c r="K173" t="n">
+        <v>0.2814686866463166</v>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr"/>
+      <c r="N173" t="inlineStr"/>
+      <c r="O173" t="inlineStr"/>
+      <c r="P173" t="inlineStr"/>
+      <c r="Q173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Hamburger SV</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>1. FC Heidenheim</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>60.07%</t>
+        </is>
+      </c>
+      <c r="G174" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>21.91%</t>
+        </is>
+      </c>
+      <c r="I174" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J174" t="n">
+        <v>0.02203627120817205</v>
+      </c>
+      <c r="K174" t="n">
+        <v>0.2203627120817205</v>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr"/>
+      <c r="N174" t="inlineStr"/>
+      <c r="O174" t="inlineStr"/>
+      <c r="P174" t="inlineStr"/>
+      <c r="Q174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Nottingham Forest</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>54.03%</t>
+        </is>
+      </c>
+      <c r="G175" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>17.67%</t>
+        </is>
+      </c>
+      <c r="I175" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J175" t="n">
+        <v>0.0157147312677417</v>
+      </c>
+      <c r="K175" t="n">
+        <v>0.157147312677417</v>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M175" t="inlineStr"/>
+      <c r="N175" t="inlineStr"/>
+      <c r="O175" t="inlineStr"/>
+      <c r="P175" t="inlineStr"/>
+      <c r="Q175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>OH Leuven</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>RAAL La Louvière</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>58.71%</t>
+        </is>
+      </c>
+      <c r="G176" t="n">
+        <v>2</v>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>16.25%</t>
+        </is>
+      </c>
+      <c r="I176" t="n">
+        <v>1</v>
+      </c>
+      <c r="J176" t="n">
+        <v>0.01742688338953624</v>
+      </c>
+      <c r="K176" t="n">
+        <v>0.1742688338953624</v>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M176" t="inlineStr"/>
+      <c r="N176" t="inlineStr"/>
+      <c r="O176" t="inlineStr"/>
+      <c r="P176" t="inlineStr"/>
+      <c r="Q176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Santa Clara</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Alverca</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>73.02%</t>
+        </is>
+      </c>
+      <c r="G177" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>22.89%</t>
+        </is>
+      </c>
+      <c r="I177" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J177" t="n">
+        <v>0.03447428762155269</v>
+      </c>
+      <c r="K177" t="n">
+        <v>0.3447428762155269</v>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M177" t="inlineStr"/>
+      <c r="N177" t="inlineStr"/>
+      <c r="O177" t="inlineStr"/>
+      <c r="P177" t="inlineStr"/>
+      <c r="Q177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Nantes</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Rennes</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>57.55%</t>
+        </is>
+      </c>
+      <c r="G178" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>19.64%</t>
+        </is>
+      </c>
+      <c r="I178" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J178" t="n">
+        <v>0.01895520766078265</v>
+      </c>
+      <c r="K178" t="n">
+        <v>0.1895520766078264</v>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M178" t="inlineStr"/>
+      <c r="N178" t="inlineStr"/>
+      <c r="O178" t="inlineStr"/>
+      <c r="P178" t="inlineStr"/>
+      <c r="Q178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>New York City FC</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>62.18%</t>
+        </is>
+      </c>
+      <c r="G179" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>20.04%</t>
+        </is>
+      </c>
+      <c r="I179" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J179" t="n">
+        <v>0.02236911800293895</v>
+      </c>
+      <c r="K179" t="n">
+        <v>0.2236911800293895</v>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M179" t="inlineStr"/>
+      <c r="N179" t="inlineStr"/>
+      <c r="O179" t="inlineStr"/>
+      <c r="P179" t="inlineStr"/>
+      <c r="Q179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Verona</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>86.71%</t>
+        </is>
+      </c>
+      <c r="G180" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>33.06%</t>
+        </is>
+      </c>
+      <c r="I180" t="n">
+        <v>3</v>
+      </c>
+      <c r="J180" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K180" t="n">
+        <v>0.6255237989564904</v>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M180" t="inlineStr"/>
+      <c r="N180" t="inlineStr"/>
+      <c r="O180" t="inlineStr"/>
+      <c r="P180" t="inlineStr"/>
+      <c r="Q180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>1.FC Köln</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>79.64%</t>
+        </is>
+      </c>
+      <c r="G181" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>30.09%</t>
+        </is>
+      </c>
+      <c r="I181" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J181" t="n">
+        <v>0.04830935016684129</v>
+      </c>
+      <c r="K181" t="n">
+        <v>0.4830935016684129</v>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M181" t="inlineStr"/>
+      <c r="N181" t="inlineStr"/>
+      <c r="O181" t="inlineStr"/>
+      <c r="P181" t="inlineStr"/>
+      <c r="Q181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Osasuna</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>83.18%</t>
+        </is>
+      </c>
+      <c r="G182" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>26.00%</t>
+        </is>
+      </c>
+      <c r="I182" t="n">
+        <v>3</v>
+      </c>
+      <c r="J182" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K182" t="n">
+        <v>0.5144917479232674</v>
+      </c>
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M182" t="inlineStr"/>
+      <c r="N182" t="inlineStr"/>
+      <c r="O182" t="inlineStr"/>
+      <c r="P182" t="inlineStr"/>
+      <c r="Q182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Groningen</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Telstar</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>72.75%</t>
+        </is>
+      </c>
+      <c r="G183" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>24.60%</t>
+        </is>
+      </c>
+      <c r="I183" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J183" t="n">
+        <v>0.03541586171382875</v>
+      </c>
+      <c r="K183" t="n">
+        <v>0.3541586171382875</v>
+      </c>
+      <c r="L183" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M183" t="inlineStr"/>
+      <c r="N183" t="inlineStr"/>
+      <c r="O183" t="inlineStr"/>
+      <c r="P183" t="inlineStr"/>
+      <c r="Q183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Antalyaspor</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Kayserispor</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>52.96%</t>
+        </is>
+      </c>
+      <c r="G184" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>10.10%</t>
+        </is>
+      </c>
+      <c r="I184" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J184" t="n">
+        <v>0.01019344182333626</v>
+      </c>
+      <c r="K184" t="n">
+        <v>0.1019344182333626</v>
+      </c>
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M184" t="inlineStr"/>
+      <c r="N184" t="inlineStr"/>
+      <c r="O184" t="inlineStr"/>
+      <c r="P184" t="inlineStr"/>
+      <c r="Q184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Trabzonspor</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Gazişehir Gaziantep</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>74.63%</t>
+        </is>
+      </c>
+      <c r="G185" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>21.91%</t>
+        </is>
+      </c>
+      <c r="I185" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J185" t="n">
+        <v>0.0356065278171503</v>
+      </c>
+      <c r="K185" t="n">
+        <v>0.356065278171503</v>
+      </c>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M185" t="inlineStr"/>
+      <c r="N185" t="inlineStr"/>
+      <c r="O185" t="inlineStr"/>
+      <c r="P185" t="inlineStr"/>
+      <c r="Q185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Fortuna Sittard</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>65.75%</t>
+        </is>
+      </c>
+      <c r="G186" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>24.32%</t>
+        </is>
+      </c>
+      <c r="I186" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J186" t="n">
+        <v>0.02810525306201105</v>
+      </c>
+      <c r="K186" t="n">
+        <v>0.2810525306201105</v>
+      </c>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M186" t="inlineStr"/>
+      <c r="N186" t="inlineStr"/>
+      <c r="O186" t="inlineStr"/>
+      <c r="P186" t="inlineStr"/>
+      <c r="Q186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Philadelphia Union</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>New England Revolution</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>83.68%</t>
+        </is>
+      </c>
+      <c r="G187" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>26.74%</t>
+        </is>
+      </c>
+      <c r="I187" t="n">
+        <v>3</v>
+      </c>
+      <c r="J187" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K187" t="n">
+        <v>0.5287626762530216</v>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M187" t="inlineStr"/>
+      <c r="N187" t="inlineStr"/>
+      <c r="O187" t="inlineStr"/>
+      <c r="P187" t="inlineStr"/>
+      <c r="Q187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>AC Milan</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>70.52%</t>
+        </is>
+      </c>
+      <c r="G188" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>27.76%</t>
+        </is>
+      </c>
+      <c r="I188" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J188" t="n">
+        <v>0.03500238967882782</v>
+      </c>
+      <c r="K188" t="n">
+        <v>0.3500238967882781</v>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M188" t="inlineStr"/>
+      <c r="N188" t="inlineStr"/>
+      <c r="O188" t="inlineStr"/>
+      <c r="P188" t="inlineStr"/>
+      <c r="Q188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Anderlecht</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Antwerp</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>74.71%</t>
+        </is>
+      </c>
+      <c r="G189" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>23.53%</t>
+        </is>
+      </c>
+      <c r="I189" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J189" t="n">
+        <v>0.03697455724965507</v>
+      </c>
+      <c r="K189" t="n">
+        <v>0.3697455724965507</v>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M189" t="inlineStr"/>
+      <c r="N189" t="inlineStr"/>
+      <c r="O189" t="inlineStr"/>
+      <c r="P189" t="inlineStr"/>
+      <c r="Q189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>62.22%</t>
+        </is>
+      </c>
+      <c r="G190" t="n">
+        <v>2</v>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>23.20%</t>
+        </is>
+      </c>
+      <c r="I190" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J190" t="n">
+        <v>0.02444102816862315</v>
+      </c>
+      <c r="K190" t="n">
+        <v>0.2444102816862315</v>
+      </c>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M190" t="inlineStr"/>
+      <c r="N190" t="inlineStr"/>
+      <c r="O190" t="inlineStr"/>
+      <c r="P190" t="inlineStr"/>
+      <c r="Q190" t="inlineStr"/>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>NAC Breda</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Heracles</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>57.30%</t>
+        </is>
+      </c>
+      <c r="G191" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>19.13%</t>
+        </is>
+      </c>
+      <c r="I191" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J191" t="n">
+        <v>0.01848467630931988</v>
+      </c>
+      <c r="K191" t="n">
+        <v>0.1848467630931988</v>
+      </c>
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M191" t="inlineStr"/>
+      <c r="N191" t="inlineStr"/>
+      <c r="O191" t="inlineStr"/>
+      <c r="P191" t="inlineStr"/>
+      <c r="Q191" t="inlineStr"/>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Athletic Club</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>41.11%</t>
+        </is>
+      </c>
+      <c r="G192" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>5.81%</t>
+        </is>
+      </c>
+      <c r="I192" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J192" t="n">
+        <v>0.004302016136839969</v>
+      </c>
+      <c r="K192" t="n">
+        <v>0.04302016136839969</v>
+      </c>
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M192" t="inlineStr"/>
+      <c r="N192" t="inlineStr"/>
+      <c r="O192" t="inlineStr"/>
+      <c r="P192" t="inlineStr"/>
+      <c r="Q192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Guimaraes</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>SC Braga</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>50.61%</t>
+        </is>
+      </c>
+      <c r="G193" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>15.24%</t>
+        </is>
+      </c>
+      <c r="I193" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J193" t="n">
+        <v>0.01261885373257252</v>
+      </c>
+      <c r="K193" t="n">
+        <v>0.1261885373257252</v>
+      </c>
+      <c r="L193" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M193" t="inlineStr"/>
+      <c r="N193" t="inlineStr"/>
+      <c r="O193" t="inlineStr"/>
+      <c r="P193" t="inlineStr"/>
+      <c r="Q193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Columbus Crew</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Toronto FC</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>86.57%</t>
+        </is>
+      </c>
+      <c r="G194" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>24.27%</t>
+        </is>
+      </c>
+      <c r="I194" t="n">
+        <v>3</v>
+      </c>
+      <c r="J194" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K194" t="n">
+        <v>0.5671545306825067</v>
+      </c>
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M194" t="inlineStr"/>
+      <c r="N194" t="inlineStr"/>
+      <c r="O194" t="inlineStr"/>
+      <c r="P194" t="inlineStr"/>
+      <c r="Q194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>CF Montreal</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>New York Red Bulls</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>47.36%</t>
+        </is>
+      </c>
+      <c r="G195" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>7.85%</t>
+        </is>
+      </c>
+      <c r="I195" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J195" t="n">
+        <v>0.006875409234375524</v>
+      </c>
+      <c r="K195" t="n">
+        <v>0.06875409234375524</v>
+      </c>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M195" t="inlineStr"/>
+      <c r="N195" t="inlineStr"/>
+      <c r="O195" t="inlineStr"/>
+      <c r="P195" t="inlineStr"/>
+      <c r="Q195" t="inlineStr"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Orlando City SC</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Nashville SC</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>56.10%</t>
+        </is>
+      </c>
+      <c r="G196" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>16.64%</t>
+        </is>
+      </c>
+      <c r="I196" t="n">
+        <v>1</v>
+      </c>
+      <c r="J196" t="n">
+        <v>0.01619684359091262</v>
+      </c>
+      <c r="K196" t="n">
+        <v>0.1619684359091262</v>
+      </c>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M196" t="inlineStr"/>
+      <c r="N196" t="inlineStr"/>
+      <c r="O196" t="inlineStr"/>
+      <c r="P196" t="inlineStr"/>
+      <c r="Q196" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-20 18:41:04 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -12720,14 +12720,30 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M164" t="inlineStr"/>
-      <c r="N164" t="inlineStr"/>
-      <c r="O164" t="inlineStr"/>
-      <c r="P164" t="inlineStr"/>
-      <c r="Q164" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N164" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O164" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="P164" t="n">
+        <v>135</v>
+      </c>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>2025-09-20 04:25:46</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -12779,14 +12795,30 @@
       </c>
       <c r="L165" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M165" t="inlineStr"/>
-      <c r="N165" t="inlineStr"/>
-      <c r="O165" t="inlineStr"/>
-      <c r="P165" t="inlineStr"/>
-      <c r="Q165" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N165" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O165" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="P165" t="n">
+        <v>73</v>
+      </c>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>2025-09-20 04:25:46</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -12838,14 +12870,30 @@
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M166" t="inlineStr"/>
-      <c r="N166" t="inlineStr"/>
-      <c r="O166" t="inlineStr"/>
-      <c r="P166" t="inlineStr"/>
-      <c r="Q166" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N166" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O166" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="P166" t="n">
+        <v>73</v>
+      </c>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>2025-09-20 04:25:46</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -12897,14 +12945,30 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M167" t="inlineStr"/>
-      <c r="N167" t="inlineStr"/>
-      <c r="O167" t="inlineStr"/>
-      <c r="P167" t="inlineStr"/>
-      <c r="Q167" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N167" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O167" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P167" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>2025-09-20 04:25:46</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -12956,14 +13020,30 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M168" t="inlineStr"/>
-      <c r="N168" t="inlineStr"/>
-      <c r="O168" t="inlineStr"/>
-      <c r="P168" t="inlineStr"/>
-      <c r="Q168" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O168" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="P168" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>2025-09-20 04:25:46</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -13015,14 +13095,30 @@
       </c>
       <c r="L169" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M169" t="inlineStr"/>
-      <c r="N169" t="inlineStr"/>
-      <c r="O169" t="inlineStr"/>
-      <c r="P169" t="inlineStr"/>
-      <c r="Q169" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O169" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P169" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>2025-09-20 04:25:46</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-21 18:43:20 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -13170,14 +13170,30 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M170" t="inlineStr"/>
-      <c r="N170" t="inlineStr"/>
-      <c r="O170" t="inlineStr"/>
-      <c r="P170" t="inlineStr"/>
-      <c r="Q170" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O170" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="P170" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q170" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -13229,14 +13245,30 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M171" t="inlineStr"/>
-      <c r="N171" t="inlineStr"/>
-      <c r="O171" t="inlineStr"/>
-      <c r="P171" t="inlineStr"/>
-      <c r="Q171" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O171" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="P171" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q171" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -13288,14 +13320,30 @@
       </c>
       <c r="L172" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M172" t="inlineStr"/>
-      <c r="N172" t="inlineStr"/>
-      <c r="O172" t="inlineStr"/>
-      <c r="P172" t="inlineStr"/>
-      <c r="Q172" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O172" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P172" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q172" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -13347,14 +13395,30 @@
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M173" t="inlineStr"/>
-      <c r="N173" t="inlineStr"/>
-      <c r="O173" t="inlineStr"/>
-      <c r="P173" t="inlineStr"/>
-      <c r="Q173" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O173" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="P173" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q173" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -13406,14 +13470,30 @@
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M174" t="inlineStr"/>
-      <c r="N174" t="inlineStr"/>
-      <c r="O174" t="inlineStr"/>
-      <c r="P174" t="inlineStr"/>
-      <c r="Q174" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O174" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="P174" t="n">
+        <v>105</v>
+      </c>
+      <c r="Q174" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -13465,14 +13545,30 @@
       </c>
       <c r="L175" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M175" t="inlineStr"/>
-      <c r="N175" t="inlineStr"/>
-      <c r="O175" t="inlineStr"/>
-      <c r="P175" t="inlineStr"/>
-      <c r="Q175" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O175" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P175" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q175" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -13524,14 +13620,30 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M176" t="inlineStr"/>
-      <c r="N176" t="inlineStr"/>
-      <c r="O176" t="inlineStr"/>
-      <c r="P176" t="inlineStr"/>
-      <c r="Q176" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O176" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P176" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q176" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -13583,14 +13695,30 @@
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M177" t="inlineStr"/>
-      <c r="N177" t="inlineStr"/>
-      <c r="O177" t="inlineStr"/>
-      <c r="P177" t="inlineStr"/>
-      <c r="Q177" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N177" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O177" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="P177" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q177" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -13642,14 +13770,30 @@
       </c>
       <c r="L178" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M178" t="inlineStr"/>
-      <c r="N178" t="inlineStr"/>
-      <c r="O178" t="inlineStr"/>
-      <c r="P178" t="inlineStr"/>
-      <c r="Q178" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O178" t="n">
+        <v>-1.1</v>
+      </c>
+      <c r="P178" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q178" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -13701,14 +13845,30 @@
       </c>
       <c r="L179" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M179" t="inlineStr"/>
-      <c r="N179" t="inlineStr"/>
-      <c r="O179" t="inlineStr"/>
-      <c r="P179" t="inlineStr"/>
-      <c r="Q179" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N179" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O179" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="P179" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q179" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -13760,14 +13920,30 @@
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M180" t="inlineStr"/>
-      <c r="N180" t="inlineStr"/>
-      <c r="O180" t="inlineStr"/>
-      <c r="P180" t="inlineStr"/>
-      <c r="Q180" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N180" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O180" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P180" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q180" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -13819,14 +13995,30 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M181" t="inlineStr"/>
-      <c r="N181" t="inlineStr"/>
-      <c r="O181" t="inlineStr"/>
-      <c r="P181" t="inlineStr"/>
-      <c r="Q181" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O181" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="P181" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q181" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -13878,14 +14070,30 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M182" t="inlineStr"/>
-      <c r="N182" t="inlineStr"/>
-      <c r="O182" t="inlineStr"/>
-      <c r="P182" t="inlineStr"/>
-      <c r="Q182" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M182" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N182" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O182" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="P182" t="n">
+        <v>53</v>
+      </c>
+      <c r="Q182" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -13937,14 +14145,30 @@
       </c>
       <c r="L183" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M183" t="inlineStr"/>
-      <c r="N183" t="inlineStr"/>
-      <c r="O183" t="inlineStr"/>
-      <c r="P183" t="inlineStr"/>
-      <c r="Q183" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M183" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N183" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O183" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="P183" t="n">
+        <v>73</v>
+      </c>
+      <c r="Q183" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -13996,14 +14220,30 @@
       </c>
       <c r="L184" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M184" t="inlineStr"/>
-      <c r="N184" t="inlineStr"/>
-      <c r="O184" t="inlineStr"/>
-      <c r="P184" t="inlineStr"/>
-      <c r="Q184" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N184" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O184" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="P184" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q184" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -14055,14 +14295,30 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M185" t="inlineStr"/>
-      <c r="N185" t="inlineStr"/>
-      <c r="O185" t="inlineStr"/>
-      <c r="P185" t="inlineStr"/>
-      <c r="Q185" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N185" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O185" t="n">
+        <v>-2.1</v>
+      </c>
+      <c r="P185" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q185" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -14114,14 +14370,30 @@
       </c>
       <c r="L186" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M186" t="inlineStr"/>
-      <c r="N186" t="inlineStr"/>
-      <c r="O186" t="inlineStr"/>
-      <c r="P186" t="inlineStr"/>
-      <c r="Q186" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M186" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N186" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O186" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P186" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q186" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -14173,14 +14445,30 @@
       </c>
       <c r="L187" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M187" t="inlineStr"/>
-      <c r="N187" t="inlineStr"/>
-      <c r="O187" t="inlineStr"/>
-      <c r="P187" t="inlineStr"/>
-      <c r="Q187" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M187" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N187" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O187" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="P187" t="n">
+        <v>53</v>
+      </c>
+      <c r="Q187" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -14232,14 +14520,30 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M188" t="inlineStr"/>
-      <c r="N188" t="inlineStr"/>
-      <c r="O188" t="inlineStr"/>
-      <c r="P188" t="inlineStr"/>
-      <c r="Q188" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N188" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O188" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="P188" t="n">
+        <v>83</v>
+      </c>
+      <c r="Q188" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -14291,14 +14595,30 @@
       </c>
       <c r="L189" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M189" t="inlineStr"/>
-      <c r="N189" t="inlineStr"/>
-      <c r="O189" t="inlineStr"/>
-      <c r="P189" t="inlineStr"/>
-      <c r="Q189" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N189" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O189" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="P189" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q189" t="inlineStr">
+        <is>
+          <t>2025-09-21 04:26:29</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -14350,14 +14670,30 @@
       </c>
       <c r="L190" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M190" t="inlineStr"/>
-      <c r="N190" t="inlineStr"/>
-      <c r="O190" t="inlineStr"/>
-      <c r="P190" t="inlineStr"/>
-      <c r="Q190" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M190" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N190" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O190" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P190" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q190" t="inlineStr">
+        <is>
+          <t>2025-09-21 15:20:12</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -14409,14 +14745,30 @@
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M191" t="inlineStr"/>
-      <c r="N191" t="inlineStr"/>
-      <c r="O191" t="inlineStr"/>
-      <c r="P191" t="inlineStr"/>
-      <c r="Q191" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M191" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N191" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O191" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="P191" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q191" t="inlineStr">
+        <is>
+          <t>2025-09-21 15:20:12</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -14468,14 +14820,30 @@
       </c>
       <c r="L192" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M192" t="inlineStr"/>
-      <c r="N192" t="inlineStr"/>
-      <c r="O192" t="inlineStr"/>
-      <c r="P192" t="inlineStr"/>
-      <c r="Q192" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M192" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N192" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O192" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="P192" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q192" t="inlineStr">
+        <is>
+          <t>2025-09-21 15:20:12</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -14527,14 +14895,30 @@
       </c>
       <c r="L193" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M193" t="inlineStr"/>
-      <c r="N193" t="inlineStr"/>
-      <c r="O193" t="inlineStr"/>
-      <c r="P193" t="inlineStr"/>
-      <c r="Q193" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M193" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N193" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O193" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="P193" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q193" t="inlineStr">
+        <is>
+          <t>2025-09-21 15:20:12</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -14586,14 +14970,30 @@
       </c>
       <c r="L194" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M194" t="inlineStr"/>
-      <c r="N194" t="inlineStr"/>
-      <c r="O194" t="inlineStr"/>
-      <c r="P194" t="inlineStr"/>
-      <c r="Q194" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M194" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N194" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O194" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P194" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q194" t="inlineStr">
+        <is>
+          <t>2025-09-21 15:20:12</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -14645,14 +15045,30 @@
       </c>
       <c r="L195" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M195" t="inlineStr"/>
-      <c r="N195" t="inlineStr"/>
-      <c r="O195" t="inlineStr"/>
-      <c r="P195" t="inlineStr"/>
-      <c r="Q195" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M195" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N195" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O195" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="P195" t="n">
+        <v>130</v>
+      </c>
+      <c r="Q195" t="inlineStr">
+        <is>
+          <t>2025-09-21 15:20:12</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -14704,14 +15120,30 @@
       </c>
       <c r="L196" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M196" t="inlineStr"/>
-      <c r="N196" t="inlineStr"/>
-      <c r="O196" t="inlineStr"/>
-      <c r="P196" t="inlineStr"/>
-      <c r="Q196" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M196" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N196" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O196" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="P196" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q196" t="inlineStr">
+        <is>
+          <t>2025-09-21 15:20:12</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-09-22 18:45:55 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q196"/>
+  <dimension ref="A1:Q199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15145,6 +15145,183 @@
         </is>
       </c>
     </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Athletic Club</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Girona</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>87.31%</t>
+        </is>
+      </c>
+      <c r="G197" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>25.34%</t>
+        </is>
+      </c>
+      <c r="I197" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J197" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K197" t="n">
+        <v>0.5912082196903051</v>
+      </c>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M197" t="inlineStr"/>
+      <c r="N197" t="inlineStr"/>
+      <c r="O197" t="inlineStr"/>
+      <c r="P197" t="inlineStr"/>
+      <c r="Q197" t="inlineStr"/>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Anderlecht</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Gent</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>69.62%</t>
+        </is>
+      </c>
+      <c r="G198" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>24.06%</t>
+        </is>
+      </c>
+      <c r="I198" t="n">
+        <v>2</v>
+      </c>
+      <c r="J198" t="n">
+        <v>0.03163538932465376</v>
+      </c>
+      <c r="K198" t="n">
+        <v>0.3163538932465376</v>
+      </c>
+      <c r="L198" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M198" t="inlineStr"/>
+      <c r="N198" t="inlineStr"/>
+      <c r="O198" t="inlineStr"/>
+      <c r="P198" t="inlineStr"/>
+      <c r="Q198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>49.72%</t>
+        </is>
+      </c>
+      <c r="G199" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>10.74%</t>
+        </is>
+      </c>
+      <c r="I199" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J199" t="n">
+        <v>0.009488641199056218</v>
+      </c>
+      <c r="K199" t="n">
+        <v>0.09488641199056218</v>
+      </c>
+      <c r="L199" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M199" t="inlineStr"/>
+      <c r="N199" t="inlineStr"/>
+      <c r="O199" t="inlineStr"/>
+      <c r="P199" t="inlineStr"/>
+      <c r="Q199" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-01 18:47:09 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q199"/>
+  <dimension ref="A1:Q212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15195,14 +15195,30 @@
       </c>
       <c r="L197" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M197" t="inlineStr"/>
-      <c r="N197" t="inlineStr"/>
-      <c r="O197" t="inlineStr"/>
-      <c r="P197" t="inlineStr"/>
-      <c r="Q197" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M197" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N197" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O197" t="n">
+        <v>-3.2</v>
+      </c>
+      <c r="P197" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q197" t="inlineStr">
+        <is>
+          <t>2025-10-01 04:26:50</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -15254,14 +15270,30 @@
       </c>
       <c r="L198" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M198" t="inlineStr"/>
-      <c r="N198" t="inlineStr"/>
-      <c r="O198" t="inlineStr"/>
-      <c r="P198" t="inlineStr"/>
-      <c r="Q198" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M198" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N198" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O198" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="P198" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q198" t="inlineStr">
+        <is>
+          <t>2025-10-01 04:26:50</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -15313,14 +15345,797 @@
       </c>
       <c r="L199" t="inlineStr">
         <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M199" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N199" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O199" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="P199" t="n">
+        <v>125</v>
+      </c>
+      <c r="Q199" t="inlineStr">
+        <is>
+          <t>2025-10-01 04:26:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Celtic</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>SC Braga</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>65.66%</t>
+        </is>
+      </c>
+      <c r="G200" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>24.15%</t>
+        </is>
+      </c>
+      <c r="I200" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J200" t="n">
+        <v>0.02791515253207479</v>
+      </c>
+      <c r="K200" t="n">
+        <v>0.2791515253207478</v>
+      </c>
+      <c r="L200" t="inlineStr">
+        <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="M199" t="inlineStr"/>
-      <c r="N199" t="inlineStr"/>
-      <c r="O199" t="inlineStr"/>
-      <c r="P199" t="inlineStr"/>
-      <c r="Q199" t="inlineStr"/>
+      <c r="M200" t="inlineStr"/>
+      <c r="N200" t="inlineStr"/>
+      <c r="O200" t="inlineStr"/>
+      <c r="P200" t="inlineStr"/>
+      <c r="Q200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Panathinaikos</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>GO Ahead Eagles</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>81.52%</t>
+        </is>
+      </c>
+      <c r="G201" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>26.70%</t>
+        </is>
+      </c>
+      <c r="I201" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J201" t="n">
+        <v>0.04909559739067899</v>
+      </c>
+      <c r="K201" t="n">
+        <v>0.4909559739067899</v>
+      </c>
+      <c r="L201" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M201" t="inlineStr"/>
+      <c r="N201" t="inlineStr"/>
+      <c r="O201" t="inlineStr"/>
+      <c r="P201" t="inlineStr"/>
+      <c r="Q201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Ludogorets</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Real Betis</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>70.52%</t>
+        </is>
+      </c>
+      <c r="G202" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>27.76%</t>
+        </is>
+      </c>
+      <c r="I202" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J202" t="n">
+        <v>0.03500238967882782</v>
+      </c>
+      <c r="K202" t="n">
+        <v>0.3500238967882781</v>
+      </c>
+      <c r="L202" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M202" t="inlineStr"/>
+      <c r="N202" t="inlineStr"/>
+      <c r="O202" t="inlineStr"/>
+      <c r="P202" t="inlineStr"/>
+      <c r="Q202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>SC Freiburg</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>66.01%</t>
+        </is>
+      </c>
+      <c r="G203" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>24.16%</t>
+        </is>
+      </c>
+      <c r="I203" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J203" t="n">
+        <v>0.02824007439207552</v>
+      </c>
+      <c r="K203" t="n">
+        <v>0.2824007439207552</v>
+      </c>
+      <c r="L203" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M203" t="inlineStr"/>
+      <c r="N203" t="inlineStr"/>
+      <c r="O203" t="inlineStr"/>
+      <c r="P203" t="inlineStr"/>
+      <c r="Q203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Fenerbahce</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>73.21%</t>
+        </is>
+      </c>
+      <c r="G204" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>25.39%</t>
+        </is>
+      </c>
+      <c r="I204" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J204" t="n">
+        <v>0.03651991158815074</v>
+      </c>
+      <c r="K204" t="n">
+        <v>0.3651991158815074</v>
+      </c>
+      <c r="L204" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M204" t="inlineStr"/>
+      <c r="N204" t="inlineStr"/>
+      <c r="O204" t="inlineStr"/>
+      <c r="P204" t="inlineStr"/>
+      <c r="Q204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Plzen</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Malmo FF</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>64.00%</t>
+        </is>
+      </c>
+      <c r="G205" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>23.56%</t>
+        </is>
+      </c>
+      <c r="I205" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J205" t="n">
+        <v>0.02610924401215796</v>
+      </c>
+      <c r="K205" t="n">
+        <v>0.2610924401215796</v>
+      </c>
+      <c r="L205" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M205" t="inlineStr"/>
+      <c r="N205" t="inlineStr"/>
+      <c r="O205" t="inlineStr"/>
+      <c r="P205" t="inlineStr"/>
+      <c r="Q205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>AS Roma</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Lille</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>74.97%</t>
+        </is>
+      </c>
+      <c r="G206" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>26.18%</t>
+        </is>
+      </c>
+      <c r="I206" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J206" t="n">
+        <v>0.03922194584395017</v>
+      </c>
+      <c r="K206" t="n">
+        <v>0.3922194584395016</v>
+      </c>
+      <c r="L206" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M206" t="inlineStr"/>
+      <c r="N206" t="inlineStr"/>
+      <c r="O206" t="inlineStr"/>
+      <c r="P206" t="inlineStr"/>
+      <c r="Q206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>FC Basel 1893</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>VfB Stuttgart</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>67.10%</t>
+        </is>
+      </c>
+      <c r="G207" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>21.57%</t>
+        </is>
+      </c>
+      <c r="I207" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J207" t="n">
+        <v>0.0274689875466225</v>
+      </c>
+      <c r="K207" t="n">
+        <v>0.274689875466225</v>
+      </c>
+      <c r="L207" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M207" t="inlineStr"/>
+      <c r="N207" t="inlineStr"/>
+      <c r="O207" t="inlineStr"/>
+      <c r="P207" t="inlineStr"/>
+      <c r="Q207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Genk</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Ferencvarosi TC</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>76.61%</t>
+        </is>
+      </c>
+      <c r="G208" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>28.94%</t>
+        </is>
+      </c>
+      <c r="I208" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J208" t="n">
+        <v>0.04319713003957059</v>
+      </c>
+      <c r="K208" t="n">
+        <v>0.4319713003957059</v>
+      </c>
+      <c r="L208" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M208" t="inlineStr"/>
+      <c r="N208" t="inlineStr"/>
+      <c r="O208" t="inlineStr"/>
+      <c r="P208" t="inlineStr"/>
+      <c r="Q208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Lyon</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Red Bull Salzburg</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>83.41%</t>
+        </is>
+      </c>
+      <c r="G209" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>27.99%</t>
+        </is>
+      </c>
+      <c r="I209" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J209" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K209" t="n">
+        <v>0.5323940662311937</v>
+      </c>
+      <c r="L209" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M209" t="inlineStr"/>
+      <c r="N209" t="inlineStr"/>
+      <c r="O209" t="inlineStr"/>
+      <c r="P209" t="inlineStr"/>
+      <c r="Q209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>FC Porto</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>FK Crvena Zvezda</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>90.59%</t>
+        </is>
+      </c>
+      <c r="G210" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>25.56%</t>
+        </is>
+      </c>
+      <c r="I210" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J210" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K210" t="n">
+        <v>0.6706630702058514</v>
+      </c>
+      <c r="L210" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M210" t="inlineStr"/>
+      <c r="N210" t="inlineStr"/>
+      <c r="O210" t="inlineStr"/>
+      <c r="P210" t="inlineStr"/>
+      <c r="Q210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Nottingham Forest</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>FC Midtjylland</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>87.44%</t>
+        </is>
+      </c>
+      <c r="G211" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>28.12%</t>
+        </is>
+      </c>
+      <c r="I211" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J211" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K211" t="n">
+        <v>0.6128013083179003</v>
+      </c>
+      <c r="L211" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M211" t="inlineStr"/>
+      <c r="N211" t="inlineStr"/>
+      <c r="O211" t="inlineStr"/>
+      <c r="P211" t="inlineStr"/>
+      <c r="Q211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>UEFA Europa League</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Celta Vigo</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>PAOK</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>73.63%</t>
+        </is>
+      </c>
+      <c r="G212" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>26.11%</t>
+        </is>
+      </c>
+      <c r="I212" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J212" t="n">
+        <v>0.0375062794028851</v>
+      </c>
+      <c r="K212" t="n">
+        <v>0.375062794028851</v>
+      </c>
+      <c r="L212" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M212" t="inlineStr"/>
+      <c r="N212" t="inlineStr"/>
+      <c r="O212" t="inlineStr"/>
+      <c r="P212" t="inlineStr"/>
+      <c r="Q212" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-02 18:44:36 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q212"/>
+  <dimension ref="A1:Q219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16137,6 +16137,419 @@
       <c r="P212" t="inlineStr"/>
       <c r="Q212" t="inlineStr"/>
     </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Trabzonspor</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Kayserispor</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>85.01%</t>
+        </is>
+      </c>
+      <c r="G213" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>26.24%</t>
+        </is>
+      </c>
+      <c r="I213" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="J213" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K213" t="n">
+        <v>0.5502407679019199</v>
+      </c>
+      <c r="L213" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M213" t="inlineStr"/>
+      <c r="N213" t="inlineStr"/>
+      <c r="O213" t="inlineStr"/>
+      <c r="P213" t="inlineStr"/>
+      <c r="Q213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>1899 Hoffenheim</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>1.FC Köln</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>65.09%</t>
+        </is>
+      </c>
+      <c r="G214" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>22.43%</t>
+        </is>
+      </c>
+      <c r="I214" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J214" t="n">
+        <v>0.02629742390973933</v>
+      </c>
+      <c r="K214" t="n">
+        <v>0.2629742390973933</v>
+      </c>
+      <c r="L214" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M214" t="inlineStr"/>
+      <c r="N214" t="inlineStr"/>
+      <c r="O214" t="inlineStr"/>
+      <c r="P214" t="inlineStr"/>
+      <c r="Q214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Gent</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Charleroi</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>57.63%</t>
+        </is>
+      </c>
+      <c r="G215" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>16.96%</t>
+        </is>
+      </c>
+      <c r="I215" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J215" t="n">
+        <v>0.01727445339087996</v>
+      </c>
+      <c r="K215" t="n">
+        <v>0.1727445339087995</v>
+      </c>
+      <c r="L215" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M215" t="inlineStr"/>
+      <c r="N215" t="inlineStr"/>
+      <c r="O215" t="inlineStr"/>
+      <c r="P215" t="inlineStr"/>
+      <c r="Q215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Paris FC</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Lorient</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>70.16%</t>
+        </is>
+      </c>
+      <c r="G216" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>27.11%</t>
+        </is>
+      </c>
+      <c r="I216" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J216" t="n">
+        <v>0.03420866828729644</v>
+      </c>
+      <c r="K216" t="n">
+        <v>0.3420866828729644</v>
+      </c>
+      <c r="L216" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M216" t="inlineStr"/>
+      <c r="N216" t="inlineStr"/>
+      <c r="O216" t="inlineStr"/>
+      <c r="P216" t="inlineStr"/>
+      <c r="Q216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>68.87%</t>
+        </is>
+      </c>
+      <c r="G217" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>26.13%</t>
+        </is>
+      </c>
+      <c r="I217" t="n">
+        <v>2</v>
+      </c>
+      <c r="J217" t="n">
+        <v>0.03223787987903293</v>
+      </c>
+      <c r="K217" t="n">
+        <v>0.3223787987903293</v>
+      </c>
+      <c r="L217" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M217" t="inlineStr"/>
+      <c r="N217" t="inlineStr"/>
+      <c r="O217" t="inlineStr"/>
+      <c r="P217" t="inlineStr"/>
+      <c r="Q217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Osasuna</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Getafe</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>52.29%</t>
+        </is>
+      </c>
+      <c r="G218" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>13.90%</t>
+        </is>
+      </c>
+      <c r="I218" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J218" t="n">
+        <v>0.01253911440951226</v>
+      </c>
+      <c r="K218" t="n">
+        <v>0.1253911440951226</v>
+      </c>
+      <c r="L218" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M218" t="inlineStr"/>
+      <c r="N218" t="inlineStr"/>
+      <c r="O218" t="inlineStr"/>
+      <c r="P218" t="inlineStr"/>
+      <c r="Q218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Tapatío</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Alebrijes de Oaxaca</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>79.54%</t>
+        </is>
+      </c>
+      <c r="G219" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>27.57%</t>
+        </is>
+      </c>
+      <c r="I219" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J219" t="n">
+        <v>0.04654222003881247</v>
+      </c>
+      <c r="K219" t="n">
+        <v>0.4654222003881247</v>
+      </c>
+      <c r="L219" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M219" t="inlineStr"/>
+      <c r="N219" t="inlineStr"/>
+      <c r="O219" t="inlineStr"/>
+      <c r="P219" t="inlineStr"/>
+      <c r="Q219" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-03 18:45:41 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q219"/>
+  <dimension ref="A1:Q248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15420,14 +15420,30 @@
       </c>
       <c r="L200" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M200" t="inlineStr"/>
-      <c r="N200" t="inlineStr"/>
-      <c r="O200" t="inlineStr"/>
-      <c r="P200" t="inlineStr"/>
-      <c r="Q200" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M200" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N200" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O200" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="P200" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q200" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -15479,14 +15495,30 @@
       </c>
       <c r="L201" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M201" t="inlineStr"/>
-      <c r="N201" t="inlineStr"/>
-      <c r="O201" t="inlineStr"/>
-      <c r="P201" t="inlineStr"/>
-      <c r="Q201" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M201" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N201" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O201" t="n">
+        <v>-3.1</v>
+      </c>
+      <c r="P201" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q201" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -15538,14 +15570,30 @@
       </c>
       <c r="L202" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M202" t="inlineStr"/>
-      <c r="N202" t="inlineStr"/>
-      <c r="O202" t="inlineStr"/>
-      <c r="P202" t="inlineStr"/>
-      <c r="Q202" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M202" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N202" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O202" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="P202" t="n">
+        <v>83</v>
+      </c>
+      <c r="Q202" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -15597,14 +15645,30 @@
       </c>
       <c r="L203" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M203" t="inlineStr"/>
-      <c r="N203" t="inlineStr"/>
-      <c r="O203" t="inlineStr"/>
-      <c r="P203" t="inlineStr"/>
-      <c r="Q203" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M203" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N203" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O203" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="P203" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q203" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -15656,14 +15720,30 @@
       </c>
       <c r="L204" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M204" t="inlineStr"/>
-      <c r="N204" t="inlineStr"/>
-      <c r="O204" t="inlineStr"/>
-      <c r="P204" t="inlineStr"/>
-      <c r="Q204" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M204" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N204" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O204" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="P204" t="n">
+        <v>73</v>
+      </c>
+      <c r="Q204" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -15715,14 +15795,30 @@
       </c>
       <c r="L205" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M205" t="inlineStr"/>
-      <c r="N205" t="inlineStr"/>
-      <c r="O205" t="inlineStr"/>
-      <c r="P205" t="inlineStr"/>
-      <c r="Q205" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M205" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N205" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O205" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="P205" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q205" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -15774,14 +15870,30 @@
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M206" t="inlineStr"/>
-      <c r="N206" t="inlineStr"/>
-      <c r="O206" t="inlineStr"/>
-      <c r="P206" t="inlineStr"/>
-      <c r="Q206" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M206" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N206" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O206" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="P206" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q206" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -15833,14 +15945,30 @@
       </c>
       <c r="L207" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M207" t="inlineStr"/>
-      <c r="N207" t="inlineStr"/>
-      <c r="O207" t="inlineStr"/>
-      <c r="P207" t="inlineStr"/>
-      <c r="Q207" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M207" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N207" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O207" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P207" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q207" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -15892,14 +16020,30 @@
       </c>
       <c r="L208" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M208" t="inlineStr"/>
-      <c r="N208" t="inlineStr"/>
-      <c r="O208" t="inlineStr"/>
-      <c r="P208" t="inlineStr"/>
-      <c r="Q208" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M208" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N208" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O208" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="P208" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q208" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -15951,14 +16095,30 @@
       </c>
       <c r="L209" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M209" t="inlineStr"/>
-      <c r="N209" t="inlineStr"/>
-      <c r="O209" t="inlineStr"/>
-      <c r="P209" t="inlineStr"/>
-      <c r="Q209" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M209" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N209" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O209" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="P209" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q209" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -16010,14 +16170,30 @@
       </c>
       <c r="L210" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M210" t="inlineStr"/>
-      <c r="N210" t="inlineStr"/>
-      <c r="O210" t="inlineStr"/>
-      <c r="P210" t="inlineStr"/>
-      <c r="Q210" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M210" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N210" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O210" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="P210" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q210" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -16069,14 +16245,30 @@
       </c>
       <c r="L211" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M211" t="inlineStr"/>
-      <c r="N211" t="inlineStr"/>
-      <c r="O211" t="inlineStr"/>
-      <c r="P211" t="inlineStr"/>
-      <c r="Q211" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M211" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N211" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O211" t="n">
+        <v>-3.2</v>
+      </c>
+      <c r="P211" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q211" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -16128,14 +16320,30 @@
       </c>
       <c r="L212" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M212" t="inlineStr"/>
-      <c r="N212" t="inlineStr"/>
-      <c r="O212" t="inlineStr"/>
-      <c r="P212" t="inlineStr"/>
-      <c r="Q212" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M212" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N212" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O212" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="P212" t="n">
+        <v>73</v>
+      </c>
+      <c r="Q212" t="inlineStr">
+        <is>
+          <t>2025-10-03 04:26:15</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -16550,6 +16758,1717 @@
       <c r="P219" t="inlineStr"/>
       <c r="Q219" t="inlineStr"/>
     </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Tepatitlán</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Monarcas</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>61.05%</t>
+        </is>
+      </c>
+      <c r="G220" t="n">
+        <v>2</v>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>20.89%</t>
+        </is>
+      </c>
+      <c r="I220" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J220" t="n">
+        <v>0.0221066358449753</v>
+      </c>
+      <c r="K220" t="n">
+        <v>0.221066358449753</v>
+      </c>
+      <c r="L220" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M220" t="inlineStr"/>
+      <c r="N220" t="inlineStr"/>
+      <c r="O220" t="inlineStr"/>
+      <c r="P220" t="inlineStr"/>
+      <c r="Q220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Irapuato</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Correcaminos Uat</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>80.04%</t>
+        </is>
+      </c>
+      <c r="G221" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>24.41%</t>
+        </is>
+      </c>
+      <c r="I221" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J221" t="n">
+        <v>0.04503244837959176</v>
+      </c>
+      <c r="K221" t="n">
+        <v>0.4503244837959176</v>
+      </c>
+      <c r="L221" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M221" t="inlineStr"/>
+      <c r="N221" t="inlineStr"/>
+      <c r="O221" t="inlineStr"/>
+      <c r="P221" t="inlineStr"/>
+      <c r="Q221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>CA La Paz</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Cancún</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>49.35%</t>
+        </is>
+      </c>
+      <c r="G222" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>5.04%</t>
+        </is>
+      </c>
+      <c r="I222" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J222" t="n">
+        <v>0.005306031055924832</v>
+      </c>
+      <c r="K222" t="n">
+        <v>0.05306031055924831</v>
+      </c>
+      <c r="L222" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M222" t="inlineStr"/>
+      <c r="N222" t="inlineStr"/>
+      <c r="O222" t="inlineStr"/>
+      <c r="P222" t="inlineStr"/>
+      <c r="Q222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Genclerbirligi</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Alanyaspor</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>47.63%</t>
+        </is>
+      </c>
+      <c r="G223" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>8.45%</t>
+        </is>
+      </c>
+      <c r="I223" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J223" t="n">
+        <v>0.007344927880400635</v>
+      </c>
+      <c r="K223" t="n">
+        <v>0.07344927880400635</v>
+      </c>
+      <c r="L223" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M223" t="inlineStr"/>
+      <c r="N223" t="inlineStr"/>
+      <c r="O223" t="inlineStr"/>
+      <c r="P223" t="inlineStr"/>
+      <c r="Q223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>74.05%</t>
+        </is>
+      </c>
+      <c r="G224" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>24.63%</t>
+        </is>
+      </c>
+      <c r="I224" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J224" t="n">
+        <v>0.03698735443962806</v>
+      </c>
+      <c r="K224" t="n">
+        <v>0.3698735443962806</v>
+      </c>
+      <c r="L224" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M224" t="inlineStr"/>
+      <c r="N224" t="inlineStr"/>
+      <c r="O224" t="inlineStr"/>
+      <c r="P224" t="inlineStr"/>
+      <c r="Q224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>68.31%</t>
+        </is>
+      </c>
+      <c r="G225" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>25.11%</t>
+        </is>
+      </c>
+      <c r="I225" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J225" t="n">
+        <v>0.03102291399080768</v>
+      </c>
+      <c r="K225" t="n">
+        <v>0.3102291399080768</v>
+      </c>
+      <c r="L225" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M225" t="inlineStr"/>
+      <c r="N225" t="inlineStr"/>
+      <c r="O225" t="inlineStr"/>
+      <c r="P225" t="inlineStr"/>
+      <c r="Q225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Bayer Leverkusen</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Union Berlin</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>75.77%</t>
+        </is>
+      </c>
+      <c r="G226" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>27.52%</t>
+        </is>
+      </c>
+      <c r="I226" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J226" t="n">
+        <v>0.04115853331348995</v>
+      </c>
+      <c r="K226" t="n">
+        <v>0.4115853331348994</v>
+      </c>
+      <c r="L226" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M226" t="inlineStr"/>
+      <c r="N226" t="inlineStr"/>
+      <c r="O226" t="inlineStr"/>
+      <c r="P226" t="inlineStr"/>
+      <c r="Q226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Borussia Dortmund</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>76.20%</t>
+        </is>
+      </c>
+      <c r="G227" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>28.24%</t>
+        </is>
+      </c>
+      <c r="I227" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J227" t="n">
+        <v>0.04219153317619669</v>
+      </c>
+      <c r="K227" t="n">
+        <v>0.4219153317619668</v>
+      </c>
+      <c r="L227" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M227" t="inlineStr"/>
+      <c r="N227" t="inlineStr"/>
+      <c r="O227" t="inlineStr"/>
+      <c r="P227" t="inlineStr"/>
+      <c r="Q227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Manchester United</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Sunderland</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>85.94%</t>
+        </is>
+      </c>
+      <c r="G228" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>27.63%</t>
+        </is>
+      </c>
+      <c r="I228" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J228" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K228" t="n">
+        <v>0.5783401156739442</v>
+      </c>
+      <c r="L228" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M228" t="inlineStr"/>
+      <c r="N228" t="inlineStr"/>
+      <c r="O228" t="inlineStr"/>
+      <c r="P228" t="inlineStr"/>
+      <c r="Q228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>KV Mechelen</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>St. Truiden</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>51.87%</t>
+        </is>
+      </c>
+      <c r="G229" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>7.85%</t>
+        </is>
+      </c>
+      <c r="I229" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J229" t="n">
+        <v>0.008123692352551332</v>
+      </c>
+      <c r="K229" t="n">
+        <v>0.08123692352551332</v>
+      </c>
+      <c r="L229" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M229" t="inlineStr"/>
+      <c r="N229" t="inlineStr"/>
+      <c r="O229" t="inlineStr"/>
+      <c r="P229" t="inlineStr"/>
+      <c r="Q229" t="inlineStr"/>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Kocaelispor</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Eyüpspor</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>54.89%</t>
+        </is>
+      </c>
+      <c r="G230" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>16.83%</t>
+        </is>
+      </c>
+      <c r="I230" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J230" t="n">
+        <v>0.01566385563149848</v>
+      </c>
+      <c r="K230" t="n">
+        <v>0.1566385563149848</v>
+      </c>
+      <c r="L230" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M230" t="inlineStr"/>
+      <c r="N230" t="inlineStr"/>
+      <c r="O230" t="inlineStr"/>
+      <c r="P230" t="inlineStr"/>
+      <c r="Q230" t="inlineStr"/>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Sparta Rotterdam</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Ajax</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>72.39%</t>
+        </is>
+      </c>
+      <c r="G231" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>25.41%</t>
+        </is>
+      </c>
+      <c r="I231" t="n">
+        <v>2</v>
+      </c>
+      <c r="J231" t="n">
+        <v>0.03557134443545039</v>
+      </c>
+      <c r="K231" t="n">
+        <v>0.3557134443545039</v>
+      </c>
+      <c r="L231" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M231" t="inlineStr"/>
+      <c r="N231" t="inlineStr"/>
+      <c r="O231" t="inlineStr"/>
+      <c r="P231" t="inlineStr"/>
+      <c r="Q231" t="inlineStr"/>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>GIL Vicente</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Estrela</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>76.12%</t>
+        </is>
+      </c>
+      <c r="G232" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>24.34%</t>
+        </is>
+      </c>
+      <c r="I232" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J232" t="n">
+        <v>0.03937194839604734</v>
+      </c>
+      <c r="K232" t="n">
+        <v>0.3937194839604733</v>
+      </c>
+      <c r="L232" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M232" t="inlineStr"/>
+      <c r="N232" t="inlineStr"/>
+      <c r="O232" t="inlineStr"/>
+      <c r="P232" t="inlineStr"/>
+      <c r="Q232" t="inlineStr"/>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Metz</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Marseille</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>89.49%</t>
+        </is>
+      </c>
+      <c r="G233" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>28.46%</t>
+        </is>
+      </c>
+      <c r="I233" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J233" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K233" t="n">
+        <v>0.6613321679554292</v>
+      </c>
+      <c r="L233" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M233" t="inlineStr"/>
+      <c r="N233" t="inlineStr"/>
+      <c r="O233" t="inlineStr"/>
+      <c r="P233" t="inlineStr"/>
+      <c r="Q233" t="inlineStr"/>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Eintracht Frankfurt</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Bayern München</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>90.80%</t>
+        </is>
+      </c>
+      <c r="G234" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>27.64%</t>
+        </is>
+      </c>
+      <c r="I234" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J234" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K234" t="n">
+        <v>0.6888053477164349</v>
+      </c>
+      <c r="L234" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M234" t="inlineStr"/>
+      <c r="N234" t="inlineStr"/>
+      <c r="O234" t="inlineStr"/>
+      <c r="P234" t="inlineStr"/>
+      <c r="Q234" t="inlineStr"/>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Athletic Club</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>82.49%</t>
+        </is>
+      </c>
+      <c r="G235" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>24.95%</t>
+        </is>
+      </c>
+      <c r="I235" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J235" t="n">
+        <v>0.04945013951384732</v>
+      </c>
+      <c r="K235" t="n">
+        <v>0.4945013951384732</v>
+      </c>
+      <c r="L235" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M235" t="inlineStr"/>
+      <c r="N235" t="inlineStr"/>
+      <c r="O235" t="inlineStr"/>
+      <c r="P235" t="inlineStr"/>
+      <c r="Q235" t="inlineStr"/>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Fortuna Sittard</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>FC Volendam</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>68.27%</t>
+        </is>
+      </c>
+      <c r="G236" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>25.03%</t>
+        </is>
+      </c>
+      <c r="I236" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J236" t="n">
+        <v>0.03093574139949624</v>
+      </c>
+      <c r="K236" t="n">
+        <v>0.3093574139949624</v>
+      </c>
+      <c r="L236" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M236" t="inlineStr"/>
+      <c r="N236" t="inlineStr"/>
+      <c r="O236" t="inlineStr"/>
+      <c r="P236" t="inlineStr"/>
+      <c r="Q236" t="inlineStr"/>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Stade Brestois 29</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Nantes</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>68.40%</t>
+        </is>
+      </c>
+      <c r="G237" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>25.27%</t>
+        </is>
+      </c>
+      <c r="I237" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J237" t="n">
+        <v>0.0312141166391008</v>
+      </c>
+      <c r="K237" t="n">
+        <v>0.312141166391008</v>
+      </c>
+      <c r="L237" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M237" t="inlineStr"/>
+      <c r="N237" t="inlineStr"/>
+      <c r="O237" t="inlineStr"/>
+      <c r="P237" t="inlineStr"/>
+      <c r="Q237" t="inlineStr"/>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Galatasaray</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Besiktas</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>80.75%</t>
+        </is>
+      </c>
+      <c r="G238" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>27.91%</t>
+        </is>
+      </c>
+      <c r="I238" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J238" t="n">
+        <v>0.04867124949005033</v>
+      </c>
+      <c r="K238" t="n">
+        <v>0.4867124949005033</v>
+      </c>
+      <c r="L238" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M238" t="inlineStr"/>
+      <c r="N238" t="inlineStr"/>
+      <c r="O238" t="inlineStr"/>
+      <c r="P238" t="inlineStr"/>
+      <c r="Q238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>PEC Zwolle</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>PSV Eindhoven</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>91.89%</t>
+        </is>
+      </c>
+      <c r="G239" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>27.36%</t>
+        </is>
+      </c>
+      <c r="I239" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J239" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K239" t="n">
+        <v>0.7161301380564049</v>
+      </c>
+      <c r="L239" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M239" t="inlineStr"/>
+      <c r="N239" t="inlineStr"/>
+      <c r="O239" t="inlineStr"/>
+      <c r="P239" t="inlineStr"/>
+      <c r="Q239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>CF Montreal</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Nashville SC</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>61.38%</t>
+        </is>
+      </c>
+      <c r="G240" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>18.50%</t>
+        </is>
+      </c>
+      <c r="I240" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J240" t="n">
+        <v>0.02072937060961989</v>
+      </c>
+      <c r="K240" t="n">
+        <v>0.2072937060961989</v>
+      </c>
+      <c r="L240" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M240" t="inlineStr"/>
+      <c r="N240" t="inlineStr"/>
+      <c r="O240" t="inlineStr"/>
+      <c r="P240" t="inlineStr"/>
+      <c r="Q240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>53.17%</t>
+        </is>
+      </c>
+      <c r="G241" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>15.79%</t>
+        </is>
+      </c>
+      <c r="I241" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J241" t="n">
+        <v>0.01413631738383686</v>
+      </c>
+      <c r="K241" t="n">
+        <v>0.1413631738383686</v>
+      </c>
+      <c r="L241" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M241" t="inlineStr"/>
+      <c r="N241" t="inlineStr"/>
+      <c r="O241" t="inlineStr"/>
+      <c r="P241" t="inlineStr"/>
+      <c r="Q241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Heerenveen</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Excelsior</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>80.48%</t>
+        </is>
+      </c>
+      <c r="G242" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>27.48%</t>
+        </is>
+      </c>
+      <c r="I242" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J242" t="n">
+        <v>0.04793940798154306</v>
+      </c>
+      <c r="K242" t="n">
+        <v>0.4793940798154305</v>
+      </c>
+      <c r="L242" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M242" t="inlineStr"/>
+      <c r="N242" t="inlineStr"/>
+      <c r="O242" t="inlineStr"/>
+      <c r="P242" t="inlineStr"/>
+      <c r="Q242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>88.17%</t>
+        </is>
+      </c>
+      <c r="G243" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>26.56%</t>
+        </is>
+      </c>
+      <c r="I243" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J243" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K243" t="n">
+        <v>0.618687584100581</v>
+      </c>
+      <c r="L243" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M243" t="inlineStr"/>
+      <c r="N243" t="inlineStr"/>
+      <c r="O243" t="inlineStr"/>
+      <c r="P243" t="inlineStr"/>
+      <c r="Q243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Auxerre</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Lens</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>62.45%</t>
+        </is>
+      </c>
+      <c r="G244" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>20.56%</t>
+        </is>
+      </c>
+      <c r="I244" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J244" t="n">
+        <v>0.02292031252075558</v>
+      </c>
+      <c r="K244" t="n">
+        <v>0.2292031252075557</v>
+      </c>
+      <c r="L244" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M244" t="inlineStr"/>
+      <c r="N244" t="inlineStr"/>
+      <c r="O244" t="inlineStr"/>
+      <c r="P244" t="inlineStr"/>
+      <c r="Q244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>FC Dallas</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Los Angeles Galaxy</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>73.07%</t>
+        </is>
+      </c>
+      <c r="G245" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>26.59%</t>
+        </is>
+      </c>
+      <c r="I245" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J245" t="n">
+        <v>0.03715350044779366</v>
+      </c>
+      <c r="K245" t="n">
+        <v>0.3715350044779366</v>
+      </c>
+      <c r="L245" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M245" t="inlineStr"/>
+      <c r="N245" t="inlineStr"/>
+      <c r="O245" t="inlineStr"/>
+      <c r="P245" t="inlineStr"/>
+      <c r="Q245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Inter Miami</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>New England Revolution</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>89.19%</t>
+        </is>
+      </c>
+      <c r="G246" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>25.39%</t>
+        </is>
+      </c>
+      <c r="I246" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J246" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K246" t="n">
+        <v>0.6346531140929691</v>
+      </c>
+      <c r="L246" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M246" t="inlineStr"/>
+      <c r="N246" t="inlineStr"/>
+      <c r="O246" t="inlineStr"/>
+      <c r="P246" t="inlineStr"/>
+      <c r="Q246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Orlando City SC</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Columbus Crew</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>63.63%</t>
+        </is>
+      </c>
+      <c r="G247" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>22.84%</t>
+        </is>
+      </c>
+      <c r="I247" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J247" t="n">
+        <v>0.02535333651174848</v>
+      </c>
+      <c r="K247" t="n">
+        <v>0.2535333651174848</v>
+      </c>
+      <c r="L247" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M247" t="inlineStr"/>
+      <c r="N247" t="inlineStr"/>
+      <c r="O247" t="inlineStr"/>
+      <c r="P247" t="inlineStr"/>
+      <c r="Q247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Philadelphia Union</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>New York City FC</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>67.34%</t>
+        </is>
+      </c>
+      <c r="G248" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>26.66%</t>
+        </is>
+      </c>
+      <c r="I248" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J248" t="n">
+        <v>0.03104816648596754</v>
+      </c>
+      <c r="K248" t="n">
+        <v>0.3104816648596754</v>
+      </c>
+      <c r="L248" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M248" t="inlineStr"/>
+      <c r="N248" t="inlineStr"/>
+      <c r="O248" t="inlineStr"/>
+      <c r="P248" t="inlineStr"/>
+      <c r="Q248" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-04 18:42:49 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q248"/>
+  <dimension ref="A1:Q281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16395,14 +16395,30 @@
       </c>
       <c r="L213" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M213" t="inlineStr"/>
-      <c r="N213" t="inlineStr"/>
-      <c r="O213" t="inlineStr"/>
-      <c r="P213" t="inlineStr"/>
-      <c r="Q213" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M213" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N213" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O213" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="P213" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q213" t="inlineStr">
+        <is>
+          <t>2025-10-04 04:25:39</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -16454,14 +16470,30 @@
       </c>
       <c r="L214" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M214" t="inlineStr"/>
-      <c r="N214" t="inlineStr"/>
-      <c r="O214" t="inlineStr"/>
-      <c r="P214" t="inlineStr"/>
-      <c r="Q214" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M214" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N214" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O214" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P214" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q214" t="inlineStr">
+        <is>
+          <t>2025-10-04 04:25:39</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -16513,14 +16545,30 @@
       </c>
       <c r="L215" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M215" t="inlineStr"/>
-      <c r="N215" t="inlineStr"/>
-      <c r="O215" t="inlineStr"/>
-      <c r="P215" t="inlineStr"/>
-      <c r="Q215" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M215" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N215" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O215" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="P215" t="n">
+        <v>105</v>
+      </c>
+      <c r="Q215" t="inlineStr">
+        <is>
+          <t>2025-10-04 04:25:39</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -16572,14 +16620,30 @@
       </c>
       <c r="L216" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M216" t="inlineStr"/>
-      <c r="N216" t="inlineStr"/>
-      <c r="O216" t="inlineStr"/>
-      <c r="P216" t="inlineStr"/>
-      <c r="Q216" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M216" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N216" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O216" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="P216" t="n">
+        <v>83</v>
+      </c>
+      <c r="Q216" t="inlineStr">
+        <is>
+          <t>2025-10-04 04:25:39</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -16631,14 +16695,30 @@
       </c>
       <c r="L217" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M217" t="inlineStr"/>
-      <c r="N217" t="inlineStr"/>
-      <c r="O217" t="inlineStr"/>
-      <c r="P217" t="inlineStr"/>
-      <c r="Q217" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M217" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N217" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O217" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="P217" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q217" t="inlineStr">
+        <is>
+          <t>2025-10-04 04:25:39</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -16690,14 +16770,30 @@
       </c>
       <c r="L218" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M218" t="inlineStr"/>
-      <c r="N218" t="inlineStr"/>
-      <c r="O218" t="inlineStr"/>
-      <c r="P218" t="inlineStr"/>
-      <c r="Q218" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M218" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N218" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O218" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="P218" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q218" t="inlineStr">
+        <is>
+          <t>2025-10-04 04:25:39</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -16749,14 +16845,30 @@
       </c>
       <c r="L219" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M219" t="inlineStr"/>
-      <c r="N219" t="inlineStr"/>
-      <c r="O219" t="inlineStr"/>
-      <c r="P219" t="inlineStr"/>
-      <c r="Q219" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M219" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N219" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O219" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P219" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q219" t="inlineStr">
+        <is>
+          <t>2025-10-04 04:25:39</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -18469,6 +18581,1953 @@
       <c r="P248" t="inlineStr"/>
       <c r="Q248" t="inlineStr"/>
     </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Austin</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>St. Louis City</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>65.95%</t>
+        </is>
+      </c>
+      <c r="G249" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>24.70%</t>
+        </is>
+      </c>
+      <c r="I249" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J249" t="n">
+        <v>0.02852430635893474</v>
+      </c>
+      <c r="K249" t="n">
+        <v>0.2852430635893474</v>
+      </c>
+      <c r="L249" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M249" t="inlineStr"/>
+      <c r="N249" t="inlineStr"/>
+      <c r="O249" t="inlineStr"/>
+      <c r="P249" t="inlineStr"/>
+      <c r="Q249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Chicago Fire</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Toronto FC</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>85.28%</t>
+        </is>
+      </c>
+      <c r="G250" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>24.96%</t>
+        </is>
+      </c>
+      <c r="I250" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J250" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K250" t="n">
+        <v>0.5462027284969586</v>
+      </c>
+      <c r="L250" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M250" t="inlineStr"/>
+      <c r="N250" t="inlineStr"/>
+      <c r="O250" t="inlineStr"/>
+      <c r="P250" t="inlineStr"/>
+      <c r="Q250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Minnesota United FC</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Sporting Kansas City</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>86.21%</t>
+        </is>
+      </c>
+      <c r="G251" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>28.03%</t>
+        </is>
+      </c>
+      <c r="I251" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J251" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K251" t="n">
+        <v>0.5863997464200692</v>
+      </c>
+      <c r="L251" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M251" t="inlineStr"/>
+      <c r="N251" t="inlineStr"/>
+      <c r="O251" t="inlineStr"/>
+      <c r="P251" t="inlineStr"/>
+      <c r="Q251" t="inlineStr"/>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Leones Negros UDG</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Dorados</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>86.96%</t>
+        </is>
+      </c>
+      <c r="G252" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>24.83%</t>
+        </is>
+      </c>
+      <c r="I252" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J252" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K252" t="n">
+        <v>0.5796955674362929</v>
+      </c>
+      <c r="L252" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M252" t="inlineStr"/>
+      <c r="N252" t="inlineStr"/>
+      <c r="O252" t="inlineStr"/>
+      <c r="P252" t="inlineStr"/>
+      <c r="Q252" t="inlineStr"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Real Salt Lake</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Colorado Rapids</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>71.96%</t>
+        </is>
+      </c>
+      <c r="G253" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>28.23%</t>
+        </is>
+      </c>
+      <c r="I253" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J253" t="n">
+        <v>0.03690642620391769</v>
+      </c>
+      <c r="K253" t="n">
+        <v>0.3690642620391769</v>
+      </c>
+      <c r="L253" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M253" t="inlineStr"/>
+      <c r="N253" t="inlineStr"/>
+      <c r="O253" t="inlineStr"/>
+      <c r="P253" t="inlineStr"/>
+      <c r="Q253" t="inlineStr"/>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Seattle Sounders</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Portland Timbers</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>81.52%</t>
+        </is>
+      </c>
+      <c r="G254" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>26.70%</t>
+        </is>
+      </c>
+      <c r="I254" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J254" t="n">
+        <v>0.04909559739067899</v>
+      </c>
+      <c r="K254" t="n">
+        <v>0.4909559739067899</v>
+      </c>
+      <c r="L254" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M254" t="inlineStr"/>
+      <c r="N254" t="inlineStr"/>
+      <c r="O254" t="inlineStr"/>
+      <c r="P254" t="inlineStr"/>
+      <c r="Q254" t="inlineStr"/>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>55.10%</t>
+        </is>
+      </c>
+      <c r="G255" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>17.29%</t>
+        </is>
+      </c>
+      <c r="I255" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J255" t="n">
+        <v>0.01606474219962978</v>
+      </c>
+      <c r="K255" t="n">
+        <v>0.1606474219962978</v>
+      </c>
+      <c r="L255" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M255" t="inlineStr"/>
+      <c r="N255" t="inlineStr"/>
+      <c r="O255" t="inlineStr"/>
+      <c r="P255" t="inlineStr"/>
+      <c r="Q255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Anderlecht</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Standard Liege</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>78.08%</t>
+        </is>
+      </c>
+      <c r="G256" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>23.69%</t>
+        </is>
+      </c>
+      <c r="I256" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J256" t="n">
+        <v>0.04155934346461405</v>
+      </c>
+      <c r="K256" t="n">
+        <v>0.4155934346461405</v>
+      </c>
+      <c r="L256" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M256" t="inlineStr"/>
+      <c r="N256" t="inlineStr"/>
+      <c r="O256" t="inlineStr"/>
+      <c r="P256" t="inlineStr"/>
+      <c r="Q256" t="inlineStr"/>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Feyenoord</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Utrecht</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>85.32%</t>
+        </is>
+      </c>
+      <c r="G257" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>25.00%</t>
+        </is>
+      </c>
+      <c r="I257" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J257" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K257" t="n">
+        <v>0.5472348430558764</v>
+      </c>
+      <c r="L257" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M257" t="inlineStr"/>
+      <c r="N257" t="inlineStr"/>
+      <c r="O257" t="inlineStr"/>
+      <c r="P257" t="inlineStr"/>
+      <c r="Q257" t="inlineStr"/>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Pisa</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>76.50%</t>
+        </is>
+      </c>
+      <c r="G258" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>24.96%</t>
+        </is>
+      </c>
+      <c r="I258" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J258" t="n">
+        <v>0.04033849837514651</v>
+      </c>
+      <c r="K258" t="n">
+        <v>0.4033849837514651</v>
+      </c>
+      <c r="L258" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M258" t="inlineStr"/>
+      <c r="N258" t="inlineStr"/>
+      <c r="O258" t="inlineStr"/>
+      <c r="P258" t="inlineStr"/>
+      <c r="Q258" t="inlineStr"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>AS Roma</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>45.53%</t>
+        </is>
+      </c>
+      <c r="G259" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>7.29%</t>
+        </is>
+      </c>
+      <c r="I259" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J259" t="n">
+        <v>0.006065077104808627</v>
+      </c>
+      <c r="K259" t="n">
+        <v>0.06065077104808627</v>
+      </c>
+      <c r="L259" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M259" t="inlineStr"/>
+      <c r="N259" t="inlineStr"/>
+      <c r="O259" t="inlineStr"/>
+      <c r="P259" t="inlineStr"/>
+      <c r="Q259" t="inlineStr"/>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Aston Villa</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>80.02%</t>
+        </is>
+      </c>
+      <c r="G260" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>26.75%</t>
+        </is>
+      </c>
+      <c r="I260" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J260" t="n">
+        <v>0.04672023273814085</v>
+      </c>
+      <c r="K260" t="n">
+        <v>0.4672023273814085</v>
+      </c>
+      <c r="L260" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M260" t="inlineStr"/>
+      <c r="N260" t="inlineStr"/>
+      <c r="O260" t="inlineStr"/>
+      <c r="P260" t="inlineStr"/>
+      <c r="Q260" t="inlineStr"/>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Nottingham Forest</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>82.37%</t>
+        </is>
+      </c>
+      <c r="G261" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>26.40%</t>
+        </is>
+      </c>
+      <c r="I261" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J261" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K261" t="n">
+        <v>0.5031254641766906</v>
+      </c>
+      <c r="L261" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M261" t="inlineStr"/>
+      <c r="N261" t="inlineStr"/>
+      <c r="O261" t="inlineStr"/>
+      <c r="P261" t="inlineStr"/>
+      <c r="Q261" t="inlineStr"/>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Brighton</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>60.17%</t>
+        </is>
+      </c>
+      <c r="G262" t="n">
+        <v>2</v>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>19.13%</t>
+        </is>
+      </c>
+      <c r="I262" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J262" t="n">
+        <v>0.02033402148412829</v>
+      </c>
+      <c r="K262" t="n">
+        <v>0.2033402148412828</v>
+      </c>
+      <c r="L262" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M262" t="inlineStr"/>
+      <c r="N262" t="inlineStr"/>
+      <c r="O262" t="inlineStr"/>
+      <c r="P262" t="inlineStr"/>
+      <c r="Q262" t="inlineStr"/>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Lyon</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Toulouse</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>65.41%</t>
+        </is>
+      </c>
+      <c r="G263" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>23.68%</t>
+        </is>
+      </c>
+      <c r="I263" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J263" t="n">
+        <v>0.02739590042120696</v>
+      </c>
+      <c r="K263" t="n">
+        <v>0.2739590042120696</v>
+      </c>
+      <c r="L263" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M263" t="inlineStr"/>
+      <c r="N263" t="inlineStr"/>
+      <c r="O263" t="inlineStr"/>
+      <c r="P263" t="inlineStr"/>
+      <c r="Q263" t="inlineStr"/>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>VfB Stuttgart</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>1. FC Heidenheim</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>88.79%</t>
+        </is>
+      </c>
+      <c r="G264" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>24.82%</t>
+        </is>
+      </c>
+      <c r="I264" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J264" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K264" t="n">
+        <v>0.6210598392500283</v>
+      </c>
+      <c r="L264" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M264" t="inlineStr"/>
+      <c r="N264" t="inlineStr"/>
+      <c r="O264" t="inlineStr"/>
+      <c r="P264" t="inlineStr"/>
+      <c r="Q264" t="inlineStr"/>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>81.46%</t>
+        </is>
+      </c>
+      <c r="G265" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>29.04%</t>
+        </is>
+      </c>
+      <c r="I265" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J265" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K265" t="n">
+        <v>0.5056998787861097</v>
+      </c>
+      <c r="L265" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M265" t="inlineStr"/>
+      <c r="N265" t="inlineStr"/>
+      <c r="O265" t="inlineStr"/>
+      <c r="P265" t="inlineStr"/>
+      <c r="Q265" t="inlineStr"/>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Arouca</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Famalicao</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>55.38%</t>
+        </is>
+      </c>
+      <c r="G266" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>17.88%</t>
+        </is>
+      </c>
+      <c r="I266" t="n">
+        <v>1</v>
+      </c>
+      <c r="J266" t="n">
+        <v>0.01658135201814348</v>
+      </c>
+      <c r="K266" t="n">
+        <v>0.1658135201814348</v>
+      </c>
+      <c r="L266" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M266" t="inlineStr"/>
+      <c r="N266" t="inlineStr"/>
+      <c r="O266" t="inlineStr"/>
+      <c r="P266" t="inlineStr"/>
+      <c r="Q266" t="inlineStr"/>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Le Havre</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Rennes</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>44.81%</t>
+        </is>
+      </c>
+      <c r="G267" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>4.26%</t>
+        </is>
+      </c>
+      <c r="I267" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J267" t="n">
+        <v>0.003933473502998035</v>
+      </c>
+      <c r="K267" t="n">
+        <v>0.03933473502998034</v>
+      </c>
+      <c r="L267" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M267" t="inlineStr"/>
+      <c r="N267" t="inlineStr"/>
+      <c r="O267" t="inlineStr"/>
+      <c r="P267" t="inlineStr"/>
+      <c r="Q267" t="inlineStr"/>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>69.98%</t>
+        </is>
+      </c>
+      <c r="G268" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>26.78%</t>
+        </is>
+      </c>
+      <c r="I268" t="n">
+        <v>2</v>
+      </c>
+      <c r="J268" t="n">
+        <v>0.03380254945400395</v>
+      </c>
+      <c r="K268" t="n">
+        <v>0.3380254945400396</v>
+      </c>
+      <c r="L268" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M268" t="inlineStr"/>
+      <c r="N268" t="inlineStr"/>
+      <c r="O268" t="inlineStr"/>
+      <c r="P268" t="inlineStr"/>
+      <c r="Q268" t="inlineStr"/>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Strasbourg</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Angers</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>74.92%</t>
+        </is>
+      </c>
+      <c r="G269" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H269" t="inlineStr">
+        <is>
+          <t>26.08%</t>
+        </is>
+      </c>
+      <c r="I269" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J269" t="n">
+        <v>0.0390823403316318</v>
+      </c>
+      <c r="K269" t="n">
+        <v>0.390823403316318</v>
+      </c>
+      <c r="L269" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M269" t="inlineStr"/>
+      <c r="N269" t="inlineStr"/>
+      <c r="O269" t="inlineStr"/>
+      <c r="P269" t="inlineStr"/>
+      <c r="Q269" t="inlineStr"/>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>78.05%</t>
+        </is>
+      </c>
+      <c r="G270" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>27.49%</t>
+        </is>
+      </c>
+      <c r="I270" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J270" t="n">
+        <v>0.04427157557607664</v>
+      </c>
+      <c r="K270" t="n">
+        <v>0.4427157557607664</v>
+      </c>
+      <c r="L270" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M270" t="inlineStr"/>
+      <c r="N270" t="inlineStr"/>
+      <c r="O270" t="inlineStr"/>
+      <c r="P270" t="inlineStr"/>
+      <c r="Q270" t="inlineStr"/>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>87.46%</t>
+        </is>
+      </c>
+      <c r="G271" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>24.68%</t>
+        </is>
+      </c>
+      <c r="I271" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J271" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K271" t="n">
+        <v>0.5894866388658516</v>
+      </c>
+      <c r="L271" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M271" t="inlineStr"/>
+      <c r="N271" t="inlineStr"/>
+      <c r="O271" t="inlineStr"/>
+      <c r="P271" t="inlineStr"/>
+      <c r="Q271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>Club Brugge KV</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Union St. Gilloise</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>52.18%</t>
+        </is>
+      </c>
+      <c r="G272" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>11.06%</t>
+        </is>
+      </c>
+      <c r="I272" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J272" t="n">
+        <v>0.01059283753346811</v>
+      </c>
+      <c r="K272" t="n">
+        <v>0.1059283753346811</v>
+      </c>
+      <c r="L272" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M272" t="inlineStr"/>
+      <c r="N272" t="inlineStr"/>
+      <c r="O272" t="inlineStr"/>
+      <c r="P272" t="inlineStr"/>
+      <c r="Q272" t="inlineStr"/>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Rayo Vallecano</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>58.71%</t>
+        </is>
+      </c>
+      <c r="G273" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>19.15%</t>
+        </is>
+      </c>
+      <c r="I273" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J273" t="n">
+        <v>0.01938560028281509</v>
+      </c>
+      <c r="K273" t="n">
+        <v>0.1938560028281509</v>
+      </c>
+      <c r="L273" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M273" t="inlineStr"/>
+      <c r="N273" t="inlineStr"/>
+      <c r="O273" t="inlineStr"/>
+      <c r="P273" t="inlineStr"/>
+      <c r="Q273" t="inlineStr"/>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Goztepe</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Istanbul Basaksehir</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>70.72%</t>
+        </is>
+      </c>
+      <c r="G274" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>22.53%</t>
+        </is>
+      </c>
+      <c r="I274" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J274" t="n">
+        <v>0.03168569966640591</v>
+      </c>
+      <c r="K274" t="n">
+        <v>0.316856996664059</v>
+      </c>
+      <c r="L274" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M274" t="inlineStr"/>
+      <c r="N274" t="inlineStr"/>
+      <c r="O274" t="inlineStr"/>
+      <c r="P274" t="inlineStr"/>
+      <c r="Q274" t="inlineStr"/>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Samsunspor</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Fenerbahce</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>77.23%</t>
+        </is>
+      </c>
+      <c r="G275" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>23.86%</t>
+        </is>
+      </c>
+      <c r="I275" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J275" t="n">
+        <v>0.04049405374724598</v>
+      </c>
+      <c r="K275" t="n">
+        <v>0.4049405374724597</v>
+      </c>
+      <c r="L275" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M275" t="inlineStr"/>
+      <c r="N275" t="inlineStr"/>
+      <c r="O275" t="inlineStr"/>
+      <c r="P275" t="inlineStr"/>
+      <c r="Q275" t="inlineStr"/>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>KVC Westerlo</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>OH Leuven</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>67.12%</t>
+        </is>
+      </c>
+      <c r="G276" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>22.92%</t>
+        </is>
+      </c>
+      <c r="I276" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J276" t="n">
+        <v>0.02842739545499423</v>
+      </c>
+      <c r="K276" t="n">
+        <v>0.2842739545499423</v>
+      </c>
+      <c r="L276" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M276" t="inlineStr"/>
+      <c r="N276" t="inlineStr"/>
+      <c r="O276" t="inlineStr"/>
+      <c r="P276" t="inlineStr"/>
+      <c r="Q276" t="inlineStr"/>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Sporting CP</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>SC Braga</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>86.63%</t>
+        </is>
+      </c>
+      <c r="G277" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>23.50%</t>
+        </is>
+      </c>
+      <c r="I277" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J277" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K277" t="n">
+        <v>0.5624007025882916</v>
+      </c>
+      <c r="L277" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M277" t="inlineStr"/>
+      <c r="N277" t="inlineStr"/>
+      <c r="O277" t="inlineStr"/>
+      <c r="P277" t="inlineStr"/>
+      <c r="Q277" t="inlineStr"/>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>Lille</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Paris Saint Germain</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>74.10%</t>
+        </is>
+      </c>
+      <c r="G278" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>28.38%</t>
+        </is>
+      </c>
+      <c r="I278" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J278" t="n">
+        <v>0.03957039603630205</v>
+      </c>
+      <c r="K278" t="n">
+        <v>0.3957039603630205</v>
+      </c>
+      <c r="L278" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M278" t="inlineStr"/>
+      <c r="N278" t="inlineStr"/>
+      <c r="O278" t="inlineStr"/>
+      <c r="P278" t="inlineStr"/>
+      <c r="Q278" t="inlineStr"/>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Celta Vigo</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>73.04%</t>
+        </is>
+      </c>
+      <c r="G279" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>26.55%</t>
+        </is>
+      </c>
+      <c r="I279" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J279" t="n">
+        <v>0.03710310147878624</v>
+      </c>
+      <c r="K279" t="n">
+        <v>0.3710310147878624</v>
+      </c>
+      <c r="L279" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M279" t="inlineStr"/>
+      <c r="N279" t="inlineStr"/>
+      <c r="O279" t="inlineStr"/>
+      <c r="P279" t="inlineStr"/>
+      <c r="Q279" t="inlineStr"/>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Primeira Liga</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>FC Porto</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Benfica</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>62.62%</t>
+        </is>
+      </c>
+      <c r="G280" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>20.89%</t>
+        </is>
+      </c>
+      <c r="I280" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J280" t="n">
+        <v>0.02327370309292166</v>
+      </c>
+      <c r="K280" t="n">
+        <v>0.2327370309292165</v>
+      </c>
+      <c r="L280" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M280" t="inlineStr"/>
+      <c r="N280" t="inlineStr"/>
+      <c r="O280" t="inlineStr"/>
+      <c r="P280" t="inlineStr"/>
+      <c r="Q280" t="inlineStr"/>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Vancouver Whitecaps</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>San Jose Earthquakes</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>80.20%</t>
+        </is>
+      </c>
+      <c r="G281" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>27.03%</t>
+        </is>
+      </c>
+      <c r="I281" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J281" t="n">
+        <v>0.04719396969126342</v>
+      </c>
+      <c r="K281" t="n">
+        <v>0.4719396969126342</v>
+      </c>
+      <c r="L281" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M281" t="inlineStr"/>
+      <c r="N281" t="inlineStr"/>
+      <c r="O281" t="inlineStr"/>
+      <c r="P281" t="inlineStr"/>
+      <c r="Q281" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-05 18:43:02 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q281"/>
+  <dimension ref="A1:Q282"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16920,14 +16920,30 @@
       </c>
       <c r="L220" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M220" t="inlineStr"/>
-      <c r="N220" t="inlineStr"/>
-      <c r="O220" t="inlineStr"/>
-      <c r="P220" t="inlineStr"/>
-      <c r="Q220" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M220" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N220" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O220" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="P220" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q220" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -16979,14 +16995,30 @@
       </c>
       <c r="L221" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M221" t="inlineStr"/>
-      <c r="N221" t="inlineStr"/>
-      <c r="O221" t="inlineStr"/>
-      <c r="P221" t="inlineStr"/>
-      <c r="Q221" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M221" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N221" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O221" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="P221" t="n">
+        <v>57</v>
+      </c>
+      <c r="Q221" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -17038,14 +17070,30 @@
       </c>
       <c r="L222" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M222" t="inlineStr"/>
-      <c r="N222" t="inlineStr"/>
-      <c r="O222" t="inlineStr"/>
-      <c r="P222" t="inlineStr"/>
-      <c r="Q222" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M222" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N222" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O222" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="P222" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q222" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -17097,14 +17145,30 @@
       </c>
       <c r="L223" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M223" t="inlineStr"/>
-      <c r="N223" t="inlineStr"/>
-      <c r="O223" t="inlineStr"/>
-      <c r="P223" t="inlineStr"/>
-      <c r="Q223" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M223" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N223" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O223" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="P223" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q223" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -17156,14 +17220,30 @@
       </c>
       <c r="L224" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M224" t="inlineStr"/>
-      <c r="N224" t="inlineStr"/>
-      <c r="O224" t="inlineStr"/>
-      <c r="P224" t="inlineStr"/>
-      <c r="Q224" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M224" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N224" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O224" t="n">
+        <v>-2.1</v>
+      </c>
+      <c r="P224" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q224" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -17215,14 +17295,30 @@
       </c>
       <c r="L225" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M225" t="inlineStr"/>
-      <c r="N225" t="inlineStr"/>
-      <c r="O225" t="inlineStr"/>
-      <c r="P225" t="inlineStr"/>
-      <c r="Q225" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M225" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N225" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O225" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P225" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q225" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -17274,14 +17370,30 @@
       </c>
       <c r="L226" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M226" t="inlineStr"/>
-      <c r="N226" t="inlineStr"/>
-      <c r="O226" t="inlineStr"/>
-      <c r="P226" t="inlineStr"/>
-      <c r="Q226" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M226" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N226" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O226" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="P226" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q226" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -17333,14 +17445,30 @@
       </c>
       <c r="L227" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M227" t="inlineStr"/>
-      <c r="N227" t="inlineStr"/>
-      <c r="O227" t="inlineStr"/>
-      <c r="P227" t="inlineStr"/>
-      <c r="Q227" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M227" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N227" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O227" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="P227" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q227" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -17392,14 +17520,30 @@
       </c>
       <c r="L228" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M228" t="inlineStr"/>
-      <c r="N228" t="inlineStr"/>
-      <c r="O228" t="inlineStr"/>
-      <c r="P228" t="inlineStr"/>
-      <c r="Q228" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M228" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N228" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O228" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P228" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q228" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -17451,14 +17595,30 @@
       </c>
       <c r="L229" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M229" t="inlineStr"/>
-      <c r="N229" t="inlineStr"/>
-      <c r="O229" t="inlineStr"/>
-      <c r="P229" t="inlineStr"/>
-      <c r="Q229" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M229" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N229" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O229" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="P229" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q229" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -17510,14 +17670,30 @@
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M230" t="inlineStr"/>
-      <c r="N230" t="inlineStr"/>
-      <c r="O230" t="inlineStr"/>
-      <c r="P230" t="inlineStr"/>
-      <c r="Q230" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M230" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N230" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O230" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="P230" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q230" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -17569,14 +17745,30 @@
       </c>
       <c r="L231" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M231" t="inlineStr"/>
-      <c r="N231" t="inlineStr"/>
-      <c r="O231" t="inlineStr"/>
-      <c r="P231" t="inlineStr"/>
-      <c r="Q231" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M231" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N231" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O231" t="n">
+        <v>-2</v>
+      </c>
+      <c r="P231" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q231" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -17628,14 +17820,30 @@
       </c>
       <c r="L232" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M232" t="inlineStr"/>
-      <c r="N232" t="inlineStr"/>
-      <c r="O232" t="inlineStr"/>
-      <c r="P232" t="inlineStr"/>
-      <c r="Q232" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M232" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N232" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O232" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="P232" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q232" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -17687,14 +17895,30 @@
       </c>
       <c r="L233" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M233" t="inlineStr"/>
-      <c r="N233" t="inlineStr"/>
-      <c r="O233" t="inlineStr"/>
-      <c r="P233" t="inlineStr"/>
-      <c r="Q233" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M233" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N233" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O233" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="P233" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q233" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -17746,14 +17970,30 @@
       </c>
       <c r="L234" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M234" t="inlineStr"/>
-      <c r="N234" t="inlineStr"/>
-      <c r="O234" t="inlineStr"/>
-      <c r="P234" t="inlineStr"/>
-      <c r="Q234" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M234" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N234" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O234" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="P234" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q234" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -17805,14 +18045,30 @@
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M235" t="inlineStr"/>
-      <c r="N235" t="inlineStr"/>
-      <c r="O235" t="inlineStr"/>
-      <c r="P235" t="inlineStr"/>
-      <c r="Q235" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M235" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N235" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O235" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="P235" t="n">
+        <v>53</v>
+      </c>
+      <c r="Q235" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -17864,14 +18120,30 @@
       </c>
       <c r="L236" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M236" t="inlineStr"/>
-      <c r="N236" t="inlineStr"/>
-      <c r="O236" t="inlineStr"/>
-      <c r="P236" t="inlineStr"/>
-      <c r="Q236" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M236" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N236" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O236" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="P236" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q236" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -17923,14 +18195,30 @@
       </c>
       <c r="L237" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M237" t="inlineStr"/>
-      <c r="N237" t="inlineStr"/>
-      <c r="O237" t="inlineStr"/>
-      <c r="P237" t="inlineStr"/>
-      <c r="Q237" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M237" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N237" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O237" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="P237" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q237" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -17982,14 +18270,30 @@
       </c>
       <c r="L238" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M238" t="inlineStr"/>
-      <c r="N238" t="inlineStr"/>
-      <c r="O238" t="inlineStr"/>
-      <c r="P238" t="inlineStr"/>
-      <c r="Q238" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M238" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N238" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O238" t="n">
+        <v>-2.7</v>
+      </c>
+      <c r="P238" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q238" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -18041,14 +18345,30 @@
       </c>
       <c r="L239" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M239" t="inlineStr"/>
-      <c r="N239" t="inlineStr"/>
-      <c r="O239" t="inlineStr"/>
-      <c r="P239" t="inlineStr"/>
-      <c r="Q239" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M239" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N239" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O239" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="P239" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q239" t="inlineStr">
+        <is>
+          <t>2025-10-05 04:25:11</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -18100,14 +18420,30 @@
       </c>
       <c r="L240" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M240" t="inlineStr"/>
-      <c r="N240" t="inlineStr"/>
-      <c r="O240" t="inlineStr"/>
-      <c r="P240" t="inlineStr"/>
-      <c r="Q240" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M240" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N240" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O240" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="P240" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q240" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -18159,14 +18495,30 @@
       </c>
       <c r="L241" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M241" t="inlineStr"/>
-      <c r="N241" t="inlineStr"/>
-      <c r="O241" t="inlineStr"/>
-      <c r="P241" t="inlineStr"/>
-      <c r="Q241" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M241" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N241" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O241" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="P241" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q241" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -18218,14 +18570,30 @@
       </c>
       <c r="L242" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M242" t="inlineStr"/>
-      <c r="N242" t="inlineStr"/>
-      <c r="O242" t="inlineStr"/>
-      <c r="P242" t="inlineStr"/>
-      <c r="Q242" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M242" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N242" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O242" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="P242" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q242" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -18277,14 +18645,30 @@
       </c>
       <c r="L243" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M243" t="inlineStr"/>
-      <c r="N243" t="inlineStr"/>
-      <c r="O243" t="inlineStr"/>
-      <c r="P243" t="inlineStr"/>
-      <c r="Q243" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M243" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N243" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O243" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="P243" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q243" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -18336,14 +18720,30 @@
       </c>
       <c r="L244" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M244" t="inlineStr"/>
-      <c r="N244" t="inlineStr"/>
-      <c r="O244" t="inlineStr"/>
-      <c r="P244" t="inlineStr"/>
-      <c r="Q244" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M244" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N244" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O244" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="P244" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q244" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -18395,14 +18795,30 @@
       </c>
       <c r="L245" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M245" t="inlineStr"/>
-      <c r="N245" t="inlineStr"/>
-      <c r="O245" t="inlineStr"/>
-      <c r="P245" t="inlineStr"/>
-      <c r="Q245" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M245" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N245" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O245" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="P245" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q245" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -18454,14 +18870,30 @@
       </c>
       <c r="L246" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M246" t="inlineStr"/>
-      <c r="N246" t="inlineStr"/>
-      <c r="O246" t="inlineStr"/>
-      <c r="P246" t="inlineStr"/>
-      <c r="Q246" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M246" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N246" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O246" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="P246" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q246" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -18513,14 +18945,30 @@
       </c>
       <c r="L247" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M247" t="inlineStr"/>
-      <c r="N247" t="inlineStr"/>
-      <c r="O247" t="inlineStr"/>
-      <c r="P247" t="inlineStr"/>
-      <c r="Q247" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M247" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N247" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O247" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="P247" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q247" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -18572,14 +19020,30 @@
       </c>
       <c r="L248" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M248" t="inlineStr"/>
-      <c r="N248" t="inlineStr"/>
-      <c r="O248" t="inlineStr"/>
-      <c r="P248" t="inlineStr"/>
-      <c r="Q248" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M248" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N248" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O248" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="P248" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q248" t="inlineStr">
+        <is>
+          <t>2025-10-05 15:19:34</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -20528,6 +20992,65 @@
       <c r="P281" t="inlineStr"/>
       <c r="Q281" t="inlineStr"/>
     </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Los Angeles FC</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Atlanta United FC</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>90.09%</t>
+        </is>
+      </c>
+      <c r="G282" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>24.87%</t>
+        </is>
+      </c>
+      <c r="I282" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J282" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K282" t="n">
+        <v>0.6533065723213444</v>
+      </c>
+      <c r="L282" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M282" t="inlineStr"/>
+      <c r="N282" t="inlineStr"/>
+      <c r="O282" t="inlineStr"/>
+      <c r="P282" t="inlineStr"/>
+      <c r="Q282" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-06 18:47:48 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -19095,14 +19095,30 @@
       </c>
       <c r="L249" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M249" t="inlineStr"/>
-      <c r="N249" t="inlineStr"/>
-      <c r="O249" t="inlineStr"/>
-      <c r="P249" t="inlineStr"/>
-      <c r="Q249" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M249" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N249" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O249" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P249" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q249" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -19154,14 +19170,30 @@
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M250" t="inlineStr"/>
-      <c r="N250" t="inlineStr"/>
-      <c r="O250" t="inlineStr"/>
-      <c r="P250" t="inlineStr"/>
-      <c r="Q250" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M250" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N250" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O250" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P250" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q250" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -19213,14 +19245,30 @@
       </c>
       <c r="L251" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M251" t="inlineStr"/>
-      <c r="N251" t="inlineStr"/>
-      <c r="O251" t="inlineStr"/>
-      <c r="P251" t="inlineStr"/>
-      <c r="Q251" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M251" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N251" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O251" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="P251" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q251" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -19272,14 +19320,30 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M252" t="inlineStr"/>
-      <c r="N252" t="inlineStr"/>
-      <c r="O252" t="inlineStr"/>
-      <c r="P252" t="inlineStr"/>
-      <c r="Q252" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M252" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N252" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O252" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P252" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q252" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -19331,14 +19395,30 @@
       </c>
       <c r="L253" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M253" t="inlineStr"/>
-      <c r="N253" t="inlineStr"/>
-      <c r="O253" t="inlineStr"/>
-      <c r="P253" t="inlineStr"/>
-      <c r="Q253" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M253" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N253" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O253" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="P253" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q253" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -19390,14 +19470,30 @@
       </c>
       <c r="L254" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M254" t="inlineStr"/>
-      <c r="N254" t="inlineStr"/>
-      <c r="O254" t="inlineStr"/>
-      <c r="P254" t="inlineStr"/>
-      <c r="Q254" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M254" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N254" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O254" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="P254" t="n">
+        <v>57</v>
+      </c>
+      <c r="Q254" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -19449,14 +19545,30 @@
       </c>
       <c r="L255" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M255" t="inlineStr"/>
-      <c r="N255" t="inlineStr"/>
-      <c r="O255" t="inlineStr"/>
-      <c r="P255" t="inlineStr"/>
-      <c r="Q255" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M255" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N255" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O255" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P255" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q255" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -19508,14 +19620,30 @@
       </c>
       <c r="L256" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M256" t="inlineStr"/>
-      <c r="N256" t="inlineStr"/>
-      <c r="O256" t="inlineStr"/>
-      <c r="P256" t="inlineStr"/>
-      <c r="Q256" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M256" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N256" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O256" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="P256" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q256" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -19567,14 +19695,30 @@
       </c>
       <c r="L257" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M257" t="inlineStr"/>
-      <c r="N257" t="inlineStr"/>
-      <c r="O257" t="inlineStr"/>
-      <c r="P257" t="inlineStr"/>
-      <c r="Q257" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M257" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N257" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O257" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="P257" t="n">
+        <v>48</v>
+      </c>
+      <c r="Q257" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -19626,14 +19770,30 @@
       </c>
       <c r="L258" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M258" t="inlineStr"/>
-      <c r="N258" t="inlineStr"/>
-      <c r="O258" t="inlineStr"/>
-      <c r="P258" t="inlineStr"/>
-      <c r="Q258" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M258" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N258" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O258" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="P258" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q258" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -19685,14 +19845,30 @@
       </c>
       <c r="L259" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M259" t="inlineStr"/>
-      <c r="N259" t="inlineStr"/>
-      <c r="O259" t="inlineStr"/>
-      <c r="P259" t="inlineStr"/>
-      <c r="Q259" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M259" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N259" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O259" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="P259" t="n">
+        <v>138</v>
+      </c>
+      <c r="Q259" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -19744,14 +19920,30 @@
       </c>
       <c r="L260" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M260" t="inlineStr"/>
-      <c r="N260" t="inlineStr"/>
-      <c r="O260" t="inlineStr"/>
-      <c r="P260" t="inlineStr"/>
-      <c r="Q260" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M260" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N260" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O260" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="P260" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q260" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -19803,14 +19995,30 @@
       </c>
       <c r="L261" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M261" t="inlineStr"/>
-      <c r="N261" t="inlineStr"/>
-      <c r="O261" t="inlineStr"/>
-      <c r="P261" t="inlineStr"/>
-      <c r="Q261" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M261" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N261" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O261" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="P261" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q261" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -19862,14 +20070,30 @@
       </c>
       <c r="L262" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M262" t="inlineStr"/>
-      <c r="N262" t="inlineStr"/>
-      <c r="O262" t="inlineStr"/>
-      <c r="P262" t="inlineStr"/>
-      <c r="Q262" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M262" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N262" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O262" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="P262" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q262" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -19921,14 +20145,30 @@
       </c>
       <c r="L263" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M263" t="inlineStr"/>
-      <c r="N263" t="inlineStr"/>
-      <c r="O263" t="inlineStr"/>
-      <c r="P263" t="inlineStr"/>
-      <c r="Q263" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M263" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N263" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O263" t="n">
+        <v>-1.6</v>
+      </c>
+      <c r="P263" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q263" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -19980,14 +20220,30 @@
       </c>
       <c r="L264" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M264" t="inlineStr"/>
-      <c r="N264" t="inlineStr"/>
-      <c r="O264" t="inlineStr"/>
-      <c r="P264" t="inlineStr"/>
-      <c r="Q264" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M264" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N264" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O264" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="P264" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q264" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -20039,14 +20295,30 @@
       </c>
       <c r="L265" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M265" t="inlineStr"/>
-      <c r="N265" t="inlineStr"/>
-      <c r="O265" t="inlineStr"/>
-      <c r="P265" t="inlineStr"/>
-      <c r="Q265" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M265" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N265" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O265" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P265" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q265" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -20098,14 +20370,30 @@
       </c>
       <c r="L266" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M266" t="inlineStr"/>
-      <c r="N266" t="inlineStr"/>
-      <c r="O266" t="inlineStr"/>
-      <c r="P266" t="inlineStr"/>
-      <c r="Q266" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M266" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N266" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O266" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P266" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q266" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -20157,14 +20445,30 @@
       </c>
       <c r="L267" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M267" t="inlineStr"/>
-      <c r="N267" t="inlineStr"/>
-      <c r="O267" t="inlineStr"/>
-      <c r="P267" t="inlineStr"/>
-      <c r="Q267" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M267" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N267" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O267" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="P267" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q267" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -20216,14 +20520,30 @@
       </c>
       <c r="L268" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M268" t="inlineStr"/>
-      <c r="N268" t="inlineStr"/>
-      <c r="O268" t="inlineStr"/>
-      <c r="P268" t="inlineStr"/>
-      <c r="Q268" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M268" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N268" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O268" t="n">
+        <v>-2</v>
+      </c>
+      <c r="P268" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q268" t="inlineStr">
+        <is>
+          <t>2025-10-06 04:26:46</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -20275,14 +20595,30 @@
       </c>
       <c r="L269" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M269" t="inlineStr"/>
-      <c r="N269" t="inlineStr"/>
-      <c r="O269" t="inlineStr"/>
-      <c r="P269" t="inlineStr"/>
-      <c r="Q269" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M269" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N269" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O269" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="P269" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q269" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -20334,14 +20670,30 @@
       </c>
       <c r="L270" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M270" t="inlineStr"/>
-      <c r="N270" t="inlineStr"/>
-      <c r="O270" t="inlineStr"/>
-      <c r="P270" t="inlineStr"/>
-      <c r="Q270" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M270" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N270" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O270" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="P270" t="n">
+        <v>65</v>
+      </c>
+      <c r="Q270" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -20393,14 +20745,30 @@
       </c>
       <c r="L271" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M271" t="inlineStr"/>
-      <c r="N271" t="inlineStr"/>
-      <c r="O271" t="inlineStr"/>
-      <c r="P271" t="inlineStr"/>
-      <c r="Q271" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M271" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N271" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O271" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="P271" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q271" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -20452,14 +20820,30 @@
       </c>
       <c r="L272" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M272" t="inlineStr"/>
-      <c r="N272" t="inlineStr"/>
-      <c r="O272" t="inlineStr"/>
-      <c r="P272" t="inlineStr"/>
-      <c r="Q272" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M272" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N272" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O272" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="P272" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q272" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -20511,14 +20895,30 @@
       </c>
       <c r="L273" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M273" t="inlineStr"/>
-      <c r="N273" t="inlineStr"/>
-      <c r="O273" t="inlineStr"/>
-      <c r="P273" t="inlineStr"/>
-      <c r="Q273" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M273" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N273" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O273" t="n">
+        <v>-1.1</v>
+      </c>
+      <c r="P273" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q273" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -20570,14 +20970,30 @@
       </c>
       <c r="L274" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M274" t="inlineStr"/>
-      <c r="N274" t="inlineStr"/>
-      <c r="O274" t="inlineStr"/>
-      <c r="P274" t="inlineStr"/>
-      <c r="Q274" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M274" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N274" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O274" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="P274" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q274" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -20629,14 +21045,30 @@
       </c>
       <c r="L275" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M275" t="inlineStr"/>
-      <c r="N275" t="inlineStr"/>
-      <c r="O275" t="inlineStr"/>
-      <c r="P275" t="inlineStr"/>
-      <c r="Q275" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M275" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N275" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O275" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="P275" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q275" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -20688,14 +21120,30 @@
       </c>
       <c r="L276" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M276" t="inlineStr"/>
-      <c r="N276" t="inlineStr"/>
-      <c r="O276" t="inlineStr"/>
-      <c r="P276" t="inlineStr"/>
-      <c r="Q276" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M276" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N276" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O276" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="P276" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q276" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -20747,14 +21195,30 @@
       </c>
       <c r="L277" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M277" t="inlineStr"/>
-      <c r="N277" t="inlineStr"/>
-      <c r="O277" t="inlineStr"/>
-      <c r="P277" t="inlineStr"/>
-      <c r="Q277" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M277" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N277" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O277" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="P277" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q277" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -20806,14 +21270,30 @@
       </c>
       <c r="L278" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M278" t="inlineStr"/>
-      <c r="N278" t="inlineStr"/>
-      <c r="O278" t="inlineStr"/>
-      <c r="P278" t="inlineStr"/>
-      <c r="Q278" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M278" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N278" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O278" t="n">
+        <v>-2.3</v>
+      </c>
+      <c r="P278" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q278" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -20865,14 +21345,30 @@
       </c>
       <c r="L279" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M279" t="inlineStr"/>
-      <c r="N279" t="inlineStr"/>
-      <c r="O279" t="inlineStr"/>
-      <c r="P279" t="inlineStr"/>
-      <c r="Q279" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M279" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N279" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O279" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="P279" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q279" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -20924,14 +21420,30 @@
       </c>
       <c r="L280" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M280" t="inlineStr"/>
-      <c r="N280" t="inlineStr"/>
-      <c r="O280" t="inlineStr"/>
-      <c r="P280" t="inlineStr"/>
-      <c r="Q280" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M280" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N280" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O280" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="P280" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q280" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -20983,14 +21495,30 @@
       </c>
       <c r="L281" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M281" t="inlineStr"/>
-      <c r="N281" t="inlineStr"/>
-      <c r="O281" t="inlineStr"/>
-      <c r="P281" t="inlineStr"/>
-      <c r="Q281" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M281" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N281" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O281" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="P281" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q281" t="inlineStr">
+        <is>
+          <t>2025-10-06 15:23:53</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-07 18:48:17 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -21570,14 +21570,30 @@
       </c>
       <c r="L282" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M282" t="inlineStr"/>
-      <c r="N282" t="inlineStr"/>
-      <c r="O282" t="inlineStr"/>
-      <c r="P282" t="inlineStr"/>
-      <c r="Q282" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M282" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N282" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O282" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="P282" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q282" t="inlineStr">
+        <is>
+          <t>2025-10-07 04:27:05</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-08 18:49:05 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q282"/>
+  <dimension ref="A1:Q283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21595,6 +21595,65 @@
         </is>
       </c>
     </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2025-10-09</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Los Angeles FC</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Toronto FC</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>87.75%</t>
+        </is>
+      </c>
+      <c r="G283" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>25.97%</t>
+        </is>
+      </c>
+      <c r="I283" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J283" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K283" t="n">
+        <v>0.6053342623591915</v>
+      </c>
+      <c r="L283" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M283" t="inlineStr"/>
+      <c r="N283" t="inlineStr"/>
+      <c r="O283" t="inlineStr"/>
+      <c r="P283" t="inlineStr"/>
+      <c r="Q283" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-10 18:46:17 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q283"/>
+  <dimension ref="A1:Q288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21645,14 +21645,325 @@
       </c>
       <c r="L283" t="inlineStr">
         <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M283" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N283" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O283" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="P283" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q283" t="inlineStr">
+        <is>
+          <t>2025-10-10 04:27:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2025-10-11</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Cancún</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Irapuato</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>63.78%</t>
+        </is>
+      </c>
+      <c r="G284" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>23.14%</t>
+        </is>
+      </c>
+      <c r="I284" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J284" t="n">
+        <v>0.02566256111386165</v>
+      </c>
+      <c r="K284" t="n">
+        <v>0.2566256111386165</v>
+      </c>
+      <c r="L284" t="inlineStr">
+        <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="M283" t="inlineStr"/>
-      <c r="N283" t="inlineStr"/>
-      <c r="O283" t="inlineStr"/>
-      <c r="P283" t="inlineStr"/>
-      <c r="Q283" t="inlineStr"/>
+      <c r="M284" t="inlineStr"/>
+      <c r="N284" t="inlineStr"/>
+      <c r="O284" t="inlineStr"/>
+      <c r="P284" t="inlineStr"/>
+      <c r="Q284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2025-10-11</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Venados FC</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Tepatitlán</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>52.44%</t>
+        </is>
+      </c>
+      <c r="G285" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>14.21%</t>
+        </is>
+      </c>
+      <c r="I285" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J285" t="n">
+        <v>0.01280385768872484</v>
+      </c>
+      <c r="K285" t="n">
+        <v>0.1280385768872484</v>
+      </c>
+      <c r="L285" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M285" t="inlineStr"/>
+      <c r="N285" t="inlineStr"/>
+      <c r="O285" t="inlineStr"/>
+      <c r="P285" t="inlineStr"/>
+      <c r="Q285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2025-10-11</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Tlaxcala</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>CDS Tampico Madero</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>60.33%</t>
+        </is>
+      </c>
+      <c r="G286" t="n">
+        <v>2</v>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>19.45%</t>
+        </is>
+      </c>
+      <c r="I286" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J286" t="n">
+        <v>0.0206530237185212</v>
+      </c>
+      <c r="K286" t="n">
+        <v>0.206530237185212</v>
+      </c>
+      <c r="L286" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M286" t="inlineStr"/>
+      <c r="N286" t="inlineStr"/>
+      <c r="O286" t="inlineStr"/>
+      <c r="P286" t="inlineStr"/>
+      <c r="Q286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2025-10-11</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Inter Miami</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Atlanta United FC</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>87.79%</t>
+        </is>
+      </c>
+      <c r="G287" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>26.02%</t>
+        </is>
+      </c>
+      <c r="I287" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J287" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K287" t="n">
+        <v>0.6064470615842978</v>
+      </c>
+      <c r="L287" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M287" t="inlineStr"/>
+      <c r="N287" t="inlineStr"/>
+      <c r="O287" t="inlineStr"/>
+      <c r="P287" t="inlineStr"/>
+      <c r="Q287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2025-10-11</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Orlando City SC</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Vancouver Whitecaps</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>54.05%</t>
+        </is>
+      </c>
+      <c r="G288" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>12.37%</t>
+        </is>
+      </c>
+      <c r="I288" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J288" t="n">
+        <v>0.0122756764106551</v>
+      </c>
+      <c r="K288" t="n">
+        <v>0.122756764106551</v>
+      </c>
+      <c r="L288" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M288" t="inlineStr"/>
+      <c r="N288" t="inlineStr"/>
+      <c r="O288" t="inlineStr"/>
+      <c r="P288" t="inlineStr"/>
+      <c r="Q288" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-11 18:40:50 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q288"/>
+  <dimension ref="A1:Q292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21965,6 +21965,242 @@
       <c r="P288" t="inlineStr"/>
       <c r="Q288" t="inlineStr"/>
     </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2025-10-12</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Mineros de Zacatecas</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Leones Negros UDG</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>67.52%</t>
+        </is>
+      </c>
+      <c r="G289" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>23.67%</t>
+        </is>
+      </c>
+      <c r="I289" t="n">
+        <v>2</v>
+      </c>
+      <c r="J289" t="n">
+        <v>0.02931828005568662</v>
+      </c>
+      <c r="K289" t="n">
+        <v>0.2931828005568662</v>
+      </c>
+      <c r="L289" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M289" t="inlineStr"/>
+      <c r="N289" t="inlineStr"/>
+      <c r="O289" t="inlineStr"/>
+      <c r="P289" t="inlineStr"/>
+      <c r="Q289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2025-10-12</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Monarcas</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Tapatío</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>71.43%</t>
+        </is>
+      </c>
+      <c r="G290" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>23.76%</t>
+        </is>
+      </c>
+      <c r="I290" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J290" t="n">
+        <v>0.03334237389304449</v>
+      </c>
+      <c r="K290" t="n">
+        <v>0.3334237389304449</v>
+      </c>
+      <c r="L290" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M290" t="inlineStr"/>
+      <c r="N290" t="inlineStr"/>
+      <c r="O290" t="inlineStr"/>
+      <c r="P290" t="inlineStr"/>
+      <c r="Q290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2025-10-12</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Seattle Sounders</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Real Salt Lake</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>75.61%</t>
+        </is>
+      </c>
+      <c r="G291" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>29.49%</t>
+        </is>
+      </c>
+      <c r="I291" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J291" t="n">
+        <v>0.04218802910321603</v>
+      </c>
+      <c r="K291" t="n">
+        <v>0.4218802910321602</v>
+      </c>
+      <c r="L291" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M291" t="inlineStr"/>
+      <c r="N291" t="inlineStr"/>
+      <c r="O291" t="inlineStr"/>
+      <c r="P291" t="inlineStr"/>
+      <c r="Q291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2025-10-12</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Dorados</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Atlante FC</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>82.81%</t>
+        </is>
+      </c>
+      <c r="G292" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>28.71%</t>
+        </is>
+      </c>
+      <c r="I292" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J292" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K292" t="n">
+        <v>0.5264720044992697</v>
+      </c>
+      <c r="L292" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M292" t="inlineStr"/>
+      <c r="N292" t="inlineStr"/>
+      <c r="O292" t="inlineStr"/>
+      <c r="P292" t="inlineStr"/>
+      <c r="Q292" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-12 18:43:08 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -21720,14 +21720,30 @@
       </c>
       <c r="L284" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M284" t="inlineStr"/>
-      <c r="N284" t="inlineStr"/>
-      <c r="O284" t="inlineStr"/>
-      <c r="P284" t="inlineStr"/>
-      <c r="Q284" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M284" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N284" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O284" t="n">
+        <v>-1.7</v>
+      </c>
+      <c r="P284" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q284" t="inlineStr">
+        <is>
+          <t>2025-10-12 04:25:52</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -21779,14 +21795,30 @@
       </c>
       <c r="L285" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M285" t="inlineStr"/>
-      <c r="N285" t="inlineStr"/>
-      <c r="O285" t="inlineStr"/>
-      <c r="P285" t="inlineStr"/>
-      <c r="Q285" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M285" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N285" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O285" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="P285" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q285" t="inlineStr">
+        <is>
+          <t>2025-10-12 04:25:52</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -21838,14 +21870,30 @@
       </c>
       <c r="L286" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M286" t="inlineStr"/>
-      <c r="N286" t="inlineStr"/>
-      <c r="O286" t="inlineStr"/>
-      <c r="P286" t="inlineStr"/>
-      <c r="Q286" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M286" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N286" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O286" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="P286" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q286" t="inlineStr">
+        <is>
+          <t>2025-10-12 04:25:52</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -21897,14 +21945,30 @@
       </c>
       <c r="L287" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M287" t="inlineStr"/>
-      <c r="N287" t="inlineStr"/>
-      <c r="O287" t="inlineStr"/>
-      <c r="P287" t="inlineStr"/>
-      <c r="Q287" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M287" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N287" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O287" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="P287" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q287" t="inlineStr">
+        <is>
+          <t>2025-10-12 04:25:52</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -21956,14 +22020,30 @@
       </c>
       <c r="L288" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M288" t="inlineStr"/>
-      <c r="N288" t="inlineStr"/>
-      <c r="O288" t="inlineStr"/>
-      <c r="P288" t="inlineStr"/>
-      <c r="Q288" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M288" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="N288" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O288" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="P288" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q288" t="inlineStr">
+        <is>
+          <t>2025-10-12 04:25:52</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-13 18:46:27 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -22095,14 +22095,30 @@
       </c>
       <c r="L289" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M289" t="inlineStr"/>
-      <c r="N289" t="inlineStr"/>
-      <c r="O289" t="inlineStr"/>
-      <c r="P289" t="inlineStr"/>
-      <c r="Q289" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M289" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N289" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O289" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="P289" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q289" t="inlineStr">
+        <is>
+          <t>2025-10-13 04:27:56</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -22154,14 +22170,30 @@
       </c>
       <c r="L290" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M290" t="inlineStr"/>
-      <c r="N290" t="inlineStr"/>
-      <c r="O290" t="inlineStr"/>
-      <c r="P290" t="inlineStr"/>
-      <c r="Q290" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M290" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N290" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O290" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="P290" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q290" t="inlineStr">
+        <is>
+          <t>2025-10-13 04:27:56</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -22213,14 +22245,30 @@
       </c>
       <c r="L291" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M291" t="inlineStr"/>
-      <c r="N291" t="inlineStr"/>
-      <c r="O291" t="inlineStr"/>
-      <c r="P291" t="inlineStr"/>
-      <c r="Q291" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M291" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="N291" t="inlineStr">
+        <is>
+          <t>Acierto</t>
+        </is>
+      </c>
+      <c r="O291" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="P291" t="n">
+        <v>73</v>
+      </c>
+      <c r="Q291" t="inlineStr">
+        <is>
+          <t>2025-10-13 04:27:56</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -22272,14 +22320,30 @@
       </c>
       <c r="L292" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M292" t="inlineStr"/>
-      <c r="N292" t="inlineStr"/>
-      <c r="O292" t="inlineStr"/>
-      <c r="P292" t="inlineStr"/>
-      <c r="Q292" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M292" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N292" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O292" t="n">
+        <v>-3.3</v>
+      </c>
+      <c r="P292" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q292" t="inlineStr">
+        <is>
+          <t>2025-10-13 04:27:56</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-15 18:48:18 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q292"/>
+  <dimension ref="A1:Q293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22345,6 +22345,65 @@
         </is>
       </c>
     </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2025-10-16</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>CDS Tampico Madero</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Mineros de Zacatecas</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>60.74%</t>
+        </is>
+      </c>
+      <c r="G293" t="n">
+        <v>2</v>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>20.26%</t>
+        </is>
+      </c>
+      <c r="I293" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J293" t="n">
+        <v>0.0214724743360502</v>
+      </c>
+      <c r="K293" t="n">
+        <v>0.214724743360502</v>
+      </c>
+      <c r="L293" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M293" t="inlineStr"/>
+      <c r="N293" t="inlineStr"/>
+      <c r="O293" t="inlineStr"/>
+      <c r="P293" t="inlineStr"/>
+      <c r="Q293" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-16 18:48:33 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q293"/>
+  <dimension ref="A1:Q295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22404,6 +22404,124 @@
       <c r="P293" t="inlineStr"/>
       <c r="Q293" t="inlineStr"/>
     </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Union Berlin</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Borussia Mönchengladbach</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>53.67%</t>
+        </is>
+      </c>
+      <c r="G294" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>16.90%</t>
+        </is>
+      </c>
+      <c r="I294" t="n">
+        <v>1</v>
+      </c>
+      <c r="J294" t="n">
+        <v>0.01506903899037965</v>
+      </c>
+      <c r="K294" t="n">
+        <v>0.1506903899037965</v>
+      </c>
+      <c r="L294" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M294" t="inlineStr"/>
+      <c r="N294" t="inlineStr"/>
+      <c r="O294" t="inlineStr"/>
+      <c r="P294" t="inlineStr"/>
+      <c r="Q294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Standard Liege</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Antwerp</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>52.95%</t>
+        </is>
+      </c>
+      <c r="G295" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>15.33%</t>
+        </is>
+      </c>
+      <c r="I295" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J295" t="n">
+        <v>0.01374884480492102</v>
+      </c>
+      <c r="K295" t="n">
+        <v>0.1374884480492102</v>
+      </c>
+      <c r="L295" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M295" t="inlineStr"/>
+      <c r="N295" t="inlineStr"/>
+      <c r="O295" t="inlineStr"/>
+      <c r="P295" t="inlineStr"/>
+      <c r="Q295" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Sync automático del tracker - 2025-10-17 18:45:46 UTC
</commit_message>
<xml_diff>
--- a/predictions_tracker.xlsx
+++ b/predictions_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q295"/>
+  <dimension ref="A1:Q321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22395,14 +22395,30 @@
       </c>
       <c r="L293" t="inlineStr">
         <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="M293" t="inlineStr"/>
-      <c r="N293" t="inlineStr"/>
-      <c r="O293" t="inlineStr"/>
-      <c r="P293" t="inlineStr"/>
-      <c r="Q293" t="inlineStr"/>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="M293" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="N293" t="inlineStr">
+        <is>
+          <t>Fallo</t>
+        </is>
+      </c>
+      <c r="O293" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="P293" t="n">
+        <v>-100</v>
+      </c>
+      <c r="Q293" t="inlineStr">
+        <is>
+          <t>2025-10-17 04:28:10</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -22522,6 +22538,1540 @@
       <c r="P295" t="inlineStr"/>
       <c r="Q295" t="inlineStr"/>
     </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Tepatitlán</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Cancún</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>65.60%</t>
+        </is>
+      </c>
+      <c r="G296" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>23.40%</t>
+        </is>
+      </c>
+      <c r="I296" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J296" t="n">
+        <v>0.02737950716520192</v>
+      </c>
+      <c r="K296" t="n">
+        <v>0.2737950716520192</v>
+      </c>
+      <c r="L296" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M296" t="inlineStr"/>
+      <c r="N296" t="inlineStr"/>
+      <c r="O296" t="inlineStr"/>
+      <c r="P296" t="inlineStr"/>
+      <c r="Q296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Correcaminos Uat</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Dorados</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>61.05%</t>
+        </is>
+      </c>
+      <c r="G297" t="n">
+        <v>2</v>
+      </c>
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>20.89%</t>
+        </is>
+      </c>
+      <c r="I297" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J297" t="n">
+        <v>0.0221066358449753</v>
+      </c>
+      <c r="K297" t="n">
+        <v>0.221066358449753</v>
+      </c>
+      <c r="L297" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M297" t="inlineStr"/>
+      <c r="N297" t="inlineStr"/>
+      <c r="O297" t="inlineStr"/>
+      <c r="P297" t="inlineStr"/>
+      <c r="Q297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Liga de Expansión MX</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Leones Negros UDG</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Alebrijes de Oaxaca</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>84.86%</t>
+        </is>
+      </c>
+      <c r="G298" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>24.33%</t>
+        </is>
+      </c>
+      <c r="I298" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J298" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K298" t="n">
+        <v>0.533062372942994</v>
+      </c>
+      <c r="L298" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M298" t="inlineStr"/>
+      <c r="N298" t="inlineStr"/>
+      <c r="O298" t="inlineStr"/>
+      <c r="P298" t="inlineStr"/>
+      <c r="Q298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Nottingham Forest</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>65.01%</t>
+        </is>
+      </c>
+      <c r="G299" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>22.93%</t>
+        </is>
+      </c>
+      <c r="I299" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J299" t="n">
+        <v>0.02655727760820212</v>
+      </c>
+      <c r="K299" t="n">
+        <v>0.2655727760820212</v>
+      </c>
+      <c r="L299" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M299" t="inlineStr"/>
+      <c r="N299" t="inlineStr"/>
+      <c r="O299" t="inlineStr"/>
+      <c r="P299" t="inlineStr"/>
+      <c r="Q299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Konyaspor</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Kocaelispor</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>64.97%</t>
+        </is>
+      </c>
+      <c r="G300" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>22.20%</t>
+        </is>
+      </c>
+      <c r="I300" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="J300" t="n">
+        <v>0.02604022708216256</v>
+      </c>
+      <c r="K300" t="n">
+        <v>0.2604022708216256</v>
+      </c>
+      <c r="L300" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M300" t="inlineStr"/>
+      <c r="N300" t="inlineStr"/>
+      <c r="O300" t="inlineStr"/>
+      <c r="P300" t="inlineStr"/>
+      <c r="Q300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>66.99%</t>
+        </is>
+      </c>
+      <c r="G301" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>22.69%</t>
+        </is>
+      </c>
+      <c r="I301" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J301" t="n">
+        <v>0.02814686866463166</v>
+      </c>
+      <c r="K301" t="n">
+        <v>0.2814686866463166</v>
+      </c>
+      <c r="L301" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M301" t="inlineStr"/>
+      <c r="N301" t="inlineStr"/>
+      <c r="O301" t="inlineStr"/>
+      <c r="P301" t="inlineStr"/>
+      <c r="Q301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>1.FC Köln</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>FC Augsburg</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>62.64%</t>
+        </is>
+      </c>
+      <c r="G302" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>20.92%</t>
+        </is>
+      </c>
+      <c r="I302" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="J302" t="n">
+        <v>0.02330777896200066</v>
+      </c>
+      <c r="K302" t="n">
+        <v>0.2330777896200066</v>
+      </c>
+      <c r="L302" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M302" t="inlineStr"/>
+      <c r="N302" t="inlineStr"/>
+      <c r="O302" t="inlineStr"/>
+      <c r="P302" t="inlineStr"/>
+      <c r="Q302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Hamburger SV</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>89.19%</t>
+        </is>
+      </c>
+      <c r="G303" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>25.39%</t>
+        </is>
+      </c>
+      <c r="I303" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J303" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K303" t="n">
+        <v>0.6346531140929691</v>
+      </c>
+      <c r="L303" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M303" t="inlineStr"/>
+      <c r="N303" t="inlineStr"/>
+      <c r="O303" t="inlineStr"/>
+      <c r="P303" t="inlineStr"/>
+      <c r="Q303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Burnley</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F304" t="inlineStr">
+        <is>
+          <t>51.63%</t>
+        </is>
+      </c>
+      <c r="G304" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>15.02%</t>
+        </is>
+      </c>
+      <c r="I304" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J304" t="n">
+        <v>0.01294208797375331</v>
+      </c>
+      <c r="K304" t="n">
+        <v>0.1294208797375331</v>
+      </c>
+      <c r="L304" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M304" t="inlineStr"/>
+      <c r="N304" t="inlineStr"/>
+      <c r="O304" t="inlineStr"/>
+      <c r="P304" t="inlineStr"/>
+      <c r="Q304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F305" t="inlineStr">
+        <is>
+          <t>53.17%</t>
+        </is>
+      </c>
+      <c r="G305" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>15.79%</t>
+        </is>
+      </c>
+      <c r="I305" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J305" t="n">
+        <v>0.01413631738383686</v>
+      </c>
+      <c r="K305" t="n">
+        <v>0.1413631738383686</v>
+      </c>
+      <c r="L305" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M305" t="inlineStr"/>
+      <c r="N305" t="inlineStr"/>
+      <c r="O305" t="inlineStr"/>
+      <c r="P305" t="inlineStr"/>
+      <c r="Q305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>90.03%</t>
+        </is>
+      </c>
+      <c r="G306" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>24.78%</t>
+        </is>
+      </c>
+      <c r="I306" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J306" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K306" t="n">
+        <v>0.6509964170845273</v>
+      </c>
+      <c r="L306" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M306" t="inlineStr"/>
+      <c r="N306" t="inlineStr"/>
+      <c r="O306" t="inlineStr"/>
+      <c r="P306" t="inlineStr"/>
+      <c r="Q306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>75.81%</t>
+        </is>
+      </c>
+      <c r="G307" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>35.10%</t>
+        </is>
+      </c>
+      <c r="I307" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J307" t="n">
+        <v>0.04557736001531452</v>
+      </c>
+      <c r="K307" t="n">
+        <v>0.4557736001531452</v>
+      </c>
+      <c r="L307" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M307" t="inlineStr"/>
+      <c r="N307" t="inlineStr"/>
+      <c r="O307" t="inlineStr"/>
+      <c r="P307" t="inlineStr"/>
+      <c r="Q307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Jupiler Pro League</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>OH Leuven</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Club Brugge KV</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>84.40%</t>
+        </is>
+      </c>
+      <c r="G308" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>27.84%</t>
+        </is>
+      </c>
+      <c r="I308" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J308" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K308" t="n">
+        <v>0.549594337446768</v>
+      </c>
+      <c r="L308" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M308" t="inlineStr"/>
+      <c r="N308" t="inlineStr"/>
+      <c r="O308" t="inlineStr"/>
+      <c r="P308" t="inlineStr"/>
+      <c r="Q308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Premier League</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>87.35%</t>
+        </is>
+      </c>
+      <c r="G309" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H309" t="inlineStr">
+        <is>
+          <t>29.72%</t>
+        </is>
+      </c>
+      <c r="I309" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J309" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K309" t="n">
+        <v>0.6205079271566802</v>
+      </c>
+      <c r="L309" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M309" t="inlineStr"/>
+      <c r="N309" t="inlineStr"/>
+      <c r="O309" t="inlineStr"/>
+      <c r="P309" t="inlineStr"/>
+      <c r="Q309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>La Liga</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Real Betis</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>65.82%</t>
+        </is>
+      </c>
+      <c r="G310" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>24.45%</t>
+        </is>
+      </c>
+      <c r="I310" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="J310" t="n">
+        <v>0.02825134617093525</v>
+      </c>
+      <c r="K310" t="n">
+        <v>0.2825134617093524</v>
+      </c>
+      <c r="L310" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M310" t="inlineStr"/>
+      <c r="N310" t="inlineStr"/>
+      <c r="O310" t="inlineStr"/>
+      <c r="P310" t="inlineStr"/>
+      <c r="Q310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Ligue 1</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Angers</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="E311" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F311" t="inlineStr">
+        <is>
+          <t>82.02%</t>
+        </is>
+      </c>
+      <c r="G311" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>31.54%</t>
+        </is>
+      </c>
+      <c r="I311" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J311" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K311" t="n">
+        <v>0.5302169785431298</v>
+      </c>
+      <c r="L311" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M311" t="inlineStr"/>
+      <c r="N311" t="inlineStr"/>
+      <c r="O311" t="inlineStr"/>
+      <c r="P311" t="inlineStr"/>
+      <c r="Q311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Süper Lig</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Istanbul Basaksehir</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Galatasaray</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>78.98%</t>
+        </is>
+      </c>
+      <c r="G312" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>25.11%</t>
+        </is>
+      </c>
+      <c r="I312" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J312" t="n">
+        <v>0.04394857908288552</v>
+      </c>
+      <c r="K312" t="n">
+        <v>0.4394857908288552</v>
+      </c>
+      <c r="L312" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M312" t="inlineStr"/>
+      <c r="N312" t="inlineStr"/>
+      <c r="O312" t="inlineStr"/>
+      <c r="P312" t="inlineStr"/>
+      <c r="Q312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Serie A</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>AS Roma</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>51.97%</t>
+        </is>
+      </c>
+      <c r="G313" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>15.76%</t>
+        </is>
+      </c>
+      <c r="I313" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J313" t="n">
+        <v>0.01354333851322352</v>
+      </c>
+      <c r="K313" t="n">
+        <v>0.1354333851322352</v>
+      </c>
+      <c r="L313" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M313" t="inlineStr"/>
+      <c r="N313" t="inlineStr"/>
+      <c r="O313" t="inlineStr"/>
+      <c r="P313" t="inlineStr"/>
+      <c r="Q313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Ajax</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>AZ Alkmaar</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>60.32%</t>
+        </is>
+      </c>
+      <c r="G314" t="n">
+        <v>2</v>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>19.44%</t>
+        </is>
+      </c>
+      <c r="I314" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J314" t="n">
+        <v>0.02064212453239047</v>
+      </c>
+      <c r="K314" t="n">
+        <v>0.2064212453239047</v>
+      </c>
+      <c r="L314" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M314" t="inlineStr"/>
+      <c r="N314" t="inlineStr"/>
+      <c r="O314" t="inlineStr"/>
+      <c r="P314" t="inlineStr"/>
+      <c r="Q314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Eredivisie</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>NAC Breda</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>PEC Zwolle</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>56.31%</t>
+        </is>
+      </c>
+      <c r="G315" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>17.08%</t>
+        </is>
+      </c>
+      <c r="I315" t="n">
+        <v>1</v>
+      </c>
+      <c r="J315" t="n">
+        <v>0.01659932491725425</v>
+      </c>
+      <c r="K315" t="n">
+        <v>0.1659932491725425</v>
+      </c>
+      <c r="L315" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M315" t="inlineStr"/>
+      <c r="N315" t="inlineStr"/>
+      <c r="O315" t="inlineStr"/>
+      <c r="P315" t="inlineStr"/>
+      <c r="Q315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Atlanta United FC</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>DC United</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>67.87%</t>
+        </is>
+      </c>
+      <c r="G316" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>24.30%</t>
+        </is>
+      </c>
+      <c r="I316" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J316" t="n">
+        <v>0.03006211383452393</v>
+      </c>
+      <c r="K316" t="n">
+        <v>0.3006211383452393</v>
+      </c>
+      <c r="L316" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M316" t="inlineStr"/>
+      <c r="N316" t="inlineStr"/>
+      <c r="O316" t="inlineStr"/>
+      <c r="P316" t="inlineStr"/>
+      <c r="Q316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>FC Cincinnati</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>CF Montreal</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>85.50%</t>
+        </is>
+      </c>
+      <c r="G317" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>26.96%</t>
+        </is>
+      </c>
+      <c r="I317" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J317" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K317" t="n">
+        <v>0.5649301371622064</v>
+      </c>
+      <c r="L317" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M317" t="inlineStr"/>
+      <c r="N317" t="inlineStr"/>
+      <c r="O317" t="inlineStr"/>
+      <c r="P317" t="inlineStr"/>
+      <c r="Q317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Columbus Crew</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>New York Red Bulls</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>84.30%</t>
+        </is>
+      </c>
+      <c r="G318" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>25.18%</t>
+        </is>
+      </c>
+      <c r="I318" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J318" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K318" t="n">
+        <v>0.5288974844958699</v>
+      </c>
+      <c r="L318" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M318" t="inlineStr"/>
+      <c r="N318" t="inlineStr"/>
+      <c r="O318" t="inlineStr"/>
+      <c r="P318" t="inlineStr"/>
+      <c r="Q318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>New England Revolution</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Chicago Fire</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>46.71%</t>
+        </is>
+      </c>
+      <c r="G319" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H319" t="inlineStr">
+        <is>
+          <t>4.06%</t>
+        </is>
+      </c>
+      <c r="I319" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J319" t="n">
+        <v>0.004086083380147407</v>
+      </c>
+      <c r="K319" t="n">
+        <v>0.04086083380147407</v>
+      </c>
+      <c r="L319" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M319" t="inlineStr"/>
+      <c r="N319" t="inlineStr"/>
+      <c r="O319" t="inlineStr"/>
+      <c r="P319" t="inlineStr"/>
+      <c r="Q319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>New York City FC</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Seattle Sounders</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>Home Win</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>56.31%</t>
+        </is>
+      </c>
+      <c r="G320" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>17.08%</t>
+        </is>
+      </c>
+      <c r="I320" t="n">
+        <v>1</v>
+      </c>
+      <c r="J320" t="n">
+        <v>0.01659932491725425</v>
+      </c>
+      <c r="K320" t="n">
+        <v>0.1659932491725425</v>
+      </c>
+      <c r="L320" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M320" t="inlineStr"/>
+      <c r="N320" t="inlineStr"/>
+      <c r="O320" t="inlineStr"/>
+      <c r="P320" t="inlineStr"/>
+      <c r="Q320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Major League Soccer</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Toronto FC</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Orlando City SC</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>Away Win</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>65.07%</t>
+        </is>
+      </c>
+      <c r="G321" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>23.04%</t>
+        </is>
+      </c>
+      <c r="I321" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J321" t="n">
+        <v>0.02667959712486534</v>
+      </c>
+      <c r="K321" t="n">
+        <v>0.2667959712486533</v>
+      </c>
+      <c r="L321" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="M321" t="inlineStr"/>
+      <c r="N321" t="inlineStr"/>
+      <c r="O321" t="inlineStr"/>
+      <c r="P321" t="inlineStr"/>
+      <c r="Q321" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>